<commit_message>
price of oil increases, so I updated the table with more columns - also increased COGS cost to /bbl
</commit_message>
<xml_diff>
--- a/mmtlp_dividend_calc.xlsx
+++ b/mmtlp_dividend_calc.xlsx
@@ -9,12 +9,13 @@
     <sheet name="MMTLP_DIVI_CALC - MMTLP_DIVI_CA" sheetId="2" r:id="rId5"/>
     <sheet name="What Happens if MMTLP Divi Get " sheetId="3" r:id="rId6"/>
     <sheet name="reinvesting_1000_shares_mmtlp -" sheetId="4" r:id="rId7"/>
+    <sheet name="divi chart from 30 to 150 oil p" sheetId="5" r:id="rId8"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="60">
   <si>
     <t>This document was exported from Numbers.  Each table was converted to an Excel worksheet. All other objects on each Numbers sheet were placed on separate worksheets. Please be aware that formula calculations may differ in Excel.</t>
   </si>
@@ -34,6 +35,12 @@
     <t>MMTLP_DIVI_CALC - MMTLP_DIVI_CA</t>
   </si>
   <si>
+    <t>Non-Taxable</t>
+  </si>
+  <si>
+    <t>Taxable</t>
+  </si>
+  <si>
     <t>Price of Oil</t>
   </si>
   <si>
@@ -179,6 +186,15 @@
   </si>
   <si>
     <t>Profit</t>
+  </si>
+  <si>
+    <t>divi chart from 30 to 150 oil prices</t>
+  </si>
+  <si>
+    <t>Sell Some Oil &amp; Gas Assets</t>
+  </si>
+  <si>
+    <t>divi chart from 30 to 150 oil p</t>
   </si>
 </sst>
 </file>
@@ -192,7 +208,7 @@
     <numFmt numFmtId="61" formatCode="0.0%"/>
     <numFmt numFmtId="62" formatCode="&quot;$&quot;#,##0"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="14">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -216,7 +232,7 @@
     </font>
     <font>
       <b val="1"/>
-      <sz val="1"/>
+      <sz val="12"/>
       <color indexed="8"/>
       <name val="Helvetica Neue"/>
     </font>
@@ -233,8 +249,40 @@
     </font>
     <font>
       <b val="1"/>
+      <sz val="1"/>
+      <color indexed="8"/>
+      <name val="Helvetica Neue"/>
+    </font>
+    <font>
+      <b val="1"/>
       <sz val="10"/>
       <color indexed="8"/>
+      <name val="Helvetica Neue"/>
+    </font>
+    <font>
+      <sz val="19"/>
+      <color indexed="17"/>
+      <name val="Helvetica Neue"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <sz val="12"/>
+      <color indexed="17"/>
+      <name val="Helvetica Neue"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color indexed="17"/>
+      <name val="Helvetica Neue"/>
+    </font>
+    <font>
+      <sz val="15"/>
+      <color indexed="17"/>
+      <name val="Helvetica Neue"/>
+    </font>
+    <font>
+      <sz val="17"/>
+      <color indexed="17"/>
       <name val="Helvetica Neue"/>
     </font>
   </fonts>
@@ -334,6 +382,21 @@
         <color indexed="13"/>
       </left>
       <right style="thin">
+        <color indexed="13"/>
+      </right>
+      <top style="thin">
+        <color indexed="14"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="13"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="13"/>
+      </left>
+      <right style="thin">
         <color indexed="14"/>
       </right>
       <top style="thin">
@@ -367,21 +430,6 @@
         <color indexed="13"/>
       </right>
       <top style="thin">
-        <color indexed="14"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="13"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="13"/>
-      </left>
-      <right style="thin">
-        <color indexed="13"/>
-      </right>
-      <top style="thin">
         <color indexed="13"/>
       </top>
       <bottom style="thin">
@@ -395,7 +443,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="78">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -423,34 +471,64 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="5" fillId="5" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="59" fontId="6" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="5" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="59" fontId="6" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="6" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="60" fontId="6" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="6" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="61" fontId="6" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="59" fontId="6" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="5" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="59" fontId="6" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="59" fontId="6" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="6" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="6" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="60" fontId="6" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="60" fontId="6" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="6" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="6" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="61" fontId="6" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="61" fontId="6" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
@@ -459,7 +537,10 @@
     <xf numFmtId="0" fontId="7" fillId="4" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -489,25 +570,25 @@
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="5" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="60" fontId="0" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="62" fontId="0" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="61" fontId="0" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="8" fillId="5" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="60" fontId="0" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="62" fontId="0" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="61" fontId="0" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -516,13 +597,13 @@
     <xf numFmtId="0" fontId="0" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="9" fontId="0" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="9" fontId="0" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -532,6 +613,69 @@
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="61" fontId="0" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="62" fontId="10" fillId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="5" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="59" fontId="11" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="59" fontId="11" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="5" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="59" fontId="11" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="59" fontId="11" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="11" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="11" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="60" fontId="11" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="60" fontId="11" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="11" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="11" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="61" fontId="11" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="61" fontId="11" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -559,9 +703,420 @@
       <rgbColor rgb="ff3f3f3f"/>
       <rgbColor rgb="ffdbdbdb"/>
       <rgbColor rgb="ffd5d5d5"/>
+      <rgbColor rgb="ff919191"/>
+      <rgbColor rgb="ffb8b8b8"/>
+      <rgbColor rgb="ffffff00"/>
     </indexedColors>
   </colors>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:roundedCorners val="0"/>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.0709777"/>
+          <c:y val="0.0435835"/>
+          <c:w val="0.924022"/>
+          <c:h val="0.881576"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'divi chart from 30 to 150 oil p'!$B$19</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Div ($/pref share)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="FFFF00"/>
+            </a:solidFill>
+            <a:ln w="12700" cap="flat">
+              <a:noFill/>
+              <a:miter lim="400000"/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:numFmt formatCode="&quot;$&quot;#,##0.00" sourceLinked="0"/>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" i="0" strike="noStrike" sz="1200" u="none">
+                    <a:solidFill>
+                      <a:srgbClr val="929292"/>
+                    </a:solidFill>
+                    <a:latin typeface="Helvetica Neue"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'divi chart from 30 to 150 oil p'!$C$2:$X$2</c:f>
+              <c:strCache>
+                <c:ptCount val="22"/>
+                <c:pt idx="0">
+                  <c:v>$30</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>$40</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>$50</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>$60</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>$65</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>$70</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>$75</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>$80</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>$85</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>$90</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>$95</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>$100</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>$105</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>$110</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>$115</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>$120</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>$125</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>$130</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>$135</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>$140</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>$145</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>$150</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'divi chart from 30 to 150 oil p'!$C$19:$X$19</c:f>
+              <c:numCache>
+                <c:ptCount val="22"/>
+                <c:pt idx="0">
+                  <c:v>0.000000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10.268042</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20.536084</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>30.804126</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>35.938147</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>41.072168</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>46.206189</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>51.340209</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>56.474230</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>61.608251</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>66.742272</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>71.876293</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>77.010314</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>82.144335</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>87.278356</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>92.412377</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>97.546398</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>102.680419</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>107.814440</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>112.948461</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>118.082482</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>123.216503</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:gapWidth val="40"/>
+        <c:overlap val="-10"/>
+        <c:axId val="2094734552"/>
+        <c:axId val="2094734553"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="2094734552"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="&quot;$&quot;#,##0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="low"/>
+        <c:spPr>
+          <a:ln w="12700" cap="flat">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:prstDash val="solid"/>
+            <a:miter lim="400000"/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" i="0" strike="noStrike" sz="1700" u="none">
+                <a:solidFill>
+                  <a:srgbClr val="929292"/>
+                </a:solidFill>
+                <a:latin typeface="Helvetica Neue"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2094734553"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:noMultiLvlLbl val="1"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2094734553"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="6350" cap="flat">
+              <a:solidFill>
+                <a:srgbClr val="B8B8B8"/>
+              </a:solidFill>
+              <a:prstDash val="solid"/>
+              <a:miter lim="400000"/>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="&quot;$&quot;#,##0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="12700" cap="flat">
+            <a:noFill/>
+            <a:prstDash val="solid"/>
+            <a:miter lim="400000"/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" i="0" strike="noStrike" sz="1900" u="none">
+                <a:solidFill>
+                  <a:srgbClr val="929292"/>
+                </a:solidFill>
+                <a:latin typeface="Helvetica Neue"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2094734552"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+        <c:majorUnit val="20"/>
+        <c:minorUnit val="10"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="12700" cap="flat">
+          <a:noFill/>
+          <a:miter lim="400000"/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.101631"/>
+          <c:y val="0.109023"/>
+          <c:w val="0.867716"/>
+          <c:h val="0.0620116"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="1"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="12700" cap="flat">
+          <a:noFill/>
+          <a:miter lim="400000"/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr b="0" i="0" strike="noStrike" sz="1500" u="none">
+              <a:solidFill>
+                <a:srgbClr val="929292"/>
+              </a:solidFill>
+              <a:latin typeface="Helvetica Neue"/>
+            </a:defRPr>
+          </a:pPr>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+  </c:chart>
+  <c:spPr>
+    <a:noFill/>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>193588</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>219077</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>446221</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>95483</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="2D Column Chart"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="447588" y="5594987"/>
+        <a:ext cx="15340234" cy="5689197"/>
+      </xdr:xfrm>
+      <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1662,7 +2217,7 @@
     </row>
     <row r="11">
       <c r="B11" t="s" s="3">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
@@ -1670,15 +2225,15 @@
     <row r="12">
       <c r="B12" s="4"/>
       <c r="C12" t="s" s="4">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D12" t="s" s="5">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="13">
       <c r="B13" t="s" s="3">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
@@ -1686,10 +2241,26 @@
     <row r="14">
       <c r="B14" s="4"/>
       <c r="C14" t="s" s="4">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D14" t="s" s="5">
-        <v>36</v>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="B15" t="s" s="3">
+        <v>57</v>
+      </c>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+    </row>
+    <row r="16">
+      <c r="B16" s="4"/>
+      <c r="C16" t="s" s="4">
+        <v>58</v>
+      </c>
+      <c r="D16" t="s" s="5">
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -1700,13 +2271,14 @@
     <hyperlink ref="D10" location="'MMTLP_DIVI_CALC - MMTLP_DIVI_CA'!R2C1" tooltip="" display="MMTLP_DIVI_CALC - MMTLP_DIVI_CA"/>
     <hyperlink ref="D12" location="'What Happens if MMTLP Divi Get '!R2C1" tooltip="" display="What Happens if MMTLP Divi Get "/>
     <hyperlink ref="D14" location="'reinvesting_1000_shares_mmtlp -'!R2C1" tooltip="" display="reinvesting_1000_shares_mmtlp -"/>
+    <hyperlink ref="D16" location="'divi chart from 30 to 150 oil p'!R2C2" tooltip="" display="divi chart from 30 to 150 oil p"/>
   </hyperlinks>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A2:B29"/>
+  <dimension ref="A2:E29"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
       <pane topLeftCell="B3" xSplit="1" ySplit="2" activePane="bottomRight" state="frozen"/>
@@ -1715,8 +2287,8 @@
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="1" max="1" width="21.8203" style="6" customWidth="1"/>
-    <col min="2" max="2" width="14.6094" style="6" customWidth="1"/>
-    <col min="3" max="16384" width="16.3516" style="6" customWidth="1"/>
+    <col min="2" max="5" width="14.6094" style="6" customWidth="1"/>
+    <col min="6" max="16384" width="16.3516" style="6" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="27.65" customHeight="1">
@@ -1724,219 +2296,361 @@
         <v>4</v>
       </c>
       <c r="B1" s="7"/>
-    </row>
-    <row r="2" ht="9.5" customHeight="1">
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+    </row>
+    <row r="2" ht="20.5" customHeight="1">
       <c r="A2" s="8"/>
-      <c r="B2" s="8"/>
+      <c r="B2" t="s" s="9">
+        <v>6</v>
+      </c>
+      <c r="C2" s="10"/>
+      <c r="D2" t="s" s="9">
+        <v>7</v>
+      </c>
+      <c r="E2" s="8"/>
     </row>
     <row r="3" ht="19.25" customHeight="1">
-      <c r="A3" t="s" s="9">
-        <v>6</v>
-      </c>
-      <c r="B3" s="10">
-        <v>75</v>
-      </c>
+      <c r="A3" t="s" s="11">
+        <v>8</v>
+      </c>
+      <c r="B3" s="12">
+        <v>100</v>
+      </c>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13">
+        <v>100</v>
+      </c>
+      <c r="E3" s="13"/>
     </row>
     <row r="4" ht="19.05" customHeight="1">
-      <c r="A4" t="s" s="11">
-        <v>7</v>
-      </c>
-      <c r="B4" s="12">
-        <v>25</v>
-      </c>
+      <c r="A4" t="s" s="14">
+        <v>9</v>
+      </c>
+      <c r="B4" s="15">
+        <v>30</v>
+      </c>
+      <c r="C4" s="16"/>
+      <c r="D4" s="16">
+        <v>30</v>
+      </c>
+      <c r="E4" s="16"/>
     </row>
     <row r="5" ht="19.05" customHeight="1">
-      <c r="A5" t="s" s="11">
-        <v>8</v>
-      </c>
-      <c r="B5" s="12">
+      <c r="A5" t="s" s="14">
+        <v>10</v>
+      </c>
+      <c r="B5" s="15">
         <f>B3-B4</f>
-        <v>50</v>
-      </c>
+        <v>70</v>
+      </c>
+      <c r="C5" s="16"/>
+      <c r="D5" s="16">
+        <f>D3-D4</f>
+        <v>70</v>
+      </c>
+      <c r="E5" s="16"/>
     </row>
     <row r="6" ht="19.05" customHeight="1">
-      <c r="A6" s="13"/>
-      <c r="B6" s="14"/>
+      <c r="A6" s="17"/>
+      <c r="B6" s="18"/>
+      <c r="C6" s="19"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="19"/>
     </row>
     <row r="7" ht="19.05" customHeight="1">
-      <c r="A7" t="s" s="11">
-        <v>9</v>
-      </c>
-      <c r="B7" s="15">
+      <c r="A7" t="s" s="14">
+        <v>11</v>
+      </c>
+      <c r="B7" s="20">
         <v>0.12</v>
       </c>
+      <c r="C7" s="19"/>
+      <c r="D7" s="21">
+        <v>0.12</v>
+      </c>
+      <c r="E7" s="19"/>
     </row>
     <row r="8" ht="19.05" customHeight="1">
-      <c r="A8" t="s" s="11">
-        <v>10</v>
-      </c>
-      <c r="B8" s="12">
+      <c r="A8" t="s" s="14">
+        <v>12</v>
+      </c>
+      <c r="B8" s="15">
         <f>B7*B5</f>
-        <v>6</v>
-      </c>
+        <v>8.4</v>
+      </c>
+      <c r="C8" s="19"/>
+      <c r="D8" s="16">
+        <f>D7*D5</f>
+        <v>8.4</v>
+      </c>
+      <c r="E8" s="19"/>
     </row>
     <row r="9" ht="19.05" customHeight="1">
-      <c r="A9" s="13"/>
-      <c r="B9" s="14"/>
+      <c r="A9" s="17"/>
+      <c r="B9" s="18"/>
+      <c r="C9" s="19"/>
+      <c r="D9" s="19"/>
+      <c r="E9" s="19"/>
     </row>
     <row r="10" ht="19.05" customHeight="1">
-      <c r="A10" t="s" s="11">
-        <v>11</v>
-      </c>
-      <c r="B10" s="15">
+      <c r="A10" t="s" s="14">
+        <v>13</v>
+      </c>
+      <c r="B10" s="20">
         <v>0.49</v>
       </c>
+      <c r="C10" s="19"/>
+      <c r="D10" s="21">
+        <v>0.49</v>
+      </c>
+      <c r="E10" s="19"/>
     </row>
     <row r="11" ht="19.05" customHeight="1">
-      <c r="A11" t="s" s="11">
-        <v>12</v>
-      </c>
-      <c r="B11" s="16">
+      <c r="A11" t="s" s="14">
+        <v>14</v>
+      </c>
+      <c r="B11" s="22">
         <f>B8*B10</f>
-        <v>2.94</v>
-      </c>
+        <v>4.116</v>
+      </c>
+      <c r="C11" s="19"/>
+      <c r="D11" s="23">
+        <f>D8*D10</f>
+        <v>4.116</v>
+      </c>
+      <c r="E11" s="19"/>
     </row>
     <row r="12" ht="19.05" customHeight="1">
-      <c r="A12" s="13"/>
-      <c r="B12" s="14"/>
+      <c r="A12" s="17"/>
+      <c r="B12" s="18"/>
+      <c r="C12" s="19"/>
+      <c r="D12" s="19"/>
+      <c r="E12" s="19"/>
     </row>
     <row r="13" ht="19.05" customHeight="1">
-      <c r="A13" t="s" s="11">
-        <v>13</v>
-      </c>
-      <c r="B13" s="14"/>
+      <c r="A13" t="s" s="14">
+        <v>15</v>
+      </c>
+      <c r="B13" s="18"/>
+      <c r="C13" s="19"/>
+      <c r="D13" s="19"/>
+      <c r="E13" s="19"/>
     </row>
     <row r="14" ht="19.05" customHeight="1">
-      <c r="A14" t="s" s="11">
-        <v>14</v>
-      </c>
-      <c r="B14" s="17">
+      <c r="A14" t="s" s="14">
+        <v>16</v>
+      </c>
+      <c r="B14" s="24">
         <v>3200000000</v>
       </c>
+      <c r="C14" s="25"/>
+      <c r="D14" s="25">
+        <v>3200000000</v>
+      </c>
+      <c r="E14" s="25"/>
     </row>
     <row r="15" ht="19.05" customHeight="1">
-      <c r="A15" t="s" s="11">
-        <v>15</v>
-      </c>
-      <c r="B15" s="17">
+      <c r="A15" t="s" s="14">
+        <v>17</v>
+      </c>
+      <c r="B15" s="24">
         <f>B14*B$11</f>
-        <v>9408000000</v>
-      </c>
+        <v>13171200000</v>
+      </c>
+      <c r="C15" s="25"/>
+      <c r="D15" s="25">
+        <f>D14*D$11</f>
+        <v>13171200000</v>
+      </c>
+      <c r="E15" s="25"/>
     </row>
     <row r="16" ht="19.05" customHeight="1">
-      <c r="A16" t="s" s="11">
+      <c r="A16" t="s" s="14">
+        <v>18</v>
+      </c>
+      <c r="B16" s="26">
+        <v>0</v>
+      </c>
+      <c r="C16" s="19"/>
+      <c r="D16" s="21">
+        <v>0.21</v>
+      </c>
+      <c r="E16" s="19"/>
+    </row>
+    <row r="17" ht="19.05" customHeight="1">
+      <c r="A17" t="s" s="14">
+        <v>19</v>
+      </c>
+      <c r="B17" s="27">
+        <v>0.1</v>
+      </c>
+      <c r="C17" s="19"/>
+      <c r="D17" s="28">
+        <v>0.1</v>
+      </c>
+      <c r="E17" s="19"/>
+    </row>
+    <row r="18" ht="19.05" customHeight="1">
+      <c r="A18" t="s" s="14">
+        <v>20</v>
+      </c>
+      <c r="B18" s="24">
+        <f>B15*(1-(B16+B17))</f>
+        <v>11854080000</v>
+      </c>
+      <c r="C18" s="19"/>
+      <c r="D18" s="25">
+        <f>D15*(1-(D16+D17))</f>
+        <v>9088128000</v>
+      </c>
+      <c r="E18" s="19"/>
+    </row>
+    <row r="19" ht="19.05" customHeight="1">
+      <c r="A19" t="s" s="14">
+        <v>21</v>
+      </c>
+      <c r="B19" s="24">
+        <v>164923363</v>
+      </c>
+      <c r="C19" s="25"/>
+      <c r="D19" s="25">
+        <v>164923363</v>
+      </c>
+      <c r="E19" s="25"/>
+    </row>
+    <row r="20" ht="19.05" customHeight="1">
+      <c r="A20" t="s" s="14">
+        <v>22</v>
+      </c>
+      <c r="B20" s="15">
+        <f>B18/B19</f>
+        <v>71.87629323323949</v>
+      </c>
+      <c r="C20" s="16"/>
+      <c r="D20" s="16">
+        <f>D18/D19</f>
+        <v>55.1051581454836</v>
+      </c>
+      <c r="E20" s="16"/>
+    </row>
+    <row r="21" ht="19.05" customHeight="1">
+      <c r="A21" s="17"/>
+      <c r="B21" s="18"/>
+      <c r="C21" s="19"/>
+      <c r="D21" s="19"/>
+      <c r="E21" s="19"/>
+    </row>
+    <row r="22" ht="19.05" customHeight="1">
+      <c r="A22" t="s" s="14">
+        <v>23</v>
+      </c>
+      <c r="B22" s="18"/>
+      <c r="C22" s="19"/>
+      <c r="D22" s="19"/>
+      <c r="E22" s="19"/>
+    </row>
+    <row r="23" ht="19.05" customHeight="1">
+      <c r="A23" t="s" s="14">
         <v>16</v>
       </c>
-      <c r="B16" s="15">
+      <c r="B23" s="24">
+        <v>2100000000</v>
+      </c>
+      <c r="C23" s="25"/>
+      <c r="D23" s="25">
+        <v>2100000000</v>
+      </c>
+      <c r="E23" s="25"/>
+    </row>
+    <row r="24" ht="19.05" customHeight="1">
+      <c r="A24" t="s" s="14">
+        <v>24</v>
+      </c>
+      <c r="B24" s="24">
+        <f>B23*B$11</f>
+        <v>8643600000</v>
+      </c>
+      <c r="C24" s="25"/>
+      <c r="D24" s="25">
+        <f>D23*D$11</f>
+        <v>8643600000</v>
+      </c>
+      <c r="E24" s="25"/>
+    </row>
+    <row r="25" ht="19.05" customHeight="1">
+      <c r="A25" t="s" s="14">
+        <v>18</v>
+      </c>
+      <c r="B25" s="20">
         <v>0.21</v>
       </c>
-    </row>
-    <row r="17" ht="19.05" customHeight="1">
-      <c r="A17" t="s" s="11">
-        <v>17</v>
-      </c>
-      <c r="B17" s="18">
+      <c r="C25" s="19"/>
+      <c r="D25" s="21">
+        <v>0.21</v>
+      </c>
+      <c r="E25" s="19"/>
+    </row>
+    <row r="26" ht="19.05" customHeight="1">
+      <c r="A26" t="s" s="14">
+        <v>19</v>
+      </c>
+      <c r="B26" s="27">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="18" ht="19.05" customHeight="1">
-      <c r="A18" t="s" s="11">
-        <v>18</v>
-      </c>
-      <c r="B18" s="17">
-        <f>B15*(1-(B16+B17))</f>
-        <v>6491520000</v>
-      </c>
-    </row>
-    <row r="19" ht="19.05" customHeight="1">
-      <c r="A19" t="s" s="11">
-        <v>19</v>
-      </c>
-      <c r="B19" s="17">
-        <v>164923363</v>
-      </c>
-    </row>
-    <row r="20" ht="19.05" customHeight="1">
-      <c r="A20" t="s" s="11">
+      <c r="C26" s="19"/>
+      <c r="D26" s="28">
+        <v>0.1</v>
+      </c>
+      <c r="E26" s="19"/>
+    </row>
+    <row r="27" ht="19.05" customHeight="1">
+      <c r="A27" t="s" s="14">
         <v>20</v>
       </c>
-      <c r="B20" s="12">
-        <f>B18/B19</f>
-        <v>39.360827246774</v>
-      </c>
-    </row>
-    <row r="21" ht="19.05" customHeight="1">
-      <c r="A21" s="13"/>
-      <c r="B21" s="14"/>
-    </row>
-    <row r="22" ht="19.05" customHeight="1">
-      <c r="A22" t="s" s="11">
+      <c r="B27" s="24">
+        <f>B24*(1-(B25+B26))</f>
+        <v>5964084000</v>
+      </c>
+      <c r="C27" s="19"/>
+      <c r="D27" s="25">
+        <f>D24*(1-(D25+D26))</f>
+        <v>5964084000</v>
+      </c>
+      <c r="E27" s="19"/>
+    </row>
+    <row r="28" ht="19.05" customHeight="1">
+      <c r="A28" t="s" s="14">
         <v>21</v>
       </c>
-      <c r="B22" s="14"/>
-    </row>
-    <row r="23" ht="19.05" customHeight="1">
-      <c r="A23" t="s" s="11">
-        <v>14</v>
-      </c>
-      <c r="B23" s="17">
-        <v>2100000000</v>
-      </c>
-    </row>
-    <row r="24" ht="19.05" customHeight="1">
-      <c r="A24" t="s" s="11">
+      <c r="B28" s="24">
+        <v>175000000</v>
+      </c>
+      <c r="C28" s="25"/>
+      <c r="D28" s="25">
+        <v>175000000</v>
+      </c>
+      <c r="E28" s="25"/>
+    </row>
+    <row r="29" ht="19.05" customHeight="1">
+      <c r="A29" t="s" s="14">
         <v>22</v>
       </c>
-      <c r="B24" s="17">
-        <f>B23*B$11</f>
-        <v>6174000000</v>
-      </c>
-    </row>
-    <row r="25" ht="19.05" customHeight="1">
-      <c r="A25" t="s" s="11">
-        <v>16</v>
-      </c>
-      <c r="B25" s="15">
-        <v>0.21</v>
-      </c>
-    </row>
-    <row r="26" ht="19.05" customHeight="1">
-      <c r="A26" t="s" s="11">
-        <v>17</v>
-      </c>
-      <c r="B26" s="18">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="27" ht="19.05" customHeight="1">
-      <c r="A27" t="s" s="11">
-        <v>18</v>
-      </c>
-      <c r="B27" s="17">
-        <f>B24*(1-(B25+B26))</f>
-        <v>4260060000</v>
-      </c>
-    </row>
-    <row r="28" ht="19.05" customHeight="1">
-      <c r="A28" t="s" s="11">
-        <v>19</v>
-      </c>
-      <c r="B28" s="17">
-        <v>175000000</v>
-      </c>
-    </row>
-    <row r="29" ht="19.05" customHeight="1">
-      <c r="A29" t="s" s="11">
-        <v>20</v>
-      </c>
-      <c r="B29" s="12">
+      <c r="B29" s="15">
         <f>B27/B28</f>
-        <v>24.3432</v>
-      </c>
+        <v>34.08048</v>
+      </c>
+      <c r="C29" s="16"/>
+      <c r="D29" s="16">
+        <f>D27/D28</f>
+        <v>34.08048</v>
+      </c>
+      <c r="E29" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A1:E1"/>
   </mergeCells>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="72" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
@@ -1956,17 +2670,17 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="21.8203" style="19" customWidth="1"/>
-    <col min="2" max="2" width="14.6094" style="19" customWidth="1"/>
-    <col min="3" max="3" width="16.3516" style="19" customWidth="1"/>
-    <col min="4" max="4" width="28.6562" style="19" customWidth="1"/>
-    <col min="5" max="7" width="13.7891" style="19" customWidth="1"/>
-    <col min="8" max="16384" width="16.3516" style="19" customWidth="1"/>
+    <col min="1" max="1" width="21.8203" style="29" customWidth="1"/>
+    <col min="2" max="2" width="14.6094" style="29" customWidth="1"/>
+    <col min="3" max="3" width="16.3516" style="29" customWidth="1"/>
+    <col min="4" max="4" width="28.6562" style="29" customWidth="1"/>
+    <col min="5" max="7" width="13.7891" style="29" customWidth="1"/>
+    <col min="8" max="16384" width="16.3516" style="29" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="27.65" customHeight="1">
       <c r="A1" t="s" s="7">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B1" s="7"/>
       <c r="C1" s="7"/>
@@ -1976,431 +2690,431 @@
       <c r="G1" s="7"/>
     </row>
     <row r="2" ht="20.25" customHeight="1">
-      <c r="A2" s="8"/>
-      <c r="B2" s="8"/>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="20"/>
+      <c r="A2" s="30"/>
+      <c r="B2" s="30"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="31"/>
     </row>
     <row r="3" ht="20.25" customHeight="1">
-      <c r="A3" t="s" s="9">
-        <v>6</v>
-      </c>
-      <c r="B3" s="10">
+      <c r="A3" t="s" s="11">
+        <v>8</v>
+      </c>
+      <c r="B3" s="12">
         <v>75</v>
       </c>
-      <c r="C3" s="21"/>
-      <c r="D3" s="21"/>
-      <c r="E3" s="21"/>
-      <c r="F3" s="21"/>
-      <c r="G3" s="21"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="32"/>
     </row>
     <row r="4" ht="20.05" customHeight="1">
-      <c r="A4" t="s" s="11">
-        <v>7</v>
-      </c>
-      <c r="B4" s="12">
+      <c r="A4" t="s" s="14">
+        <v>9</v>
+      </c>
+      <c r="B4" s="15">
         <v>25</v>
       </c>
-      <c r="C4" s="22"/>
-      <c r="D4" s="22"/>
-      <c r="E4" s="22"/>
-      <c r="F4" s="22"/>
-      <c r="G4" s="22"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="33"/>
+      <c r="F4" s="33"/>
+      <c r="G4" s="33"/>
     </row>
     <row r="5" ht="20.05" customHeight="1">
-      <c r="A5" t="s" s="11">
-        <v>8</v>
-      </c>
-      <c r="B5" s="12">
+      <c r="A5" t="s" s="14">
+        <v>10</v>
+      </c>
+      <c r="B5" s="15">
         <f>B3-B4</f>
         <v>50</v>
       </c>
-      <c r="C5" s="22"/>
-      <c r="D5" s="22"/>
-      <c r="E5" s="22"/>
-      <c r="F5" s="22"/>
-      <c r="G5" s="22"/>
+      <c r="C5" s="33"/>
+      <c r="D5" s="33"/>
+      <c r="E5" s="33"/>
+      <c r="F5" s="33"/>
+      <c r="G5" s="33"/>
     </row>
     <row r="6" ht="20.05" customHeight="1">
-      <c r="A6" s="13"/>
-      <c r="B6" s="14"/>
-      <c r="C6" s="22"/>
-      <c r="D6" s="22"/>
-      <c r="E6" s="22"/>
-      <c r="F6" s="22"/>
-      <c r="G6" s="22"/>
+      <c r="A6" s="17"/>
+      <c r="B6" s="18"/>
+      <c r="C6" s="33"/>
+      <c r="D6" s="33"/>
+      <c r="E6" s="33"/>
+      <c r="F6" s="33"/>
+      <c r="G6" s="33"/>
     </row>
     <row r="7" ht="20.05" customHeight="1">
-      <c r="A7" t="s" s="11">
-        <v>9</v>
-      </c>
-      <c r="B7" s="15">
+      <c r="A7" t="s" s="14">
+        <v>11</v>
+      </c>
+      <c r="B7" s="20">
         <v>0.12</v>
       </c>
-      <c r="C7" s="22"/>
-      <c r="D7" s="22"/>
-      <c r="E7" s="22"/>
-      <c r="F7" s="22"/>
-      <c r="G7" s="22"/>
+      <c r="C7" s="33"/>
+      <c r="D7" s="33"/>
+      <c r="E7" s="33"/>
+      <c r="F7" s="33"/>
+      <c r="G7" s="33"/>
     </row>
     <row r="8" ht="20.05" customHeight="1">
-      <c r="A8" t="s" s="11">
-        <v>10</v>
-      </c>
-      <c r="B8" s="12">
+      <c r="A8" t="s" s="14">
+        <v>12</v>
+      </c>
+      <c r="B8" s="15">
         <f>B7*B5</f>
         <v>6</v>
       </c>
-      <c r="C8" s="22"/>
-      <c r="D8" s="22"/>
-      <c r="E8" s="22"/>
-      <c r="F8" s="22"/>
-      <c r="G8" s="22"/>
+      <c r="C8" s="33"/>
+      <c r="D8" s="33"/>
+      <c r="E8" s="33"/>
+      <c r="F8" s="33"/>
+      <c r="G8" s="33"/>
     </row>
     <row r="9" ht="20.05" customHeight="1">
-      <c r="A9" s="13"/>
-      <c r="B9" s="14"/>
-      <c r="C9" s="22"/>
-      <c r="D9" s="22"/>
-      <c r="E9" s="22"/>
-      <c r="F9" s="22"/>
-      <c r="G9" s="22"/>
+      <c r="A9" s="17"/>
+      <c r="B9" s="18"/>
+      <c r="C9" s="33"/>
+      <c r="D9" s="33"/>
+      <c r="E9" s="33"/>
+      <c r="F9" s="33"/>
+      <c r="G9" s="33"/>
     </row>
     <row r="10" ht="20.05" customHeight="1">
-      <c r="A10" t="s" s="11">
-        <v>11</v>
-      </c>
-      <c r="B10" s="15">
+      <c r="A10" t="s" s="14">
+        <v>13</v>
+      </c>
+      <c r="B10" s="20">
         <v>0.49</v>
       </c>
-      <c r="C10" s="22"/>
-      <c r="D10" s="22"/>
-      <c r="E10" s="22"/>
-      <c r="F10" s="22"/>
-      <c r="G10" s="22"/>
+      <c r="C10" s="33"/>
+      <c r="D10" s="33"/>
+      <c r="E10" s="33"/>
+      <c r="F10" s="33"/>
+      <c r="G10" s="33"/>
     </row>
     <row r="11" ht="20.05" customHeight="1">
-      <c r="A11" t="s" s="11">
-        <v>12</v>
-      </c>
-      <c r="B11" s="16">
+      <c r="A11" t="s" s="14">
+        <v>14</v>
+      </c>
+      <c r="B11" s="22">
         <f>B8*B10</f>
         <v>2.94</v>
       </c>
-      <c r="C11" s="22"/>
-      <c r="D11" s="22"/>
-      <c r="E11" s="22"/>
-      <c r="F11" s="22"/>
-      <c r="G11" s="22"/>
+      <c r="C11" s="33"/>
+      <c r="D11" s="33"/>
+      <c r="E11" s="33"/>
+      <c r="F11" s="33"/>
+      <c r="G11" s="33"/>
     </row>
     <row r="12" ht="20.05" customHeight="1">
-      <c r="A12" s="13"/>
-      <c r="B12" s="14"/>
-      <c r="C12" s="22"/>
-      <c r="D12" s="22"/>
-      <c r="E12" s="23">
+      <c r="A12" s="17"/>
+      <c r="B12" s="18"/>
+      <c r="C12" s="33"/>
+      <c r="D12" s="33"/>
+      <c r="E12" s="34">
         <v>0.25</v>
       </c>
-      <c r="F12" s="22"/>
-      <c r="G12" s="22"/>
+      <c r="F12" s="33"/>
+      <c r="G12" s="33"/>
     </row>
     <row r="13" ht="20.05" customHeight="1">
-      <c r="A13" t="s" s="11">
-        <v>13</v>
-      </c>
-      <c r="B13" s="14"/>
-      <c r="C13" s="22"/>
-      <c r="D13" s="22"/>
-      <c r="E13" s="24">
+      <c r="A13" t="s" s="14">
+        <v>15</v>
+      </c>
+      <c r="B13" s="18"/>
+      <c r="C13" s="33"/>
+      <c r="D13" s="33"/>
+      <c r="E13" s="35">
         <f>E12*E22</f>
         <v>177947368.421053</v>
       </c>
-      <c r="F13" s="22"/>
-      <c r="G13" s="22"/>
+      <c r="F13" s="33"/>
+      <c r="G13" s="33"/>
     </row>
     <row r="14" ht="20.05" customHeight="1">
-      <c r="A14" t="s" s="11">
-        <v>14</v>
-      </c>
-      <c r="B14" s="17">
+      <c r="A14" t="s" s="14">
+        <v>16</v>
+      </c>
+      <c r="B14" s="24">
         <v>3200000000</v>
       </c>
-      <c r="C14" s="22"/>
-      <c r="D14" s="22"/>
-      <c r="E14" s="22"/>
-      <c r="F14" s="22"/>
-      <c r="G14" s="22"/>
+      <c r="C14" s="33"/>
+      <c r="D14" s="33"/>
+      <c r="E14" s="33"/>
+      <c r="F14" s="33"/>
+      <c r="G14" s="33"/>
     </row>
     <row r="15" ht="20.05" customHeight="1">
-      <c r="A15" t="s" s="11">
-        <v>15</v>
-      </c>
-      <c r="B15" s="17">
+      <c r="A15" t="s" s="14">
+        <v>17</v>
+      </c>
+      <c r="B15" s="24">
         <f>B14*B$11</f>
         <v>9408000000</v>
       </c>
-      <c r="C15" s="22"/>
-      <c r="D15" s="22"/>
-      <c r="E15" s="22"/>
-      <c r="F15" s="22"/>
-      <c r="G15" s="22"/>
+      <c r="C15" s="33"/>
+      <c r="D15" s="33"/>
+      <c r="E15" s="33"/>
+      <c r="F15" s="33"/>
+      <c r="G15" s="33"/>
     </row>
     <row r="16" ht="20.05" customHeight="1">
-      <c r="A16" t="s" s="11">
-        <v>16</v>
-      </c>
-      <c r="B16" s="15">
+      <c r="A16" t="s" s="14">
+        <v>18</v>
+      </c>
+      <c r="B16" s="20">
         <v>0.21</v>
       </c>
-      <c r="C16" s="22"/>
-      <c r="D16" s="22"/>
-      <c r="E16" s="22"/>
-      <c r="F16" s="22"/>
-      <c r="G16" s="22"/>
+      <c r="C16" s="33"/>
+      <c r="D16" s="33"/>
+      <c r="E16" s="33"/>
+      <c r="F16" s="33"/>
+      <c r="G16" s="33"/>
     </row>
     <row r="17" ht="20.05" customHeight="1">
-      <c r="A17" t="s" s="11">
-        <v>17</v>
-      </c>
-      <c r="B17" s="18">
+      <c r="A17" t="s" s="14">
+        <v>19</v>
+      </c>
+      <c r="B17" s="27">
         <v>0.1</v>
       </c>
-      <c r="C17" s="22"/>
-      <c r="D17" t="s" s="25">
-        <v>25</v>
-      </c>
-      <c r="E17" s="26"/>
-      <c r="F17" s="26"/>
-      <c r="G17" s="26"/>
+      <c r="C17" s="33"/>
+      <c r="D17" t="s" s="36">
+        <v>27</v>
+      </c>
+      <c r="E17" s="37"/>
+      <c r="F17" s="37"/>
+      <c r="G17" s="37"/>
     </row>
     <row r="18" ht="20.05" customHeight="1">
-      <c r="A18" t="s" s="11">
-        <v>18</v>
-      </c>
-      <c r="B18" s="17">
+      <c r="A18" t="s" s="14">
+        <v>20</v>
+      </c>
+      <c r="B18" s="24">
         <f>B15*(1-(B16+B17))</f>
         <v>6491520000</v>
       </c>
-      <c r="C18" s="22"/>
-      <c r="D18" t="s" s="27">
-        <v>26</v>
-      </c>
-      <c r="E18" s="28">
+      <c r="C18" s="33"/>
+      <c r="D18" t="s" s="38">
+        <v>28</v>
+      </c>
+      <c r="E18" s="39">
         <v>0.25</v>
       </c>
-      <c r="F18" s="22"/>
-      <c r="G18" s="28">
+      <c r="F18" s="33"/>
+      <c r="G18" s="39">
         <v>0.07000000000000001</v>
       </c>
     </row>
     <row r="19" ht="20.05" customHeight="1">
-      <c r="A19" t="s" s="11">
-        <v>19</v>
-      </c>
-      <c r="B19" s="17">
+      <c r="A19" t="s" s="14">
+        <v>21</v>
+      </c>
+      <c r="B19" s="24">
         <v>164923363</v>
       </c>
-      <c r="C19" s="22"/>
-      <c r="D19" t="s" s="27">
-        <v>27</v>
-      </c>
-      <c r="E19" s="24">
+      <c r="C19" s="33"/>
+      <c r="D19" t="s" s="38">
+        <v>29</v>
+      </c>
+      <c r="E19" s="35">
         <f>$B18*E18</f>
         <v>1622880000</v>
       </c>
-      <c r="F19" s="22"/>
-      <c r="G19" s="24">
+      <c r="F19" s="33"/>
+      <c r="G19" s="35">
         <f>$B18*G18</f>
         <v>454406400</v>
       </c>
     </row>
     <row r="20" ht="20.05" customHeight="1">
-      <c r="A20" t="s" s="11">
-        <v>20</v>
-      </c>
-      <c r="B20" s="12">
+      <c r="A20" t="s" s="14">
+        <v>22</v>
+      </c>
+      <c r="B20" s="15">
         <f>B18/B19</f>
         <v>39.360827246774</v>
       </c>
-      <c r="C20" s="22"/>
-      <c r="D20" s="26"/>
-      <c r="E20" s="22"/>
-      <c r="F20" s="22"/>
-      <c r="G20" s="22"/>
+      <c r="C20" s="33"/>
+      <c r="D20" s="37"/>
+      <c r="E20" s="33"/>
+      <c r="F20" s="33"/>
+      <c r="G20" s="33"/>
     </row>
     <row r="21" ht="20.05" customHeight="1">
-      <c r="A21" s="13"/>
-      <c r="B21" s="14"/>
-      <c r="C21" s="22"/>
-      <c r="D21" t="s" s="27">
-        <v>28</v>
-      </c>
-      <c r="E21" s="23">
+      <c r="A21" s="17"/>
+      <c r="B21" s="18"/>
+      <c r="C21" s="33"/>
+      <c r="D21" t="s" s="38">
+        <v>30</v>
+      </c>
+      <c r="E21" s="34">
         <v>2.28</v>
       </c>
-      <c r="F21" s="22"/>
-      <c r="G21" s="23">
+      <c r="F21" s="33"/>
+      <c r="G21" s="34">
         <v>2.28</v>
       </c>
     </row>
     <row r="22" ht="20.05" customHeight="1">
-      <c r="A22" t="s" s="11">
-        <v>21</v>
-      </c>
-      <c r="B22" s="14"/>
-      <c r="C22" s="22"/>
-      <c r="D22" t="s" s="27">
-        <v>29</v>
-      </c>
-      <c r="E22" s="24">
+      <c r="A22" t="s" s="14">
+        <v>23</v>
+      </c>
+      <c r="B22" s="18"/>
+      <c r="C22" s="33"/>
+      <c r="D22" t="s" s="38">
+        <v>31</v>
+      </c>
+      <c r="E22" s="35">
         <f>E19/E21</f>
         <v>711789473.684211</v>
       </c>
-      <c r="F22" s="29"/>
-      <c r="G22" s="24">
+      <c r="F22" s="40"/>
+      <c r="G22" s="35">
         <f>G19/G21</f>
         <v>199301052.631579</v>
       </c>
     </row>
     <row r="23" ht="20.05" customHeight="1">
-      <c r="A23" t="s" s="11">
-        <v>14</v>
-      </c>
-      <c r="B23" s="17">
+      <c r="A23" t="s" s="14">
+        <v>16</v>
+      </c>
+      <c r="B23" s="24">
         <v>2100000000</v>
       </c>
-      <c r="C23" s="22"/>
-      <c r="D23" s="26"/>
-      <c r="E23" s="22"/>
-      <c r="F23" s="22"/>
-      <c r="G23" s="22"/>
+      <c r="C23" s="33"/>
+      <c r="D23" s="37"/>
+      <c r="E23" s="33"/>
+      <c r="F23" s="33"/>
+      <c r="G23" s="33"/>
     </row>
     <row r="24" ht="20.05" customHeight="1">
-      <c r="A24" t="s" s="11">
-        <v>22</v>
-      </c>
-      <c r="B24" s="17">
+      <c r="A24" t="s" s="14">
+        <v>24</v>
+      </c>
+      <c r="B24" s="24">
         <f>B23*B$11</f>
         <v>6174000000</v>
       </c>
-      <c r="C24" s="22"/>
-      <c r="D24" t="s" s="27">
-        <v>30</v>
-      </c>
-      <c r="E24" s="24">
+      <c r="C24" s="33"/>
+      <c r="D24" t="s" s="38">
+        <v>32</v>
+      </c>
+      <c r="E24" s="35">
         <v>281259620</v>
       </c>
-      <c r="F24" s="24"/>
-      <c r="G24" s="24">
+      <c r="F24" s="35"/>
+      <c r="G24" s="35">
         <v>281259620</v>
       </c>
     </row>
     <row r="25" ht="20.05" customHeight="1">
-      <c r="A25" t="s" s="11">
-        <v>16</v>
-      </c>
-      <c r="B25" s="15">
+      <c r="A25" t="s" s="14">
+        <v>18</v>
+      </c>
+      <c r="B25" s="20">
         <v>0.21</v>
       </c>
-      <c r="C25" s="22"/>
-      <c r="D25" t="s" s="27">
-        <v>31</v>
-      </c>
-      <c r="E25" s="24">
+      <c r="C25" s="33"/>
+      <c r="D25" t="s" s="38">
+        <v>33</v>
+      </c>
+      <c r="E25" s="35">
         <v>50820911</v>
       </c>
-      <c r="F25" s="24"/>
-      <c r="G25" s="24">
+      <c r="F25" s="35"/>
+      <c r="G25" s="35">
         <v>50820911</v>
       </c>
     </row>
     <row r="26" ht="20.05" customHeight="1">
-      <c r="A26" t="s" s="11">
-        <v>17</v>
-      </c>
-      <c r="B26" s="18">
+      <c r="A26" t="s" s="14">
+        <v>19</v>
+      </c>
+      <c r="B26" s="27">
         <v>0.1</v>
       </c>
-      <c r="C26" s="22"/>
-      <c r="D26" t="s" s="27">
-        <v>32</v>
-      </c>
-      <c r="E26" s="24">
+      <c r="C26" s="33"/>
+      <c r="D26" t="s" s="38">
+        <v>34</v>
+      </c>
+      <c r="E26" s="35">
         <v>41845770</v>
       </c>
-      <c r="F26" s="24"/>
-      <c r="G26" s="24">
+      <c r="F26" s="35"/>
+      <c r="G26" s="35">
         <v>41845770</v>
       </c>
     </row>
     <row r="27" ht="20.05" customHeight="1">
-      <c r="A27" t="s" s="11">
-        <v>18</v>
-      </c>
-      <c r="B27" s="17">
+      <c r="A27" t="s" s="14">
+        <v>20</v>
+      </c>
+      <c r="B27" s="24">
         <f>B24*(1-(B25+B26))</f>
         <v>4260060000</v>
       </c>
-      <c r="C27" s="22"/>
-      <c r="D27" t="s" s="27">
-        <v>33</v>
-      </c>
-      <c r="E27" s="24">
+      <c r="C27" s="33"/>
+      <c r="D27" t="s" s="38">
+        <v>35</v>
+      </c>
+      <c r="E27" s="35">
         <f>E24-E25-E26</f>
         <v>188592939</v>
       </c>
-      <c r="F27" s="22"/>
-      <c r="G27" s="24">
+      <c r="F27" s="33"/>
+      <c r="G27" s="35">
         <f>G24-G25-G26</f>
         <v>188592939</v>
       </c>
     </row>
     <row r="28" ht="20.05" customHeight="1">
-      <c r="A28" t="s" s="11">
-        <v>19</v>
-      </c>
-      <c r="B28" s="17">
+      <c r="A28" t="s" s="14">
+        <v>21</v>
+      </c>
+      <c r="B28" s="24">
         <v>175000000</v>
       </c>
-      <c r="C28" s="22"/>
-      <c r="D28" s="26"/>
-      <c r="E28" s="24"/>
-      <c r="F28" s="24"/>
-      <c r="G28" s="24"/>
+      <c r="C28" s="33"/>
+      <c r="D28" s="37"/>
+      <c r="E28" s="35"/>
+      <c r="F28" s="35"/>
+      <c r="G28" s="35"/>
     </row>
     <row r="29" ht="20.05" customHeight="1">
-      <c r="A29" t="s" s="11">
-        <v>20</v>
-      </c>
-      <c r="B29" s="12">
+      <c r="A29" t="s" s="14">
+        <v>22</v>
+      </c>
+      <c r="B29" s="15">
         <f>B27/B28</f>
         <v>24.3432</v>
       </c>
-      <c r="C29" s="22"/>
-      <c r="D29" t="s" s="27">
-        <v>34</v>
-      </c>
-      <c r="E29" s="24">
+      <c r="C29" s="33"/>
+      <c r="D29" t="s" s="38">
+        <v>36</v>
+      </c>
+      <c r="E29" s="35">
         <f>E27-E22</f>
         <v>-523196534.684211</v>
       </c>
-      <c r="F29" s="29"/>
-      <c r="G29" s="24">
+      <c r="F29" s="40"/>
+      <c r="G29" s="35">
         <f>G27-G22</f>
         <v>-10708113.631579</v>
       </c>
     </row>
     <row r="30" ht="20.05" customHeight="1">
-      <c r="A30" s="13"/>
-      <c r="B30" s="12"/>
-      <c r="C30" s="22"/>
-      <c r="D30" s="22"/>
-      <c r="E30" s="22"/>
-      <c r="F30" s="22"/>
-      <c r="G30" s="22"/>
+      <c r="A30" s="17"/>
+      <c r="B30" s="15"/>
+      <c r="C30" s="33"/>
+      <c r="D30" s="33"/>
+      <c r="E30" s="33"/>
+      <c r="F30" s="33"/>
+      <c r="G30" s="33"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2427,13 +3141,13 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="6" width="16.3516" style="30" customWidth="1"/>
-    <col min="7" max="16384" width="16.3516" style="30" customWidth="1"/>
+    <col min="1" max="6" width="16.3516" style="41" customWidth="1"/>
+    <col min="7" max="16384" width="16.3516" style="41" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="27.65" customHeight="1">
       <c r="A1" t="s" s="7">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B1" s="7"/>
       <c r="C1" s="7"/>
@@ -2442,302 +3156,302 @@
       <c r="F1" s="7"/>
     </row>
     <row r="2" ht="20.05" customHeight="1">
-      <c r="A2" t="s" s="31">
-        <v>37</v>
-      </c>
-      <c r="B2" s="32">
+      <c r="A2" t="s" s="42">
+        <v>39</v>
+      </c>
+      <c r="B2" s="43">
         <v>1000</v>
       </c>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
     </row>
     <row r="3" ht="20.05" customHeight="1">
-      <c r="A3" t="s" s="31">
-        <v>38</v>
-      </c>
-      <c r="B3" s="33">
-        <v>1.28</v>
-      </c>
-      <c r="C3" s="22"/>
-      <c r="D3" s="22"/>
-      <c r="E3" s="22"/>
-      <c r="F3" s="22"/>
+      <c r="A3" t="s" s="42">
+        <v>40</v>
+      </c>
+      <c r="B3" s="44">
+        <v>1.6</v>
+      </c>
+      <c r="C3" s="33"/>
+      <c r="D3" s="33"/>
+      <c r="E3" s="33"/>
+      <c r="F3" s="33"/>
     </row>
     <row r="4" ht="20.05" customHeight="1">
-      <c r="A4" t="s" s="31">
-        <v>39</v>
-      </c>
-      <c r="B4" s="34">
+      <c r="A4" t="s" s="42">
+        <v>41</v>
+      </c>
+      <c r="B4" s="45">
         <f>B2*B3</f>
-        <v>1280</v>
-      </c>
-      <c r="C4" s="22"/>
-      <c r="D4" s="22"/>
-      <c r="E4" s="22"/>
-      <c r="F4" s="22"/>
+        <v>1600</v>
+      </c>
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="33"/>
+      <c r="F4" s="33"/>
     </row>
     <row r="5" ht="20.05" customHeight="1">
-      <c r="A5" s="35"/>
-      <c r="B5" s="36"/>
-      <c r="C5" s="22"/>
-      <c r="D5" s="22"/>
-      <c r="E5" s="22"/>
-      <c r="F5" s="22"/>
+      <c r="A5" s="46"/>
+      <c r="B5" s="47"/>
+      <c r="C5" s="33"/>
+      <c r="D5" s="33"/>
+      <c r="E5" s="33"/>
+      <c r="F5" s="33"/>
     </row>
     <row r="6" ht="20.05" customHeight="1">
-      <c r="A6" t="s" s="31">
-        <v>40</v>
-      </c>
-      <c r="B6" s="32">
+      <c r="A6" t="s" s="42">
+        <v>42</v>
+      </c>
+      <c r="B6" s="43">
+        <v>75</v>
+      </c>
+      <c r="C6" s="33"/>
+      <c r="D6" s="33"/>
+      <c r="E6" s="33"/>
+      <c r="F6" s="33"/>
+    </row>
+    <row r="7" ht="20.05" customHeight="1">
+      <c r="A7" t="s" s="42">
+        <v>43</v>
+      </c>
+      <c r="B7" s="45">
+        <f>B6*B2</f>
+        <v>75000</v>
+      </c>
+      <c r="C7" s="33"/>
+      <c r="D7" s="33"/>
+      <c r="E7" s="33"/>
+      <c r="F7" s="33"/>
+    </row>
+    <row r="8" ht="20.05" customHeight="1">
+      <c r="A8" t="s" s="42">
+        <v>44</v>
+      </c>
+      <c r="B8" s="48">
+        <v>0.371</v>
+      </c>
+      <c r="C8" s="33"/>
+      <c r="D8" t="s" s="49">
         <v>45</v>
       </c>
-      <c r="C6" s="22"/>
-      <c r="D6" s="22"/>
-      <c r="E6" s="22"/>
-      <c r="F6" s="22"/>
-    </row>
-    <row r="7" ht="20.05" customHeight="1">
-      <c r="A7" t="s" s="31">
-        <v>41</v>
-      </c>
-      <c r="B7" s="34">
-        <f>B6*B2</f>
-        <v>45000</v>
-      </c>
-      <c r="C7" s="22"/>
-      <c r="D7" s="22"/>
-      <c r="E7" s="22"/>
-      <c r="F7" s="22"/>
-    </row>
-    <row r="8" ht="20.05" customHeight="1">
-      <c r="A8" t="s" s="31">
-        <v>42</v>
-      </c>
-      <c r="B8" s="37">
+      <c r="E8" s="33"/>
+      <c r="F8" s="33"/>
+    </row>
+    <row r="9" ht="20.05" customHeight="1">
+      <c r="A9" t="s" s="42">
+        <v>46</v>
+      </c>
+      <c r="B9" s="45">
+        <f>B8*B7</f>
+        <v>27825</v>
+      </c>
+      <c r="C9" s="33"/>
+      <c r="D9" s="50"/>
+      <c r="E9" s="33"/>
+      <c r="F9" s="33"/>
+    </row>
+    <row r="10" ht="20.05" customHeight="1">
+      <c r="A10" t="s" s="42">
+        <v>47</v>
+      </c>
+      <c r="B10" s="45">
+        <f>B7-B9</f>
+        <v>47175</v>
+      </c>
+      <c r="C10" s="33"/>
+      <c r="D10" s="50"/>
+      <c r="E10" s="33"/>
+      <c r="F10" s="33"/>
+    </row>
+    <row r="11" ht="20.05" customHeight="1">
+      <c r="A11" s="46"/>
+      <c r="B11" s="47"/>
+      <c r="C11" s="33"/>
+      <c r="D11" s="50"/>
+      <c r="E11" s="33"/>
+      <c r="F11" s="33"/>
+    </row>
+    <row r="12" ht="20.05" customHeight="1">
+      <c r="A12" t="s" s="42">
+        <v>48</v>
+      </c>
+      <c r="B12" s="47"/>
+      <c r="C12" s="33"/>
+      <c r="D12" s="50"/>
+      <c r="E12" s="33"/>
+      <c r="F12" s="33"/>
+    </row>
+    <row r="13" ht="20.05" customHeight="1">
+      <c r="A13" t="s" s="42">
+        <v>49</v>
+      </c>
+      <c r="B13" s="51">
+        <v>1</v>
+      </c>
+      <c r="C13" s="33"/>
+      <c r="D13" s="50"/>
+      <c r="E13" s="33"/>
+      <c r="F13" s="33"/>
+    </row>
+    <row r="14" ht="20.05" customHeight="1">
+      <c r="A14" t="s" s="42">
+        <v>50</v>
+      </c>
+      <c r="B14" s="45">
+        <f>B13*B10</f>
+        <v>47175</v>
+      </c>
+      <c r="C14" s="33"/>
+      <c r="D14" s="50"/>
+      <c r="E14" s="33"/>
+      <c r="F14" s="33"/>
+    </row>
+    <row r="15" ht="20.05" customHeight="1">
+      <c r="A15" t="s" s="42">
+        <v>51</v>
+      </c>
+      <c r="B15" s="43">
+        <v>2.25</v>
+      </c>
+      <c r="C15" s="33"/>
+      <c r="D15" s="50"/>
+      <c r="E15" s="33"/>
+      <c r="F15" s="33"/>
+    </row>
+    <row r="16" ht="20.05" customHeight="1">
+      <c r="A16" t="s" s="42">
+        <v>52</v>
+      </c>
+      <c r="B16" s="52">
+        <f>B14/B15</f>
+        <v>20966.6666666667</v>
+      </c>
+      <c r="C16" s="33"/>
+      <c r="D16" s="50"/>
+      <c r="E16" s="33"/>
+      <c r="F16" s="33"/>
+    </row>
+    <row r="17" ht="20.05" customHeight="1">
+      <c r="A17" s="46"/>
+      <c r="B17" s="47"/>
+      <c r="C17" s="33"/>
+      <c r="D17" s="50"/>
+      <c r="E17" s="33"/>
+      <c r="F17" s="33"/>
+    </row>
+    <row r="18" ht="20.05" customHeight="1">
+      <c r="A18" s="46"/>
+      <c r="B18" t="s" s="53">
+        <v>53</v>
+      </c>
+      <c r="C18" s="54"/>
+      <c r="D18" t="s" s="55">
+        <v>54</v>
+      </c>
+      <c r="E18" s="33"/>
+      <c r="F18" s="33"/>
+    </row>
+    <row r="19" ht="20.05" customHeight="1">
+      <c r="A19" t="s" s="42">
+        <v>55</v>
+      </c>
+      <c r="B19" s="43">
+        <v>100</v>
+      </c>
+      <c r="C19" s="33"/>
+      <c r="D19" s="34">
+        <v>100</v>
+      </c>
+      <c r="E19" s="33"/>
+      <c r="F19" s="33"/>
+    </row>
+    <row r="20" ht="20.05" customHeight="1">
+      <c r="A20" t="s" s="42">
+        <v>10</v>
+      </c>
+      <c r="B20" s="52">
+        <f>B19*$B16</f>
+        <v>2096666.66666667</v>
+      </c>
+      <c r="C20" s="33"/>
+      <c r="D20" s="35">
+        <f>D19*$B16</f>
+        <v>2096666.66666667</v>
+      </c>
+      <c r="E20" s="33"/>
+      <c r="F20" s="33"/>
+    </row>
+    <row r="21" ht="20.05" customHeight="1">
+      <c r="A21" t="s" s="42">
+        <v>56</v>
+      </c>
+      <c r="B21" s="52">
+        <f>B20-$B14</f>
+        <v>2049491.66666667</v>
+      </c>
+      <c r="C21" s="33"/>
+      <c r="D21" s="35">
+        <f>D20-$B14</f>
+        <v>2049491.66666667</v>
+      </c>
+      <c r="E21" s="33"/>
+      <c r="F21" s="33"/>
+    </row>
+    <row r="22" ht="20.05" customHeight="1">
+      <c r="A22" t="s" s="42">
+        <v>44</v>
+      </c>
+      <c r="B22" s="48">
+        <v>0.541</v>
+      </c>
+      <c r="C22" s="33"/>
+      <c r="D22" s="56">
         <v>0.371</v>
       </c>
-      <c r="C8" s="22"/>
-      <c r="D8" t="s" s="38">
-        <v>43</v>
-      </c>
-      <c r="E8" s="22"/>
-      <c r="F8" s="22"/>
-    </row>
-    <row r="9" ht="20.05" customHeight="1">
-      <c r="A9" t="s" s="31">
-        <v>44</v>
-      </c>
-      <c r="B9" s="34">
-        <f>B8*B7</f>
-        <v>16695</v>
-      </c>
-      <c r="C9" s="22"/>
-      <c r="D9" s="39"/>
-      <c r="E9" s="22"/>
-      <c r="F9" s="22"/>
-    </row>
-    <row r="10" ht="20.05" customHeight="1">
-      <c r="A10" t="s" s="31">
-        <v>45</v>
-      </c>
-      <c r="B10" s="34">
-        <f>B7-B9</f>
-        <v>28305</v>
-      </c>
-      <c r="C10" s="22"/>
-      <c r="D10" s="39"/>
-      <c r="E10" s="22"/>
-      <c r="F10" s="22"/>
-    </row>
-    <row r="11" ht="20.05" customHeight="1">
-      <c r="A11" s="35"/>
-      <c r="B11" s="36"/>
-      <c r="C11" s="22"/>
-      <c r="D11" s="39"/>
-      <c r="E11" s="22"/>
-      <c r="F11" s="22"/>
-    </row>
-    <row r="12" ht="20.05" customHeight="1">
-      <c r="A12" t="s" s="31">
+      <c r="E22" s="33"/>
+      <c r="F22" s="33"/>
+    </row>
+    <row r="23" ht="20.05" customHeight="1">
+      <c r="A23" t="s" s="42">
         <v>46</v>
       </c>
-      <c r="B12" s="36"/>
-      <c r="C12" s="22"/>
-      <c r="D12" s="39"/>
-      <c r="E12" s="22"/>
-      <c r="F12" s="22"/>
-    </row>
-    <row r="13" ht="20.05" customHeight="1">
-      <c r="A13" t="s" s="31">
+      <c r="B23" s="52">
+        <f>B22*B21</f>
+        <v>1108774.99166667</v>
+      </c>
+      <c r="C23" s="33"/>
+      <c r="D23" s="35">
+        <f>D22*D21</f>
+        <v>760361.408333335</v>
+      </c>
+      <c r="E23" s="33"/>
+      <c r="F23" s="33"/>
+    </row>
+    <row r="24" ht="20.05" customHeight="1">
+      <c r="A24" t="s" s="42">
         <v>47</v>
       </c>
-      <c r="B13" s="40">
-        <v>1</v>
-      </c>
-      <c r="C13" s="22"/>
-      <c r="D13" s="39"/>
-      <c r="E13" s="22"/>
-      <c r="F13" s="22"/>
-    </row>
-    <row r="14" ht="20.05" customHeight="1">
-      <c r="A14" t="s" s="31">
-        <v>48</v>
-      </c>
-      <c r="B14" s="34">
-        <f>B13*B10</f>
-        <v>28305</v>
-      </c>
-      <c r="C14" s="22"/>
-      <c r="D14" s="39"/>
-      <c r="E14" s="22"/>
-      <c r="F14" s="22"/>
-    </row>
-    <row r="15" ht="20.05" customHeight="1">
-      <c r="A15" t="s" s="31">
-        <v>49</v>
-      </c>
-      <c r="B15" s="32">
-        <v>2.28</v>
-      </c>
-      <c r="C15" s="22"/>
-      <c r="D15" s="39"/>
-      <c r="E15" s="22"/>
-      <c r="F15" s="22"/>
-    </row>
-    <row r="16" ht="20.05" customHeight="1">
-      <c r="A16" t="s" s="31">
-        <v>50</v>
-      </c>
-      <c r="B16" s="41">
-        <f>B14/B15</f>
-        <v>12414.4736842105</v>
-      </c>
-      <c r="C16" s="22"/>
-      <c r="D16" s="39"/>
-      <c r="E16" s="22"/>
-      <c r="F16" s="22"/>
-    </row>
-    <row r="17" ht="20.05" customHeight="1">
-      <c r="A17" s="35"/>
-      <c r="B17" s="36"/>
-      <c r="C17" s="22"/>
-      <c r="D17" s="39"/>
-      <c r="E17" s="22"/>
-      <c r="F17" s="22"/>
-    </row>
-    <row r="18" ht="20.05" customHeight="1">
-      <c r="A18" s="35"/>
-      <c r="B18" t="s" s="42">
-        <v>51</v>
-      </c>
-      <c r="C18" s="43"/>
-      <c r="D18" t="s" s="44">
-        <v>52</v>
-      </c>
-      <c r="E18" s="22"/>
-      <c r="F18" s="22"/>
-    </row>
-    <row r="19" ht="20.05" customHeight="1">
-      <c r="A19" t="s" s="31">
-        <v>53</v>
-      </c>
-      <c r="B19" s="32">
-        <v>100</v>
-      </c>
-      <c r="C19" s="22"/>
-      <c r="D19" s="23">
-        <v>100</v>
-      </c>
-      <c r="E19" s="22"/>
-      <c r="F19" s="22"/>
-    </row>
-    <row r="20" ht="20.05" customHeight="1">
-      <c r="A20" t="s" s="31">
-        <v>8</v>
-      </c>
-      <c r="B20" s="41">
-        <f>B19*$B16</f>
-        <v>1241447.36842105</v>
-      </c>
-      <c r="C20" s="22"/>
-      <c r="D20" s="24">
-        <f>D19*$B16</f>
-        <v>1241447.36842105</v>
-      </c>
-      <c r="E20" s="22"/>
-      <c r="F20" s="22"/>
-    </row>
-    <row r="21" ht="20.05" customHeight="1">
-      <c r="A21" t="s" s="31">
-        <v>54</v>
-      </c>
-      <c r="B21" s="41">
-        <f>B20-$B14</f>
-        <v>1213142.36842105</v>
-      </c>
-      <c r="C21" s="22"/>
-      <c r="D21" s="24">
-        <f>D20-$B14</f>
-        <v>1213142.36842105</v>
-      </c>
-      <c r="E21" s="22"/>
-      <c r="F21" s="22"/>
-    </row>
-    <row r="22" ht="20.05" customHeight="1">
-      <c r="A22" t="s" s="31">
-        <v>42</v>
-      </c>
-      <c r="B22" s="37">
-        <v>0.541</v>
-      </c>
-      <c r="C22" s="22"/>
-      <c r="D22" s="45">
-        <v>0.371</v>
-      </c>
-      <c r="E22" s="22"/>
-      <c r="F22" s="22"/>
-    </row>
-    <row r="23" ht="20.05" customHeight="1">
-      <c r="A23" t="s" s="31">
-        <v>44</v>
-      </c>
-      <c r="B23" s="41">
-        <f>B22*B21</f>
-        <v>656310.021315788</v>
-      </c>
-      <c r="C23" s="22"/>
-      <c r="D23" s="24">
-        <f>D22*D21</f>
-        <v>450075.81868421</v>
-      </c>
-      <c r="E23" s="22"/>
-      <c r="F23" s="22"/>
-    </row>
-    <row r="24" ht="20.05" customHeight="1">
-      <c r="A24" t="s" s="31">
-        <v>45</v>
-      </c>
-      <c r="B24" s="41">
+      <c r="B24" s="52">
         <f>B21-B23</f>
-        <v>556832.347105262</v>
-      </c>
-      <c r="C24" s="22"/>
-      <c r="D24" s="24">
+        <v>940716.675</v>
+      </c>
+      <c r="C24" s="33"/>
+      <c r="D24" s="35">
         <f>D21-D23</f>
-        <v>763066.54973684</v>
-      </c>
-      <c r="E24" s="22"/>
-      <c r="F24" s="22"/>
+        <v>1289130.25833334</v>
+      </c>
+      <c r="E24" s="33"/>
+      <c r="F24" s="33"/>
     </row>
     <row r="25" ht="20.05" customHeight="1">
-      <c r="A25" s="35"/>
-      <c r="B25" s="36"/>
-      <c r="C25" s="22"/>
-      <c r="D25" s="39"/>
-      <c r="E25" s="22"/>
-      <c r="F25" s="22"/>
+      <c r="A25" s="46"/>
+      <c r="B25" s="47"/>
+      <c r="C25" s="33"/>
+      <c r="D25" s="50"/>
+      <c r="E25" s="33"/>
+      <c r="F25" s="33"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2749,4 +3463,1334 @@
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="B2:X20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
+      <pane topLeftCell="C3" xSplit="2" ySplit="2" activePane="bottomRight" state="frozen"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col min="1" max="1" width="3.40625" style="57" customWidth="1"/>
+    <col min="2" max="2" width="44.6562" style="57" customWidth="1"/>
+    <col min="3" max="24" width="15.3047" style="57" customWidth="1"/>
+    <col min="25" max="16384" width="16.3516" style="57" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="36.45" customHeight="1">
+      <c r="B1" t="s" s="58">
+        <v>58</v>
+      </c>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
+      <c r="E1" s="58"/>
+      <c r="F1" s="58"/>
+      <c r="G1" s="58"/>
+      <c r="H1" s="58"/>
+      <c r="I1" s="58"/>
+      <c r="J1" s="58"/>
+      <c r="K1" s="58"/>
+      <c r="L1" s="58"/>
+      <c r="M1" s="58"/>
+      <c r="N1" s="58"/>
+      <c r="O1" s="58"/>
+      <c r="P1" s="58"/>
+      <c r="Q1" s="58"/>
+      <c r="R1" s="58"/>
+      <c r="S1" s="58"/>
+      <c r="T1" s="58"/>
+      <c r="U1" s="58"/>
+      <c r="V1" s="58"/>
+      <c r="W1" s="58"/>
+      <c r="X1" s="58"/>
+    </row>
+    <row r="2" ht="20.55" customHeight="1">
+      <c r="B2" t="s" s="59">
+        <v>8</v>
+      </c>
+      <c r="C2" s="60">
+        <v>30</v>
+      </c>
+      <c r="D2" s="60">
+        <v>40</v>
+      </c>
+      <c r="E2" s="60">
+        <v>50</v>
+      </c>
+      <c r="F2" s="60">
+        <v>60</v>
+      </c>
+      <c r="G2" s="60">
+        <f>F2+5</f>
+        <v>65</v>
+      </c>
+      <c r="H2" s="60">
+        <f>F2+10</f>
+        <v>70</v>
+      </c>
+      <c r="I2" s="60">
+        <f>H2+5</f>
+        <v>75</v>
+      </c>
+      <c r="J2" s="60">
+        <f>H2+10</f>
+        <v>80</v>
+      </c>
+      <c r="K2" s="60">
+        <f>J2+5</f>
+        <v>85</v>
+      </c>
+      <c r="L2" s="60">
+        <f>J2+10</f>
+        <v>90</v>
+      </c>
+      <c r="M2" s="60">
+        <f>L2+5</f>
+        <v>95</v>
+      </c>
+      <c r="N2" s="60">
+        <f>L2+10</f>
+        <v>100</v>
+      </c>
+      <c r="O2" s="60">
+        <f>N2+5</f>
+        <v>105</v>
+      </c>
+      <c r="P2" s="60">
+        <f>O2+5</f>
+        <v>110</v>
+      </c>
+      <c r="Q2" s="60">
+        <f>P2+5</f>
+        <v>115</v>
+      </c>
+      <c r="R2" s="60">
+        <f>Q2+5</f>
+        <v>120</v>
+      </c>
+      <c r="S2" s="60">
+        <f>R2+5</f>
+        <v>125</v>
+      </c>
+      <c r="T2" s="60">
+        <f>S2+5</f>
+        <v>130</v>
+      </c>
+      <c r="U2" s="60">
+        <f>T2+5</f>
+        <v>135</v>
+      </c>
+      <c r="V2" s="60">
+        <f>U2+5</f>
+        <v>140</v>
+      </c>
+      <c r="W2" s="60">
+        <f>V2+5</f>
+        <v>145</v>
+      </c>
+      <c r="X2" s="60">
+        <f>W2+5</f>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="3" ht="20.35" customHeight="1">
+      <c r="B3" t="s" s="61">
+        <v>9</v>
+      </c>
+      <c r="C3" s="62">
+        <v>30</v>
+      </c>
+      <c r="D3" s="63">
+        <v>30</v>
+      </c>
+      <c r="E3" s="63">
+        <v>30</v>
+      </c>
+      <c r="F3" s="63">
+        <v>30</v>
+      </c>
+      <c r="G3" s="63">
+        <v>30</v>
+      </c>
+      <c r="H3" s="63">
+        <v>30</v>
+      </c>
+      <c r="I3" s="63">
+        <v>30</v>
+      </c>
+      <c r="J3" s="63">
+        <v>30</v>
+      </c>
+      <c r="K3" s="63">
+        <v>30</v>
+      </c>
+      <c r="L3" s="63">
+        <v>30</v>
+      </c>
+      <c r="M3" s="63">
+        <v>30</v>
+      </c>
+      <c r="N3" s="63">
+        <v>30</v>
+      </c>
+      <c r="O3" s="63">
+        <v>30</v>
+      </c>
+      <c r="P3" s="63">
+        <v>30</v>
+      </c>
+      <c r="Q3" s="63">
+        <v>30</v>
+      </c>
+      <c r="R3" s="63">
+        <v>30</v>
+      </c>
+      <c r="S3" s="63">
+        <v>30</v>
+      </c>
+      <c r="T3" s="63">
+        <v>30</v>
+      </c>
+      <c r="U3" s="63">
+        <v>30</v>
+      </c>
+      <c r="V3" s="63">
+        <v>30</v>
+      </c>
+      <c r="W3" s="63">
+        <v>30</v>
+      </c>
+      <c r="X3" s="63">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" ht="20.35" customHeight="1">
+      <c r="B4" t="s" s="64">
+        <v>10</v>
+      </c>
+      <c r="C4" s="65">
+        <f>C2-C3</f>
+        <v>0</v>
+      </c>
+      <c r="D4" s="66">
+        <f>D2-D3</f>
+        <v>10</v>
+      </c>
+      <c r="E4" s="66">
+        <f>E2-E3</f>
+        <v>20</v>
+      </c>
+      <c r="F4" s="66">
+        <f>F2-F3</f>
+        <v>30</v>
+      </c>
+      <c r="G4" s="66">
+        <f>G2-G3</f>
+        <v>35</v>
+      </c>
+      <c r="H4" s="66">
+        <f>H2-H3</f>
+        <v>40</v>
+      </c>
+      <c r="I4" s="66">
+        <f>I2-I3</f>
+        <v>45</v>
+      </c>
+      <c r="J4" s="66">
+        <f>J2-J3</f>
+        <v>50</v>
+      </c>
+      <c r="K4" s="66">
+        <f>K2-K3</f>
+        <v>55</v>
+      </c>
+      <c r="L4" s="66">
+        <f>L2-L3</f>
+        <v>60</v>
+      </c>
+      <c r="M4" s="66">
+        <f>M2-M3</f>
+        <v>65</v>
+      </c>
+      <c r="N4" s="66">
+        <f>N2-N3</f>
+        <v>70</v>
+      </c>
+      <c r="O4" s="66">
+        <f>O2-O3</f>
+        <v>75</v>
+      </c>
+      <c r="P4" s="66">
+        <f>P2-P3</f>
+        <v>80</v>
+      </c>
+      <c r="Q4" s="66">
+        <f>Q2-Q3</f>
+        <v>85</v>
+      </c>
+      <c r="R4" s="66">
+        <f>R2-R3</f>
+        <v>90</v>
+      </c>
+      <c r="S4" s="66">
+        <f>S2-S3</f>
+        <v>95</v>
+      </c>
+      <c r="T4" s="66">
+        <f>T2-T3</f>
+        <v>100</v>
+      </c>
+      <c r="U4" s="66">
+        <f>U2-U3</f>
+        <v>105</v>
+      </c>
+      <c r="V4" s="66">
+        <f>V2-V3</f>
+        <v>110</v>
+      </c>
+      <c r="W4" s="66">
+        <f>W2-W3</f>
+        <v>115</v>
+      </c>
+      <c r="X4" s="66">
+        <f>X2-X3</f>
+        <v>120</v>
+      </c>
+    </row>
+    <row r="5" ht="20.35" customHeight="1">
+      <c r="B5" s="67"/>
+      <c r="C5" s="68"/>
+      <c r="D5" s="69"/>
+      <c r="E5" s="69"/>
+      <c r="F5" s="69"/>
+      <c r="G5" s="69"/>
+      <c r="H5" s="69"/>
+      <c r="I5" s="69"/>
+      <c r="J5" s="69"/>
+      <c r="K5" s="69"/>
+      <c r="L5" s="69"/>
+      <c r="M5" s="69"/>
+      <c r="N5" s="69"/>
+      <c r="O5" s="69"/>
+      <c r="P5" s="69"/>
+      <c r="Q5" s="69"/>
+      <c r="R5" s="69"/>
+      <c r="S5" s="69"/>
+      <c r="T5" s="69"/>
+      <c r="U5" s="69"/>
+      <c r="V5" s="69"/>
+      <c r="W5" s="69"/>
+      <c r="X5" s="69"/>
+    </row>
+    <row r="6" ht="20.35" customHeight="1">
+      <c r="B6" t="s" s="64">
+        <v>11</v>
+      </c>
+      <c r="C6" s="70">
+        <v>0.12</v>
+      </c>
+      <c r="D6" s="71">
+        <v>0.12</v>
+      </c>
+      <c r="E6" s="71">
+        <v>0.12</v>
+      </c>
+      <c r="F6" s="71">
+        <v>0.12</v>
+      </c>
+      <c r="G6" s="71">
+        <v>0.12</v>
+      </c>
+      <c r="H6" s="71">
+        <v>0.12</v>
+      </c>
+      <c r="I6" s="71">
+        <v>0.12</v>
+      </c>
+      <c r="J6" s="71">
+        <v>0.12</v>
+      </c>
+      <c r="K6" s="71">
+        <v>0.12</v>
+      </c>
+      <c r="L6" s="71">
+        <v>0.12</v>
+      </c>
+      <c r="M6" s="71">
+        <v>0.12</v>
+      </c>
+      <c r="N6" s="71">
+        <v>0.12</v>
+      </c>
+      <c r="O6" s="71">
+        <v>0.12</v>
+      </c>
+      <c r="P6" s="71">
+        <v>0.12</v>
+      </c>
+      <c r="Q6" s="71">
+        <v>0.12</v>
+      </c>
+      <c r="R6" s="71">
+        <v>0.12</v>
+      </c>
+      <c r="S6" s="71">
+        <v>0.12</v>
+      </c>
+      <c r="T6" s="71">
+        <v>0.12</v>
+      </c>
+      <c r="U6" s="71">
+        <v>0.12</v>
+      </c>
+      <c r="V6" s="71">
+        <v>0.12</v>
+      </c>
+      <c r="W6" s="71">
+        <v>0.12</v>
+      </c>
+      <c r="X6" s="71">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="7" ht="20.35" customHeight="1">
+      <c r="B7" t="s" s="64">
+        <v>12</v>
+      </c>
+      <c r="C7" s="65">
+        <f>C6*C4</f>
+        <v>0</v>
+      </c>
+      <c r="D7" s="66">
+        <f>D6*D4</f>
+        <v>1.2</v>
+      </c>
+      <c r="E7" s="66">
+        <f>E6*E4</f>
+        <v>2.4</v>
+      </c>
+      <c r="F7" s="66">
+        <f>F6*F4</f>
+        <v>3.6</v>
+      </c>
+      <c r="G7" s="66">
+        <f>G6*G4</f>
+        <v>4.2</v>
+      </c>
+      <c r="H7" s="66">
+        <f>H6*H4</f>
+        <v>4.8</v>
+      </c>
+      <c r="I7" s="66">
+        <f>I6*I4</f>
+        <v>5.4</v>
+      </c>
+      <c r="J7" s="66">
+        <f>J6*J4</f>
+        <v>6</v>
+      </c>
+      <c r="K7" s="66">
+        <f>K6*K4</f>
+        <v>6.6</v>
+      </c>
+      <c r="L7" s="66">
+        <f>L6*L4</f>
+        <v>7.2</v>
+      </c>
+      <c r="M7" s="66">
+        <f>M6*M4</f>
+        <v>7.8</v>
+      </c>
+      <c r="N7" s="66">
+        <f>N6*N4</f>
+        <v>8.4</v>
+      </c>
+      <c r="O7" s="66">
+        <f>O6*O4</f>
+        <v>9</v>
+      </c>
+      <c r="P7" s="66">
+        <f>P6*P4</f>
+        <v>9.6</v>
+      </c>
+      <c r="Q7" s="66">
+        <f>Q6*Q4</f>
+        <v>10.2</v>
+      </c>
+      <c r="R7" s="66">
+        <f>R6*R4</f>
+        <v>10.8</v>
+      </c>
+      <c r="S7" s="66">
+        <f>S6*S4</f>
+        <v>11.4</v>
+      </c>
+      <c r="T7" s="66">
+        <f>T6*T4</f>
+        <v>12</v>
+      </c>
+      <c r="U7" s="66">
+        <f>U6*U4</f>
+        <v>12.6</v>
+      </c>
+      <c r="V7" s="66">
+        <f>V6*V4</f>
+        <v>13.2</v>
+      </c>
+      <c r="W7" s="66">
+        <f>W6*W4</f>
+        <v>13.8</v>
+      </c>
+      <c r="X7" s="66">
+        <f>X6*X4</f>
+        <v>14.4</v>
+      </c>
+    </row>
+    <row r="8" ht="20.35" customHeight="1">
+      <c r="B8" s="67"/>
+      <c r="C8" s="68"/>
+      <c r="D8" s="69"/>
+      <c r="E8" s="69"/>
+      <c r="F8" s="69"/>
+      <c r="G8" s="69"/>
+      <c r="H8" s="69"/>
+      <c r="I8" s="69"/>
+      <c r="J8" s="69"/>
+      <c r="K8" s="69"/>
+      <c r="L8" s="69"/>
+      <c r="M8" s="69"/>
+      <c r="N8" s="69"/>
+      <c r="O8" s="69"/>
+      <c r="P8" s="69"/>
+      <c r="Q8" s="69"/>
+      <c r="R8" s="69"/>
+      <c r="S8" s="69"/>
+      <c r="T8" s="69"/>
+      <c r="U8" s="69"/>
+      <c r="V8" s="69"/>
+      <c r="W8" s="69"/>
+      <c r="X8" s="69"/>
+    </row>
+    <row r="9" ht="20.35" customHeight="1">
+      <c r="B9" t="s" s="64">
+        <v>13</v>
+      </c>
+      <c r="C9" s="70">
+        <v>0.49</v>
+      </c>
+      <c r="D9" s="71">
+        <v>0.49</v>
+      </c>
+      <c r="E9" s="71">
+        <v>0.49</v>
+      </c>
+      <c r="F9" s="71">
+        <v>0.49</v>
+      </c>
+      <c r="G9" s="71">
+        <v>0.49</v>
+      </c>
+      <c r="H9" s="71">
+        <v>0.49</v>
+      </c>
+      <c r="I9" s="71">
+        <v>0.49</v>
+      </c>
+      <c r="J9" s="71">
+        <v>0.49</v>
+      </c>
+      <c r="K9" s="71">
+        <v>0.49</v>
+      </c>
+      <c r="L9" s="71">
+        <v>0.49</v>
+      </c>
+      <c r="M9" s="71">
+        <v>0.49</v>
+      </c>
+      <c r="N9" s="71">
+        <v>0.49</v>
+      </c>
+      <c r="O9" s="71">
+        <v>0.49</v>
+      </c>
+      <c r="P9" s="71">
+        <v>0.49</v>
+      </c>
+      <c r="Q9" s="71">
+        <v>0.49</v>
+      </c>
+      <c r="R9" s="71">
+        <v>0.49</v>
+      </c>
+      <c r="S9" s="71">
+        <v>0.49</v>
+      </c>
+      <c r="T9" s="71">
+        <v>0.49</v>
+      </c>
+      <c r="U9" s="71">
+        <v>0.49</v>
+      </c>
+      <c r="V9" s="71">
+        <v>0.49</v>
+      </c>
+      <c r="W9" s="71">
+        <v>0.49</v>
+      </c>
+      <c r="X9" s="71">
+        <v>0.49</v>
+      </c>
+    </row>
+    <row r="10" ht="20.35" customHeight="1">
+      <c r="B10" t="s" s="64">
+        <v>14</v>
+      </c>
+      <c r="C10" s="72">
+        <f>C7*C9</f>
+        <v>0</v>
+      </c>
+      <c r="D10" s="73">
+        <f>D7*D9</f>
+        <v>0.588</v>
+      </c>
+      <c r="E10" s="73">
+        <f>E7*E9</f>
+        <v>1.176</v>
+      </c>
+      <c r="F10" s="73">
+        <f>F7*F9</f>
+        <v>1.764</v>
+      </c>
+      <c r="G10" s="73">
+        <f>G7*G9</f>
+        <v>2.058</v>
+      </c>
+      <c r="H10" s="73">
+        <f>H7*H9</f>
+        <v>2.352</v>
+      </c>
+      <c r="I10" s="73">
+        <f>I7*I9</f>
+        <v>2.646</v>
+      </c>
+      <c r="J10" s="73">
+        <f>J7*J9</f>
+        <v>2.94</v>
+      </c>
+      <c r="K10" s="73">
+        <f>K7*K9</f>
+        <v>3.234</v>
+      </c>
+      <c r="L10" s="73">
+        <f>L7*L9</f>
+        <v>3.528</v>
+      </c>
+      <c r="M10" s="73">
+        <f>M7*M9</f>
+        <v>3.822</v>
+      </c>
+      <c r="N10" s="73">
+        <f>N7*N9</f>
+        <v>4.116</v>
+      </c>
+      <c r="O10" s="73">
+        <f>O7*O9</f>
+        <v>4.41</v>
+      </c>
+      <c r="P10" s="73">
+        <f>P7*P9</f>
+        <v>4.704</v>
+      </c>
+      <c r="Q10" s="73">
+        <f>Q7*Q9</f>
+        <v>4.998</v>
+      </c>
+      <c r="R10" s="73">
+        <f>R7*R9</f>
+        <v>5.292</v>
+      </c>
+      <c r="S10" s="73">
+        <f>S7*S9</f>
+        <v>5.586</v>
+      </c>
+      <c r="T10" s="73">
+        <f>T7*T9</f>
+        <v>5.88</v>
+      </c>
+      <c r="U10" s="73">
+        <f>U7*U9</f>
+        <v>6.174</v>
+      </c>
+      <c r="V10" s="73">
+        <f>V7*V9</f>
+        <v>6.468</v>
+      </c>
+      <c r="W10" s="73">
+        <f>W7*W9</f>
+        <v>6.762</v>
+      </c>
+      <c r="X10" s="73">
+        <f>X7*X9</f>
+        <v>7.056</v>
+      </c>
+    </row>
+    <row r="11" ht="20.35" customHeight="1">
+      <c r="B11" s="67"/>
+      <c r="C11" s="68"/>
+      <c r="D11" s="69"/>
+      <c r="E11" s="69"/>
+      <c r="F11" s="69"/>
+      <c r="G11" s="69"/>
+      <c r="H11" s="69"/>
+      <c r="I11" s="69"/>
+      <c r="J11" s="69"/>
+      <c r="K11" s="69"/>
+      <c r="L11" s="69"/>
+      <c r="M11" s="69"/>
+      <c r="N11" s="69"/>
+      <c r="O11" s="69"/>
+      <c r="P11" s="69"/>
+      <c r="Q11" s="69"/>
+      <c r="R11" s="69"/>
+      <c r="S11" s="69"/>
+      <c r="T11" s="69"/>
+      <c r="U11" s="69"/>
+      <c r="V11" s="69"/>
+      <c r="W11" s="69"/>
+      <c r="X11" s="69"/>
+    </row>
+    <row r="12" ht="20.35" customHeight="1">
+      <c r="B12" t="s" s="64">
+        <v>15</v>
+      </c>
+      <c r="C12" s="68"/>
+      <c r="D12" s="69"/>
+      <c r="E12" s="69"/>
+      <c r="F12" s="69"/>
+      <c r="G12" s="69"/>
+      <c r="H12" s="69"/>
+      <c r="I12" s="69"/>
+      <c r="J12" s="69"/>
+      <c r="K12" s="69"/>
+      <c r="L12" s="69"/>
+      <c r="M12" s="69"/>
+      <c r="N12" s="69"/>
+      <c r="O12" s="69"/>
+      <c r="P12" s="69"/>
+      <c r="Q12" s="69"/>
+      <c r="R12" s="69"/>
+      <c r="S12" s="69"/>
+      <c r="T12" s="69"/>
+      <c r="U12" s="69"/>
+      <c r="V12" s="69"/>
+      <c r="W12" s="69"/>
+      <c r="X12" s="69"/>
+    </row>
+    <row r="13" ht="20.35" customHeight="1">
+      <c r="B13" t="s" s="64">
+        <v>16</v>
+      </c>
+      <c r="C13" s="74">
+        <v>3200000000</v>
+      </c>
+      <c r="D13" s="75">
+        <v>3200000000</v>
+      </c>
+      <c r="E13" s="75">
+        <v>3200000000</v>
+      </c>
+      <c r="F13" s="75">
+        <v>3200000000</v>
+      </c>
+      <c r="G13" s="75">
+        <v>3200000000</v>
+      </c>
+      <c r="H13" s="75">
+        <v>3200000000</v>
+      </c>
+      <c r="I13" s="75">
+        <v>3200000000</v>
+      </c>
+      <c r="J13" s="75">
+        <v>3200000000</v>
+      </c>
+      <c r="K13" s="75">
+        <v>3200000000</v>
+      </c>
+      <c r="L13" s="75">
+        <v>3200000000</v>
+      </c>
+      <c r="M13" s="75">
+        <v>3200000000</v>
+      </c>
+      <c r="N13" s="75">
+        <v>3200000000</v>
+      </c>
+      <c r="O13" s="75">
+        <v>3200000000</v>
+      </c>
+      <c r="P13" s="75">
+        <v>3200000000</v>
+      </c>
+      <c r="Q13" s="75">
+        <v>3200000000</v>
+      </c>
+      <c r="R13" s="75">
+        <v>3200000000</v>
+      </c>
+      <c r="S13" s="75">
+        <v>3200000000</v>
+      </c>
+      <c r="T13" s="75">
+        <v>3200000000</v>
+      </c>
+      <c r="U13" s="75">
+        <v>3200000000</v>
+      </c>
+      <c r="V13" s="75">
+        <v>3200000000</v>
+      </c>
+      <c r="W13" s="75">
+        <v>3200000000</v>
+      </c>
+      <c r="X13" s="75">
+        <v>3200000000</v>
+      </c>
+    </row>
+    <row r="14" ht="20.35" customHeight="1">
+      <c r="B14" t="s" s="64">
+        <v>17</v>
+      </c>
+      <c r="C14" s="74">
+        <f>C13*C$10</f>
+        <v>0</v>
+      </c>
+      <c r="D14" s="75">
+        <f>D13*D$10</f>
+        <v>1881600000</v>
+      </c>
+      <c r="E14" s="75">
+        <f>E13*E$10</f>
+        <v>3763200000</v>
+      </c>
+      <c r="F14" s="75">
+        <f>F13*F$10</f>
+        <v>5644800000</v>
+      </c>
+      <c r="G14" s="75">
+        <f>G13*G$10</f>
+        <v>6585600000</v>
+      </c>
+      <c r="H14" s="75">
+        <f>H13*H$10</f>
+        <v>7526400000</v>
+      </c>
+      <c r="I14" s="75">
+        <f>I13*I$10</f>
+        <v>8467200000</v>
+      </c>
+      <c r="J14" s="75">
+        <f>J13*J$10</f>
+        <v>9408000000</v>
+      </c>
+      <c r="K14" s="75">
+        <f>K13*K$10</f>
+        <v>10348800000</v>
+      </c>
+      <c r="L14" s="75">
+        <f>L13*L$10</f>
+        <v>11289600000</v>
+      </c>
+      <c r="M14" s="75">
+        <f>M13*M$10</f>
+        <v>12230400000</v>
+      </c>
+      <c r="N14" s="75">
+        <f>N13*N$10</f>
+        <v>13171200000</v>
+      </c>
+      <c r="O14" s="75">
+        <f>O13*O$10</f>
+        <v>14112000000</v>
+      </c>
+      <c r="P14" s="75">
+        <f>P13*P$10</f>
+        <v>15052800000</v>
+      </c>
+      <c r="Q14" s="75">
+        <f>Q13*Q$10</f>
+        <v>15993600000</v>
+      </c>
+      <c r="R14" s="75">
+        <f>R13*R$10</f>
+        <v>16934400000</v>
+      </c>
+      <c r="S14" s="75">
+        <f>S13*S$10</f>
+        <v>17875200000</v>
+      </c>
+      <c r="T14" s="75">
+        <f>T13*T$10</f>
+        <v>18816000000</v>
+      </c>
+      <c r="U14" s="75">
+        <f>U13*U$10</f>
+        <v>19756800000</v>
+      </c>
+      <c r="V14" s="75">
+        <f>V13*V$10</f>
+        <v>20697600000</v>
+      </c>
+      <c r="W14" s="75">
+        <f>W13*W$10</f>
+        <v>21638400000</v>
+      </c>
+      <c r="X14" s="75">
+        <f>X13*X$10</f>
+        <v>22579200000</v>
+      </c>
+    </row>
+    <row r="15" ht="20.35" customHeight="1">
+      <c r="B15" t="s" s="64">
+        <v>18</v>
+      </c>
+      <c r="C15" s="70">
+        <v>0</v>
+      </c>
+      <c r="D15" s="71">
+        <v>0</v>
+      </c>
+      <c r="E15" s="71">
+        <v>0</v>
+      </c>
+      <c r="F15" s="71">
+        <v>0</v>
+      </c>
+      <c r="G15" s="71">
+        <v>0</v>
+      </c>
+      <c r="H15" s="71">
+        <v>0</v>
+      </c>
+      <c r="I15" s="71">
+        <v>0</v>
+      </c>
+      <c r="J15" s="71">
+        <v>0</v>
+      </c>
+      <c r="K15" s="71">
+        <v>0</v>
+      </c>
+      <c r="L15" s="71">
+        <v>0</v>
+      </c>
+      <c r="M15" s="71">
+        <v>0</v>
+      </c>
+      <c r="N15" s="71">
+        <v>0</v>
+      </c>
+      <c r="O15" s="71">
+        <v>0</v>
+      </c>
+      <c r="P15" s="71">
+        <v>0</v>
+      </c>
+      <c r="Q15" s="71">
+        <v>0</v>
+      </c>
+      <c r="R15" s="71">
+        <v>0</v>
+      </c>
+      <c r="S15" s="71">
+        <v>0</v>
+      </c>
+      <c r="T15" s="71">
+        <v>0</v>
+      </c>
+      <c r="U15" s="71">
+        <v>0</v>
+      </c>
+      <c r="V15" s="71">
+        <v>0</v>
+      </c>
+      <c r="W15" s="71">
+        <v>0</v>
+      </c>
+      <c r="X15" s="71">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" ht="20.35" customHeight="1">
+      <c r="B16" t="s" s="64">
+        <v>19</v>
+      </c>
+      <c r="C16" s="76">
+        <v>0.1</v>
+      </c>
+      <c r="D16" s="77">
+        <v>0.1</v>
+      </c>
+      <c r="E16" s="77">
+        <v>0.1</v>
+      </c>
+      <c r="F16" s="77">
+        <v>0.1</v>
+      </c>
+      <c r="G16" s="77">
+        <v>0.1</v>
+      </c>
+      <c r="H16" s="77">
+        <v>0.1</v>
+      </c>
+      <c r="I16" s="77">
+        <v>0.1</v>
+      </c>
+      <c r="J16" s="77">
+        <v>0.1</v>
+      </c>
+      <c r="K16" s="77">
+        <v>0.1</v>
+      </c>
+      <c r="L16" s="77">
+        <v>0.1</v>
+      </c>
+      <c r="M16" s="77">
+        <v>0.1</v>
+      </c>
+      <c r="N16" s="77">
+        <v>0.1</v>
+      </c>
+      <c r="O16" s="77">
+        <v>0.1</v>
+      </c>
+      <c r="P16" s="77">
+        <v>0.1</v>
+      </c>
+      <c r="Q16" s="77">
+        <v>0.1</v>
+      </c>
+      <c r="R16" s="77">
+        <v>0.1</v>
+      </c>
+      <c r="S16" s="77">
+        <v>0.1</v>
+      </c>
+      <c r="T16" s="77">
+        <v>0.1</v>
+      </c>
+      <c r="U16" s="77">
+        <v>0.1</v>
+      </c>
+      <c r="V16" s="77">
+        <v>0.1</v>
+      </c>
+      <c r="W16" s="77">
+        <v>0.1</v>
+      </c>
+      <c r="X16" s="77">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="17" ht="20.35" customHeight="1">
+      <c r="B17" t="s" s="64">
+        <v>20</v>
+      </c>
+      <c r="C17" s="74">
+        <f>C14*(1-(C15+C16))</f>
+        <v>0</v>
+      </c>
+      <c r="D17" s="75">
+        <f>D14*(1-(D15+D16))</f>
+        <v>1693440000</v>
+      </c>
+      <c r="E17" s="75">
+        <f>E14*(1-(E15+E16))</f>
+        <v>3386880000</v>
+      </c>
+      <c r="F17" s="75">
+        <f>F14*(1-(F15+F16))</f>
+        <v>5080320000</v>
+      </c>
+      <c r="G17" s="75">
+        <f>G14*(1-(G15+G16))</f>
+        <v>5927040000</v>
+      </c>
+      <c r="H17" s="75">
+        <f>H14*(1-(H15+H16))</f>
+        <v>6773760000</v>
+      </c>
+      <c r="I17" s="75">
+        <f>I14*(1-(I15+I16))</f>
+        <v>7620480000</v>
+      </c>
+      <c r="J17" s="75">
+        <f>J14*(1-(J15+J16))</f>
+        <v>8467200000</v>
+      </c>
+      <c r="K17" s="75">
+        <f>K14*(1-(K15+K16))</f>
+        <v>9313920000</v>
+      </c>
+      <c r="L17" s="75">
+        <f>L14*(1-(L15+L16))</f>
+        <v>10160640000</v>
+      </c>
+      <c r="M17" s="75">
+        <f>M14*(1-(M15+M16))</f>
+        <v>11007360000</v>
+      </c>
+      <c r="N17" s="75">
+        <f>N14*(1-(N15+N16))</f>
+        <v>11854080000</v>
+      </c>
+      <c r="O17" s="75">
+        <f>O14*(1-(O15+O16))</f>
+        <v>12700800000</v>
+      </c>
+      <c r="P17" s="75">
+        <f>P14*(1-(P15+P16))</f>
+        <v>13547520000</v>
+      </c>
+      <c r="Q17" s="75">
+        <f>Q14*(1-(Q15+Q16))</f>
+        <v>14394240000</v>
+      </c>
+      <c r="R17" s="75">
+        <f>R14*(1-(R15+R16))</f>
+        <v>15240960000</v>
+      </c>
+      <c r="S17" s="75">
+        <f>S14*(1-(S15+S16))</f>
+        <v>16087680000</v>
+      </c>
+      <c r="T17" s="75">
+        <f>T14*(1-(T15+T16))</f>
+        <v>16934400000</v>
+      </c>
+      <c r="U17" s="75">
+        <f>U14*(1-(U15+U16))</f>
+        <v>17781120000</v>
+      </c>
+      <c r="V17" s="75">
+        <f>V14*(1-(V15+V16))</f>
+        <v>18627840000</v>
+      </c>
+      <c r="W17" s="75">
+        <f>W14*(1-(W15+W16))</f>
+        <v>19474560000</v>
+      </c>
+      <c r="X17" s="75">
+        <f>X14*(1-(X15+X16))</f>
+        <v>20321280000</v>
+      </c>
+    </row>
+    <row r="18" ht="20.35" customHeight="1">
+      <c r="B18" t="s" s="64">
+        <v>21</v>
+      </c>
+      <c r="C18" s="74">
+        <v>164923363</v>
+      </c>
+      <c r="D18" s="75">
+        <v>164923363</v>
+      </c>
+      <c r="E18" s="75">
+        <v>164923363</v>
+      </c>
+      <c r="F18" s="75">
+        <v>164923363</v>
+      </c>
+      <c r="G18" s="75">
+        <v>164923363</v>
+      </c>
+      <c r="H18" s="75">
+        <v>164923363</v>
+      </c>
+      <c r="I18" s="75">
+        <v>164923363</v>
+      </c>
+      <c r="J18" s="75">
+        <v>164923363</v>
+      </c>
+      <c r="K18" s="75">
+        <v>164923363</v>
+      </c>
+      <c r="L18" s="75">
+        <v>164923363</v>
+      </c>
+      <c r="M18" s="75">
+        <v>164923363</v>
+      </c>
+      <c r="N18" s="75">
+        <v>164923363</v>
+      </c>
+      <c r="O18" s="75">
+        <v>164923363</v>
+      </c>
+      <c r="P18" s="75">
+        <v>164923363</v>
+      </c>
+      <c r="Q18" s="75">
+        <v>164923363</v>
+      </c>
+      <c r="R18" s="75">
+        <v>164923363</v>
+      </c>
+      <c r="S18" s="75">
+        <v>164923363</v>
+      </c>
+      <c r="T18" s="75">
+        <v>164923363</v>
+      </c>
+      <c r="U18" s="75">
+        <v>164923363</v>
+      </c>
+      <c r="V18" s="75">
+        <v>164923363</v>
+      </c>
+      <c r="W18" s="75">
+        <v>164923363</v>
+      </c>
+      <c r="X18" s="75">
+        <v>164923363</v>
+      </c>
+    </row>
+    <row r="19" ht="20.35" customHeight="1">
+      <c r="B19" t="s" s="64">
+        <v>22</v>
+      </c>
+      <c r="C19" s="65">
+        <f>C17/C18</f>
+        <v>0</v>
+      </c>
+      <c r="D19" s="66">
+        <f>D17/D18</f>
+        <v>10.2680418904628</v>
+      </c>
+      <c r="E19" s="66">
+        <f>E17/E18</f>
+        <v>20.5360837809256</v>
+      </c>
+      <c r="F19" s="66">
+        <f>F17/F18</f>
+        <v>30.8041256713884</v>
+      </c>
+      <c r="G19" s="66">
+        <f>G17/G18</f>
+        <v>35.9381466166197</v>
+      </c>
+      <c r="H19" s="66">
+        <f>H17/H18</f>
+        <v>41.0721675618511</v>
+      </c>
+      <c r="I19" s="66">
+        <f>I17/I18</f>
+        <v>46.2061885070825</v>
+      </c>
+      <c r="J19" s="66">
+        <f>J17/J18</f>
+        <v>51.3402094523139</v>
+      </c>
+      <c r="K19" s="66">
+        <f>K17/K18</f>
+        <v>56.4742303975453</v>
+      </c>
+      <c r="L19" s="66">
+        <f>L17/L18</f>
+        <v>61.6082513427767</v>
+      </c>
+      <c r="M19" s="66">
+        <f>M17/M18</f>
+        <v>66.7422722880081</v>
+      </c>
+      <c r="N19" s="66">
+        <f>N17/N18</f>
+        <v>71.87629323323949</v>
+      </c>
+      <c r="O19" s="66">
+        <f>O17/O18</f>
+        <v>77.01031417847091</v>
+      </c>
+      <c r="P19" s="66">
+        <f>P17/P18</f>
+        <v>82.14433512370231</v>
+      </c>
+      <c r="Q19" s="66">
+        <f>Q17/Q18</f>
+        <v>87.2783560689337</v>
+      </c>
+      <c r="R19" s="66">
+        <f>R17/R18</f>
+        <v>92.4123770141651</v>
+      </c>
+      <c r="S19" s="66">
+        <f>S17/S18</f>
+        <v>97.5463979593965</v>
+      </c>
+      <c r="T19" s="66">
+        <f>T17/T18</f>
+        <v>102.680418904628</v>
+      </c>
+      <c r="U19" s="66">
+        <f>U17/U18</f>
+        <v>107.814439849859</v>
+      </c>
+      <c r="V19" s="66">
+        <f>V17/V18</f>
+        <v>112.948460795091</v>
+      </c>
+      <c r="W19" s="66">
+        <f>W17/W18</f>
+        <v>118.082481740322</v>
+      </c>
+      <c r="X19" s="66">
+        <f>X17/X18</f>
+        <v>123.216502685553</v>
+      </c>
+    </row>
+    <row r="20" ht="20.35" customHeight="1">
+      <c r="B20" s="67"/>
+      <c r="C20" s="68"/>
+      <c r="D20" s="69"/>
+      <c r="E20" s="69"/>
+      <c r="F20" s="69"/>
+      <c r="G20" s="69"/>
+      <c r="H20" s="69"/>
+      <c r="I20" s="69"/>
+      <c r="J20" s="69"/>
+      <c r="K20" s="69"/>
+      <c r="L20" s="69"/>
+      <c r="M20" s="69"/>
+      <c r="N20" s="69"/>
+      <c r="O20" s="69"/>
+      <c r="P20" s="69"/>
+      <c r="Q20" s="69"/>
+      <c r="R20" s="69"/>
+      <c r="S20" s="69"/>
+      <c r="T20" s="69"/>
+      <c r="U20" s="69"/>
+      <c r="V20" s="69"/>
+      <c r="W20" s="69"/>
+      <c r="X20" s="69"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:X1"/>
+  </mergeCells>
+  <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
+  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <headerFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
+  </headerFooter>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
updated spreadsheet w/ higher COGS and max /bbl oil
</commit_message>
<xml_diff>
--- a/mmtlp_dividend_calc.xlsx
+++ b/mmtlp_dividend_calc.xlsx
@@ -7,15 +7,18 @@
   <sheets>
     <sheet name="Export Summary" sheetId="1" r:id="rId4"/>
     <sheet name="MMTLP_DIVI_CALC - MMTLP_DIVI_CA" sheetId="2" r:id="rId5"/>
-    <sheet name="What Happens if MMTLP Divi Get " sheetId="3" r:id="rId6"/>
-    <sheet name="reinvesting_1000_shares_mmtlp -" sheetId="4" r:id="rId7"/>
-    <sheet name="divi chart from 30 to 150 oil p" sheetId="5" r:id="rId8"/>
+    <sheet name="MMTLP_DIVI_CALC - Table 1" sheetId="3" r:id="rId6"/>
+    <sheet name="MMTLP_DIVI_CALC - Possible MOAS" sheetId="4" r:id="rId7"/>
+    <sheet name="MMTLP_DIVI_CALC - Table 2" sheetId="5" r:id="rId8"/>
+    <sheet name="What Happens if MMTLP Divi Get " sheetId="6" r:id="rId9"/>
+    <sheet name="reinvesting_1000_shares_mmtlp -" sheetId="7" r:id="rId10"/>
+    <sheet name="divi chart from 30 to 150 oil p" sheetId="8" r:id="rId11"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="76">
   <si>
     <t>This document was exported from Numbers.  Each table was converted to an Excel worksheet. All other objects on each Numbers sheet were placed on separate worksheets. Please be aware that formula calculations may differ in Excel.</t>
   </si>
@@ -90,6 +93,54 @@
   </si>
   <si>
     <t>$ (oil in ground)</t>
+  </si>
+  <si>
+    <t>Table 1</t>
+  </si>
+  <si>
+    <t>MMTLP_DIVI_CALC - Table 1</t>
+  </si>
+  <si>
+    <t>CF / bbl oil</t>
+  </si>
+  <si>
+    <t>TCF</t>
+  </si>
+  <si>
+    <t>BCF</t>
+  </si>
+  <si>
+    <t>MMCF</t>
+  </si>
+  <si>
+    <t>Possible MOASS Sell Schedule</t>
+  </si>
+  <si>
+    <t>MMTLP_DIVI_CALC - Possible MOAS</t>
+  </si>
+  <si>
+    <t>Price Multiplier</t>
+  </si>
+  <si>
+    <t>Index</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t># Shares to Sell</t>
+  </si>
+  <si>
+    <t>$</t>
+  </si>
+  <si>
+    <t>Running $</t>
+  </si>
+  <si>
+    <t>Table 2</t>
+  </si>
+  <si>
+    <t>MMTLP_DIVI_CALC - Table 2</t>
   </si>
   <si>
     <t>What Happens if MMTLP Divi Get Re-Invested into MMAT</t>
@@ -208,7 +259,7 @@
     <numFmt numFmtId="61" formatCode="0.0%"/>
     <numFmt numFmtId="62" formatCode="&quot;$&quot;#,##0"/>
   </numFmts>
-  <fonts count="14">
+  <fonts count="16">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -248,6 +299,16 @@
       <name val="Helvetica Neue"/>
     </font>
     <font>
+      <sz val="12"/>
+      <color indexed="16"/>
+      <name val="Helvetica Neue"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="16"/>
+      <name val="Helvetica Neue"/>
+    </font>
+    <font>
       <b val="1"/>
       <sz val="1"/>
       <color indexed="8"/>
@@ -261,28 +322,28 @@
     </font>
     <font>
       <sz val="19"/>
-      <color indexed="17"/>
+      <color indexed="18"/>
       <name val="Helvetica Neue"/>
     </font>
     <font>
       <b val="1"/>
       <sz val="12"/>
-      <color indexed="17"/>
+      <color indexed="18"/>
       <name val="Helvetica Neue"/>
     </font>
     <font>
       <sz val="12"/>
-      <color indexed="17"/>
+      <color indexed="18"/>
       <name val="Helvetica Neue"/>
     </font>
     <font>
       <sz val="15"/>
-      <color indexed="17"/>
+      <color indexed="18"/>
       <name val="Helvetica Neue"/>
     </font>
     <font>
       <sz val="17"/>
-      <color indexed="17"/>
+      <color indexed="18"/>
       <name val="Helvetica Neue"/>
     </font>
   </fonts>
@@ -319,7 +380,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="16"/>
+        <fgColor indexed="17"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
@@ -443,7 +504,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="78">
+  <cellXfs count="89">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -534,22 +595,55 @@
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="62" fontId="8" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="6" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -570,7 +664,7 @@
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="5" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="10" fillId="5" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -582,7 +676,7 @@
     <xf numFmtId="62" fontId="0" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -618,64 +712,64 @@
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="11" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="62" fontId="10" fillId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="62" fontId="12" fillId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="5" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="59" fontId="11" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="59" fontId="11" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="59" fontId="13" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="59" fontId="13" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="5" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="59" fontId="11" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="59" fontId="11" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="59" fontId="13" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="59" fontId="13" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="11" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="11" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="60" fontId="11" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="60" fontId="11" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="11" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="11" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="61" fontId="11" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="61" fontId="11" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="13" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="13" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="13" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="60" fontId="13" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="60" fontId="13" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="13" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="13" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="61" fontId="13" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="61" fontId="13" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -702,6 +796,7 @@
       <rgbColor rgb="ffa5a5a5"/>
       <rgbColor rgb="ff3f3f3f"/>
       <rgbColor rgb="ffdbdbdb"/>
+      <rgbColor rgb="ff5e5e5e"/>
       <rgbColor rgb="ffd5d5d5"/>
       <rgbColor rgb="ff919191"/>
       <rgbColor rgb="ffb8b8b8"/>
@@ -863,70 +958,70 @@
               <c:numCache>
                 <c:ptCount val="22"/>
                 <c:pt idx="0">
-                  <c:v>0.000000</c:v>
+                  <c:v>-5.134021</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10.268042</c:v>
+                  <c:v>5.134021</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>20.536084</c:v>
+                  <c:v>15.402063</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>25.670105</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>30.804126</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>35.938147</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>41.072168</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>46.206189</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>51.340209</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>56.474230</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>61.608251</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>66.742272</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>71.876293</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="13">
                   <c:v>77.010314</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="14">
                   <c:v>82.144335</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="15">
                   <c:v>87.278356</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="16">
                   <c:v>92.412377</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="17">
                   <c:v>97.546398</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="18">
                   <c:v>102.680419</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="19">
                   <c:v>107.814440</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="20">
                   <c:v>112.948461</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="21">
                   <c:v>118.082482</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>123.216503</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1023,8 +1118,8 @@
         <c:crossAx val="2094734552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
-        <c:majorUnit val="20"/>
-        <c:minorUnit val="10"/>
+        <c:majorUnit val="19.5918"/>
+        <c:minorUnit val="9.79592"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -2216,51 +2311,78 @@
       </c>
     </row>
     <row r="11">
-      <c r="B11" t="s" s="3">
+      <c r="B11" s="4"/>
+      <c r="C11" t="s" s="4">
         <v>25</v>
       </c>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
+      <c r="D11" t="s" s="5">
+        <v>26</v>
+      </c>
     </row>
     <row r="12">
       <c r="B12" s="4"/>
       <c r="C12" t="s" s="4">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="D12" t="s" s="5">
-        <v>26</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13">
-      <c r="B13" t="s" s="3">
-        <v>37</v>
-      </c>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
+      <c r="B13" s="4"/>
+      <c r="C13" t="s" s="4">
+        <v>39</v>
+      </c>
+      <c r="D13" t="s" s="5">
+        <v>40</v>
+      </c>
     </row>
     <row r="14">
-      <c r="B14" s="4"/>
-      <c r="C14" t="s" s="4">
-        <v>37</v>
-      </c>
-      <c r="D14" t="s" s="5">
-        <v>38</v>
-      </c>
+      <c r="B14" t="s" s="3">
+        <v>41</v>
+      </c>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
     </row>
     <row r="15">
-      <c r="B15" t="s" s="3">
-        <v>57</v>
-      </c>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
+      <c r="B15" s="4"/>
+      <c r="C15" t="s" s="4">
+        <v>41</v>
+      </c>
+      <c r="D15" t="s" s="5">
+        <v>42</v>
+      </c>
     </row>
     <row r="16">
-      <c r="B16" s="4"/>
-      <c r="C16" t="s" s="4">
-        <v>58</v>
-      </c>
-      <c r="D16" t="s" s="5">
-        <v>59</v>
+      <c r="B16" t="s" s="3">
+        <v>53</v>
+      </c>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+    </row>
+    <row r="17">
+      <c r="B17" s="4"/>
+      <c r="C17" t="s" s="4">
+        <v>53</v>
+      </c>
+      <c r="D17" t="s" s="5">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="B18" t="s" s="3">
+        <v>73</v>
+      </c>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+    </row>
+    <row r="19">
+      <c r="B19" s="4"/>
+      <c r="C19" t="s" s="4">
+        <v>74</v>
+      </c>
+      <c r="D19" t="s" s="5">
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -2269,9 +2391,12 @@
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D10" location="'MMTLP_DIVI_CALC - MMTLP_DIVI_CA'!R2C1" tooltip="" display="MMTLP_DIVI_CALC - MMTLP_DIVI_CA"/>
-    <hyperlink ref="D12" location="'What Happens if MMTLP Divi Get '!R2C1" tooltip="" display="What Happens if MMTLP Divi Get "/>
-    <hyperlink ref="D14" location="'reinvesting_1000_shares_mmtlp -'!R2C1" tooltip="" display="reinvesting_1000_shares_mmtlp -"/>
-    <hyperlink ref="D16" location="'divi chart from 30 to 150 oil p'!R2C2" tooltip="" display="divi chart from 30 to 150 oil p"/>
+    <hyperlink ref="D11" location="'MMTLP_DIVI_CALC - Table 1'!R2C1" tooltip="" display="MMTLP_DIVI_CALC - Table 1"/>
+    <hyperlink ref="D12" location="'MMTLP_DIVI_CALC - Possible MOAS'!R2C1" tooltip="" display="MMTLP_DIVI_CALC - Possible MOAS"/>
+    <hyperlink ref="D13" location="'MMTLP_DIVI_CALC - Table 2'!R2C1" tooltip="" display="MMTLP_DIVI_CALC - Table 2"/>
+    <hyperlink ref="D15" location="'What Happens if MMTLP Divi Get '!R2C1" tooltip="" display="What Happens if MMTLP Divi Get "/>
+    <hyperlink ref="D17" location="'reinvesting_1000_shares_mmtlp -'!R2C1" tooltip="" display="reinvesting_1000_shares_mmtlp -"/>
+    <hyperlink ref="D19" location="'divi chart from 30 to 150 oil p'!R2C2" tooltip="" display="divi chart from 30 to 150 oil p"/>
   </hyperlinks>
 </worksheet>
 </file>
@@ -2329,11 +2454,11 @@
         <v>9</v>
       </c>
       <c r="B4" s="15">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="C4" s="16"/>
       <c r="D4" s="16">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="E4" s="16"/>
     </row>
@@ -2343,12 +2468,12 @@
       </c>
       <c r="B5" s="15">
         <f>B3-B4</f>
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C5" s="16"/>
       <c r="D5" s="16">
         <f>D3-D4</f>
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="E5" s="16"/>
     </row>
@@ -2378,12 +2503,12 @@
       </c>
       <c r="B8" s="15">
         <f>B7*B5</f>
-        <v>8.4</v>
+        <v>7.8</v>
       </c>
       <c r="C8" s="19"/>
       <c r="D8" s="16">
         <f>D7*D5</f>
-        <v>8.4</v>
+        <v>7.8</v>
       </c>
       <c r="E8" s="19"/>
     </row>
@@ -2413,12 +2538,12 @@
       </c>
       <c r="B11" s="22">
         <f>B8*B10</f>
-        <v>4.116</v>
+        <v>3.822</v>
       </c>
       <c r="C11" s="19"/>
       <c r="D11" s="23">
         <f>D8*D10</f>
-        <v>4.116</v>
+        <v>3.822</v>
       </c>
       <c r="E11" s="19"/>
     </row>
@@ -2457,12 +2582,12 @@
       </c>
       <c r="B15" s="24">
         <f>B14*B$11</f>
-        <v>13171200000</v>
+        <v>12230400000</v>
       </c>
       <c r="C15" s="25"/>
       <c r="D15" s="25">
         <f>D14*D$11</f>
-        <v>13171200000</v>
+        <v>12230400000</v>
       </c>
       <c r="E15" s="25"/>
     </row>
@@ -2498,12 +2623,12 @@
       </c>
       <c r="B18" s="24">
         <f>B15*(1-(B16+B17))</f>
-        <v>11854080000</v>
+        <v>11007360000</v>
       </c>
       <c r="C18" s="19"/>
       <c r="D18" s="25">
         <f>D15*(1-(D16+D17))</f>
-        <v>9088128000</v>
+        <v>8438976000</v>
       </c>
       <c r="E18" s="19"/>
     </row>
@@ -2526,12 +2651,12 @@
       </c>
       <c r="B20" s="15">
         <f>B18/B19</f>
-        <v>71.87629323323949</v>
+        <v>66.7422722880081</v>
       </c>
       <c r="C20" s="16"/>
       <c r="D20" s="16">
         <f>D18/D19</f>
-        <v>55.1051581454836</v>
+        <v>51.1690754208062</v>
       </c>
       <c r="E20" s="16"/>
     </row>
@@ -2570,12 +2695,12 @@
       </c>
       <c r="B24" s="24">
         <f>B23*B$11</f>
-        <v>8643600000</v>
+        <v>8026200000</v>
       </c>
       <c r="C24" s="25"/>
       <c r="D24" s="25">
         <f>D23*D$11</f>
-        <v>8643600000</v>
+        <v>8026200000</v>
       </c>
       <c r="E24" s="25"/>
     </row>
@@ -2611,12 +2736,12 @@
       </c>
       <c r="B27" s="24">
         <f>B24*(1-(B25+B26))</f>
-        <v>5964084000</v>
+        <v>5538078000</v>
       </c>
       <c r="C27" s="19"/>
       <c r="D27" s="25">
         <f>D24*(1-(D25+D26))</f>
-        <v>5964084000</v>
+        <v>5538078000</v>
       </c>
       <c r="E27" s="19"/>
     </row>
@@ -2639,12 +2764,12 @@
       </c>
       <c r="B29" s="15">
         <f>B27/B28</f>
-        <v>34.08048</v>
+        <v>31.64616</v>
       </c>
       <c r="C29" s="16"/>
       <c r="D29" s="16">
         <f>D27/D28</f>
-        <v>34.08048</v>
+        <v>31.64616</v>
       </c>
       <c r="E29" s="16"/>
     </row>
@@ -2662,6 +2787,585 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A2:E8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col min="1" max="5" width="16.3516" style="29" customWidth="1"/>
+    <col min="6" max="16384" width="16.3516" style="29" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="27.65" customHeight="1">
+      <c r="A1" t="s" s="7">
+        <v>25</v>
+      </c>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+    </row>
+    <row r="2" ht="20.05" customHeight="1">
+      <c r="A2" s="30">
+        <v>6000</v>
+      </c>
+      <c r="B2" t="s" s="31">
+        <v>27</v>
+      </c>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+    </row>
+    <row r="3" ht="20.05" customHeight="1">
+      <c r="A3" s="32"/>
+      <c r="B3" s="30">
+        <v>11.4</v>
+      </c>
+      <c r="C3" t="s" s="31">
+        <v>28</v>
+      </c>
+      <c r="D3" s="30">
+        <v>7.2</v>
+      </c>
+      <c r="E3" s="32"/>
+    </row>
+    <row r="4" ht="20.05" customHeight="1">
+      <c r="A4" s="32"/>
+      <c r="B4" s="33">
+        <v>11400</v>
+      </c>
+      <c r="C4" t="s" s="31">
+        <v>29</v>
+      </c>
+      <c r="D4" s="33">
+        <f>D3*1000</f>
+        <v>7200</v>
+      </c>
+      <c r="E4" s="32"/>
+    </row>
+    <row r="5" ht="20.05" customHeight="1">
+      <c r="A5" s="32"/>
+      <c r="B5" s="33">
+        <f>B4*1000</f>
+        <v>11400000</v>
+      </c>
+      <c r="C5" t="s" s="31">
+        <v>30</v>
+      </c>
+      <c r="D5" s="33">
+        <f>D4*1000</f>
+        <v>7200000</v>
+      </c>
+      <c r="E5" s="32"/>
+    </row>
+    <row r="6" ht="20.05" customHeight="1">
+      <c r="A6" s="32"/>
+      <c r="B6" s="33">
+        <f>1000*B5</f>
+        <v>11400000000</v>
+      </c>
+      <c r="C6" s="32"/>
+      <c r="D6" s="33">
+        <f>1000*D5</f>
+        <v>7200000000</v>
+      </c>
+      <c r="E6" s="32"/>
+    </row>
+    <row r="7" ht="20.05" customHeight="1">
+      <c r="A7" s="32"/>
+      <c r="B7" s="32"/>
+      <c r="C7" s="32"/>
+      <c r="D7" s="32"/>
+      <c r="E7" s="32"/>
+    </row>
+    <row r="8" ht="20.05" customHeight="1">
+      <c r="A8" s="32"/>
+      <c r="B8" s="32"/>
+      <c r="C8" s="32"/>
+      <c r="D8" s="32"/>
+      <c r="E8" s="32"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:E1"/>
+  </mergeCells>
+  <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>
+  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="72" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <headerFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A2:F16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col min="1" max="1" width="7.29688" style="34" customWidth="1"/>
+    <col min="2" max="2" width="12.5703" style="34" customWidth="1"/>
+    <col min="3" max="3" width="8.64062" style="34" customWidth="1"/>
+    <col min="4" max="4" width="16.3516" style="34" customWidth="1"/>
+    <col min="5" max="5" width="7.39062" style="34" customWidth="1"/>
+    <col min="6" max="6" width="16.3516" style="34" customWidth="1"/>
+    <col min="7" max="16384" width="16.3516" style="34" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="27.65" customHeight="1">
+      <c r="A1" t="s" s="35">
+        <v>31</v>
+      </c>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+    </row>
+    <row r="2" ht="20.05" customHeight="1">
+      <c r="A2" t="s" s="36">
+        <v>33</v>
+      </c>
+      <c r="B2" s="37"/>
+      <c r="C2" s="38">
+        <v>1.5</v>
+      </c>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+    </row>
+    <row r="3" ht="20.05" customHeight="1">
+      <c r="A3" s="39"/>
+      <c r="B3" s="39"/>
+      <c r="C3" s="39"/>
+      <c r="D3" s="39"/>
+      <c r="E3" s="39"/>
+      <c r="F3" s="39"/>
+    </row>
+    <row r="4" ht="32.05" customHeight="1">
+      <c r="A4" t="s" s="40">
+        <v>34</v>
+      </c>
+      <c r="B4" t="s" s="40">
+        <v>35</v>
+      </c>
+      <c r="C4" t="s" s="40">
+        <v>36</v>
+      </c>
+      <c r="D4" t="s" s="40">
+        <v>37</v>
+      </c>
+      <c r="E4" s="39"/>
+      <c r="F4" t="s" s="40">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" ht="20.05" customHeight="1">
+      <c r="A5" s="38">
+        <v>1</v>
+      </c>
+      <c r="B5" s="41">
+        <v>100000</v>
+      </c>
+      <c r="C5" s="38">
+        <v>15</v>
+      </c>
+      <c r="D5" s="41">
+        <f>B5*C5</f>
+        <v>1500000</v>
+      </c>
+      <c r="E5" s="37"/>
+      <c r="F5" s="41">
+        <f>SUM(D$5:D5)</f>
+        <v>1500000</v>
+      </c>
+    </row>
+    <row r="6" ht="20.05" customHeight="1">
+      <c r="A6" s="38">
+        <v>2</v>
+      </c>
+      <c r="B6" s="41">
+        <f>FLOOR(B5*C$2,1)</f>
+        <v>150000</v>
+      </c>
+      <c r="C6" s="38">
+        <v>15</v>
+      </c>
+      <c r="D6" s="41">
+        <f>B6*C6</f>
+        <v>2250000</v>
+      </c>
+      <c r="E6" s="37"/>
+      <c r="F6" s="41">
+        <f>SUM(D$5:D6)</f>
+        <v>3750000</v>
+      </c>
+    </row>
+    <row r="7" ht="20.05" customHeight="1">
+      <c r="A7" s="38">
+        <v>3</v>
+      </c>
+      <c r="B7" s="41">
+        <f>FLOOR(B6*C$2,1)</f>
+        <v>225000</v>
+      </c>
+      <c r="C7" s="38">
+        <v>15</v>
+      </c>
+      <c r="D7" s="41">
+        <f>B7*C7</f>
+        <v>3375000</v>
+      </c>
+      <c r="E7" s="37"/>
+      <c r="F7" s="41">
+        <f>SUM(D$5:D7)</f>
+        <v>7125000</v>
+      </c>
+    </row>
+    <row r="8" ht="20.05" customHeight="1">
+      <c r="A8" s="38">
+        <v>4</v>
+      </c>
+      <c r="B8" s="41">
+        <f>FLOOR(B7*C$2,1)</f>
+        <v>337500</v>
+      </c>
+      <c r="C8" s="38">
+        <v>15</v>
+      </c>
+      <c r="D8" s="41">
+        <f>B8*C8</f>
+        <v>5062500</v>
+      </c>
+      <c r="E8" s="37"/>
+      <c r="F8" s="41">
+        <f>SUM(D$5:D8)</f>
+        <v>12187500</v>
+      </c>
+    </row>
+    <row r="9" ht="20.05" customHeight="1">
+      <c r="A9" s="38">
+        <v>5</v>
+      </c>
+      <c r="B9" s="41">
+        <f>FLOOR(B8*C$2,1)</f>
+        <v>506250</v>
+      </c>
+      <c r="C9" s="38">
+        <v>15</v>
+      </c>
+      <c r="D9" s="41">
+        <f>B9*C9</f>
+        <v>7593750</v>
+      </c>
+      <c r="E9" s="37"/>
+      <c r="F9" s="41">
+        <f>SUM(D$5:D9)</f>
+        <v>19781250</v>
+      </c>
+    </row>
+    <row r="10" ht="20.05" customHeight="1">
+      <c r="A10" s="38">
+        <v>6</v>
+      </c>
+      <c r="B10" s="41">
+        <f>FLOOR(B9*C$2,1)</f>
+        <v>759375</v>
+      </c>
+      <c r="C10" s="38">
+        <v>15</v>
+      </c>
+      <c r="D10" s="41">
+        <f>B10*C10</f>
+        <v>11390625</v>
+      </c>
+      <c r="E10" s="37"/>
+      <c r="F10" s="41">
+        <f>SUM(D$5:D10)</f>
+        <v>31171875</v>
+      </c>
+    </row>
+    <row r="11" ht="20.05" customHeight="1">
+      <c r="A11" s="38">
+        <v>7</v>
+      </c>
+      <c r="B11" s="41">
+        <f>FLOOR(B10*C$2,1)</f>
+        <v>1139062</v>
+      </c>
+      <c r="C11" s="38">
+        <v>15</v>
+      </c>
+      <c r="D11" s="41">
+        <f>B11*C11</f>
+        <v>17085930</v>
+      </c>
+      <c r="E11" s="37"/>
+      <c r="F11" s="41">
+        <f>SUM(D$5:D11)</f>
+        <v>48257805</v>
+      </c>
+    </row>
+    <row r="12" ht="20.05" customHeight="1">
+      <c r="A12" s="38">
+        <v>8</v>
+      </c>
+      <c r="B12" s="41">
+        <f>FLOOR(B11*C$2,1)</f>
+        <v>1708593</v>
+      </c>
+      <c r="C12" s="38">
+        <v>15</v>
+      </c>
+      <c r="D12" s="41">
+        <f>B12*C12</f>
+        <v>25628895</v>
+      </c>
+      <c r="E12" s="37"/>
+      <c r="F12" s="41">
+        <f>SUM(D$5:D12)</f>
+        <v>73886700</v>
+      </c>
+    </row>
+    <row r="13" ht="20.05" customHeight="1">
+      <c r="A13" s="38">
+        <v>9</v>
+      </c>
+      <c r="B13" s="41">
+        <f>FLOOR(B12*C$2,1)</f>
+        <v>2562889</v>
+      </c>
+      <c r="C13" s="38">
+        <v>15</v>
+      </c>
+      <c r="D13" s="41">
+        <f>B13*C13</f>
+        <v>38443335</v>
+      </c>
+      <c r="E13" s="37"/>
+      <c r="F13" s="41">
+        <f>SUM(D$5:D13)</f>
+        <v>112330035</v>
+      </c>
+    </row>
+    <row r="14" ht="20.05" customHeight="1">
+      <c r="A14" s="38">
+        <v>10</v>
+      </c>
+      <c r="B14" s="41">
+        <f>FLOOR(B13*C$2,1)</f>
+        <v>3844333</v>
+      </c>
+      <c r="C14" s="38">
+        <v>15</v>
+      </c>
+      <c r="D14" s="41">
+        <f>B14*C14</f>
+        <v>57664995</v>
+      </c>
+      <c r="E14" s="37"/>
+      <c r="F14" s="41">
+        <f>SUM(D$5:D14)</f>
+        <v>169995030</v>
+      </c>
+    </row>
+    <row r="15" ht="20.05" customHeight="1">
+      <c r="A15" s="37"/>
+      <c r="B15" s="37"/>
+      <c r="C15" s="37"/>
+      <c r="D15" s="37"/>
+      <c r="E15" s="37"/>
+      <c r="F15" s="37"/>
+    </row>
+    <row r="16" ht="20.05" customHeight="1">
+      <c r="A16" s="37"/>
+      <c r="B16" s="37"/>
+      <c r="C16" s="38">
+        <f>SUM(C5:C14)</f>
+        <v>150</v>
+      </c>
+      <c r="D16" s="41">
+        <f>SUM(D5:D14)</f>
+        <v>169995030</v>
+      </c>
+      <c r="E16" s="37"/>
+      <c r="F16" s="37"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:F1"/>
+  </mergeCells>
+  <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>
+  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="72" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <headerFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A2:E15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col min="1" max="5" width="16.3516" style="42" customWidth="1"/>
+    <col min="6" max="16384" width="16.3516" style="42" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="27.65" customHeight="1">
+      <c r="A1" t="s" s="7">
+        <v>39</v>
+      </c>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+    </row>
+    <row r="2" ht="20.05" customHeight="1">
+      <c r="A2" s="32"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+    </row>
+    <row r="3" ht="20.05" customHeight="1">
+      <c r="A3" s="30">
+        <v>200</v>
+      </c>
+      <c r="B3" s="33">
+        <v>20000</v>
+      </c>
+      <c r="C3" s="33">
+        <f>A3*B3</f>
+        <v>4000000</v>
+      </c>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+    </row>
+    <row r="4" ht="20.05" customHeight="1">
+      <c r="A4" s="32"/>
+      <c r="B4" s="32"/>
+      <c r="C4" s="32"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="32"/>
+    </row>
+    <row r="5" ht="20.05" customHeight="1">
+      <c r="A5" s="32"/>
+      <c r="B5" s="32"/>
+      <c r="C5" s="32"/>
+      <c r="D5" s="32"/>
+      <c r="E5" s="32"/>
+    </row>
+    <row r="6" ht="20.05" customHeight="1">
+      <c r="A6" s="30">
+        <v>70</v>
+      </c>
+      <c r="B6" s="32"/>
+      <c r="C6" s="32"/>
+      <c r="D6" s="32"/>
+      <c r="E6" s="32"/>
+    </row>
+    <row r="7" ht="20.05" customHeight="1">
+      <c r="A7" s="30">
+        <v>75</v>
+      </c>
+      <c r="B7" s="32"/>
+      <c r="C7" s="32"/>
+      <c r="D7" s="32"/>
+      <c r="E7" s="32"/>
+    </row>
+    <row r="8" ht="20.05" customHeight="1">
+      <c r="A8" s="30">
+        <v>33</v>
+      </c>
+      <c r="B8" s="32"/>
+      <c r="C8" s="32"/>
+      <c r="D8" s="32"/>
+      <c r="E8" s="32"/>
+    </row>
+    <row r="9" ht="20.05" customHeight="1">
+      <c r="A9" s="30">
+        <v>28</v>
+      </c>
+      <c r="B9" s="32"/>
+      <c r="C9" s="32"/>
+      <c r="D9" s="32"/>
+      <c r="E9" s="32"/>
+    </row>
+    <row r="10" ht="20.05" customHeight="1">
+      <c r="A10" s="30">
+        <f>SUM(A6:A9)</f>
+        <v>206</v>
+      </c>
+      <c r="B10" s="32"/>
+      <c r="C10" s="32"/>
+      <c r="D10" s="32"/>
+      <c r="E10" s="32"/>
+    </row>
+    <row r="11" ht="20.05" customHeight="1">
+      <c r="A11" s="32"/>
+      <c r="B11" s="32"/>
+      <c r="C11" s="32"/>
+      <c r="D11" s="32"/>
+      <c r="E11" s="32"/>
+    </row>
+    <row r="12" ht="20.05" customHeight="1">
+      <c r="A12" s="30">
+        <v>25</v>
+      </c>
+      <c r="B12" s="32"/>
+      <c r="C12" s="32"/>
+      <c r="D12" s="32"/>
+      <c r="E12" s="32"/>
+    </row>
+    <row r="13" ht="20.05" customHeight="1">
+      <c r="A13" s="30">
+        <v>75</v>
+      </c>
+      <c r="B13" s="32"/>
+      <c r="C13" s="32"/>
+      <c r="D13" s="32"/>
+      <c r="E13" s="32"/>
+    </row>
+    <row r="14" ht="20.05" customHeight="1">
+      <c r="A14" s="30">
+        <v>50</v>
+      </c>
+      <c r="B14" s="32"/>
+      <c r="C14" s="32"/>
+      <c r="D14" s="32"/>
+      <c r="E14" s="32"/>
+    </row>
+    <row r="15" ht="20.05" customHeight="1">
+      <c r="A15" s="30">
+        <f>SUM(A12:A14)</f>
+        <v>150</v>
+      </c>
+      <c r="B15" s="32"/>
+      <c r="C15" s="32"/>
+      <c r="D15" s="32"/>
+      <c r="E15" s="32"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:E1"/>
+  </mergeCells>
+  <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>
+  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="72" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <headerFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A2:G30"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
@@ -2670,17 +3374,17 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="21.8203" style="29" customWidth="1"/>
-    <col min="2" max="2" width="14.6094" style="29" customWidth="1"/>
-    <col min="3" max="3" width="16.3516" style="29" customWidth="1"/>
-    <col min="4" max="4" width="28.6562" style="29" customWidth="1"/>
-    <col min="5" max="7" width="13.7891" style="29" customWidth="1"/>
-    <col min="8" max="16384" width="16.3516" style="29" customWidth="1"/>
+    <col min="1" max="1" width="21.8203" style="43" customWidth="1"/>
+    <col min="2" max="2" width="14.6094" style="43" customWidth="1"/>
+    <col min="3" max="3" width="16.3516" style="43" customWidth="1"/>
+    <col min="4" max="4" width="28.6562" style="43" customWidth="1"/>
+    <col min="5" max="7" width="13.7891" style="43" customWidth="1"/>
+    <col min="8" max="16384" width="16.3516" style="43" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="27.65" customHeight="1">
       <c r="A1" t="s" s="7">
-        <v>25</v>
+        <v>41</v>
       </c>
       <c r="B1" s="7"/>
       <c r="C1" s="7"/>
@@ -2690,39 +3394,39 @@
       <c r="G1" s="7"/>
     </row>
     <row r="2" ht="20.25" customHeight="1">
-      <c r="A2" s="30"/>
-      <c r="B2" s="30"/>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="31"/>
-      <c r="G2" s="31"/>
+      <c r="A2" s="44"/>
+      <c r="B2" s="44"/>
+      <c r="C2" s="45"/>
+      <c r="D2" s="45"/>
+      <c r="E2" s="45"/>
+      <c r="F2" s="45"/>
+      <c r="G2" s="45"/>
     </row>
     <row r="3" ht="20.25" customHeight="1">
       <c r="A3" t="s" s="11">
         <v>8</v>
       </c>
       <c r="B3" s="12">
-        <v>75</v>
-      </c>
-      <c r="C3" s="32"/>
-      <c r="D3" s="32"/>
-      <c r="E3" s="32"/>
-      <c r="F3" s="32"/>
-      <c r="G3" s="32"/>
+        <v>85</v>
+      </c>
+      <c r="C3" s="46"/>
+      <c r="D3" s="46"/>
+      <c r="E3" s="46"/>
+      <c r="F3" s="46"/>
+      <c r="G3" s="46"/>
     </row>
     <row r="4" ht="20.05" customHeight="1">
       <c r="A4" t="s" s="14">
         <v>9</v>
       </c>
       <c r="B4" s="15">
-        <v>25</v>
-      </c>
-      <c r="C4" s="33"/>
-      <c r="D4" s="33"/>
-      <c r="E4" s="33"/>
-      <c r="F4" s="33"/>
-      <c r="G4" s="33"/>
+        <v>35</v>
+      </c>
+      <c r="C4" s="32"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="32"/>
+      <c r="F4" s="32"/>
+      <c r="G4" s="32"/>
     </row>
     <row r="5" ht="20.05" customHeight="1">
       <c r="A5" t="s" s="14">
@@ -2732,20 +3436,20 @@
         <f>B3-B4</f>
         <v>50</v>
       </c>
-      <c r="C5" s="33"/>
-      <c r="D5" s="33"/>
-      <c r="E5" s="33"/>
-      <c r="F5" s="33"/>
-      <c r="G5" s="33"/>
+      <c r="C5" s="32"/>
+      <c r="D5" s="32"/>
+      <c r="E5" s="32"/>
+      <c r="F5" s="32"/>
+      <c r="G5" s="32"/>
     </row>
     <row r="6" ht="20.05" customHeight="1">
       <c r="A6" s="17"/>
       <c r="B6" s="18"/>
-      <c r="C6" s="33"/>
-      <c r="D6" s="33"/>
-      <c r="E6" s="33"/>
-      <c r="F6" s="33"/>
-      <c r="G6" s="33"/>
+      <c r="C6" s="32"/>
+      <c r="D6" s="32"/>
+      <c r="E6" s="32"/>
+      <c r="F6" s="32"/>
+      <c r="G6" s="32"/>
     </row>
     <row r="7" ht="20.05" customHeight="1">
       <c r="A7" t="s" s="14">
@@ -2754,11 +3458,11 @@
       <c r="B7" s="20">
         <v>0.12</v>
       </c>
-      <c r="C7" s="33"/>
-      <c r="D7" s="33"/>
-      <c r="E7" s="33"/>
-      <c r="F7" s="33"/>
-      <c r="G7" s="33"/>
+      <c r="C7" s="32"/>
+      <c r="D7" s="32"/>
+      <c r="E7" s="32"/>
+      <c r="F7" s="32"/>
+      <c r="G7" s="32"/>
     </row>
     <row r="8" ht="20.05" customHeight="1">
       <c r="A8" t="s" s="14">
@@ -2768,20 +3472,20 @@
         <f>B7*B5</f>
         <v>6</v>
       </c>
-      <c r="C8" s="33"/>
-      <c r="D8" s="33"/>
-      <c r="E8" s="33"/>
-      <c r="F8" s="33"/>
-      <c r="G8" s="33"/>
+      <c r="C8" s="32"/>
+      <c r="D8" s="32"/>
+      <c r="E8" s="32"/>
+      <c r="F8" s="32"/>
+      <c r="G8" s="32"/>
     </row>
     <row r="9" ht="20.05" customHeight="1">
       <c r="A9" s="17"/>
       <c r="B9" s="18"/>
-      <c r="C9" s="33"/>
-      <c r="D9" s="33"/>
-      <c r="E9" s="33"/>
-      <c r="F9" s="33"/>
-      <c r="G9" s="33"/>
+      <c r="C9" s="32"/>
+      <c r="D9" s="32"/>
+      <c r="E9" s="32"/>
+      <c r="F9" s="32"/>
+      <c r="G9" s="32"/>
     </row>
     <row r="10" ht="20.05" customHeight="1">
       <c r="A10" t="s" s="14">
@@ -2790,11 +3494,11 @@
       <c r="B10" s="20">
         <v>0.49</v>
       </c>
-      <c r="C10" s="33"/>
-      <c r="D10" s="33"/>
-      <c r="E10" s="33"/>
-      <c r="F10" s="33"/>
-      <c r="G10" s="33"/>
+      <c r="C10" s="32"/>
+      <c r="D10" s="32"/>
+      <c r="E10" s="32"/>
+      <c r="F10" s="32"/>
+      <c r="G10" s="32"/>
     </row>
     <row r="11" ht="20.05" customHeight="1">
       <c r="A11" t="s" s="14">
@@ -2804,36 +3508,36 @@
         <f>B8*B10</f>
         <v>2.94</v>
       </c>
-      <c r="C11" s="33"/>
-      <c r="D11" s="33"/>
-      <c r="E11" s="33"/>
-      <c r="F11" s="33"/>
-      <c r="G11" s="33"/>
+      <c r="C11" s="32"/>
+      <c r="D11" s="32"/>
+      <c r="E11" s="32"/>
+      <c r="F11" s="32"/>
+      <c r="G11" s="32"/>
     </row>
     <row r="12" ht="20.05" customHeight="1">
       <c r="A12" s="17"/>
       <c r="B12" s="18"/>
-      <c r="C12" s="33"/>
-      <c r="D12" s="33"/>
-      <c r="E12" s="34">
+      <c r="C12" s="32"/>
+      <c r="D12" s="32"/>
+      <c r="E12" s="30">
         <v>0.25</v>
       </c>
-      <c r="F12" s="33"/>
-      <c r="G12" s="33"/>
+      <c r="F12" s="32"/>
+      <c r="G12" s="32"/>
     </row>
     <row r="13" ht="20.05" customHeight="1">
       <c r="A13" t="s" s="14">
         <v>15</v>
       </c>
       <c r="B13" s="18"/>
-      <c r="C13" s="33"/>
-      <c r="D13" s="33"/>
-      <c r="E13" s="35">
+      <c r="C13" s="32"/>
+      <c r="D13" s="32"/>
+      <c r="E13" s="33">
         <f>E12*E22</f>
-        <v>177947368.421053</v>
-      </c>
-      <c r="F13" s="33"/>
-      <c r="G13" s="33"/>
+        <v>423360000</v>
+      </c>
+      <c r="F13" s="32"/>
+      <c r="G13" s="32"/>
     </row>
     <row r="14" ht="20.05" customHeight="1">
       <c r="A14" t="s" s="14">
@@ -2842,11 +3546,11 @@
       <c r="B14" s="24">
         <v>3200000000</v>
       </c>
-      <c r="C14" s="33"/>
-      <c r="D14" s="33"/>
-      <c r="E14" s="33"/>
-      <c r="F14" s="33"/>
-      <c r="G14" s="33"/>
+      <c r="C14" s="32"/>
+      <c r="D14" s="32"/>
+      <c r="E14" s="32"/>
+      <c r="F14" s="32"/>
+      <c r="G14" s="32"/>
     </row>
     <row r="15" ht="20.05" customHeight="1">
       <c r="A15" t="s" s="14">
@@ -2856,24 +3560,24 @@
         <f>B14*B$11</f>
         <v>9408000000</v>
       </c>
-      <c r="C15" s="33"/>
-      <c r="D15" s="33"/>
-      <c r="E15" s="33"/>
-      <c r="F15" s="33"/>
-      <c r="G15" s="33"/>
+      <c r="C15" s="32"/>
+      <c r="D15" s="32"/>
+      <c r="E15" s="32"/>
+      <c r="F15" s="32"/>
+      <c r="G15" s="32"/>
     </row>
     <row r="16" ht="20.05" customHeight="1">
       <c r="A16" t="s" s="14">
         <v>18</v>
       </c>
       <c r="B16" s="20">
-        <v>0.21</v>
-      </c>
-      <c r="C16" s="33"/>
-      <c r="D16" s="33"/>
-      <c r="E16" s="33"/>
-      <c r="F16" s="33"/>
-      <c r="G16" s="33"/>
+        <v>0</v>
+      </c>
+      <c r="C16" s="32"/>
+      <c r="D16" s="32"/>
+      <c r="E16" s="32"/>
+      <c r="F16" s="32"/>
+      <c r="G16" s="32"/>
     </row>
     <row r="17" ht="20.05" customHeight="1">
       <c r="A17" t="s" s="14">
@@ -2882,13 +3586,13 @@
       <c r="B17" s="27">
         <v>0.1</v>
       </c>
-      <c r="C17" s="33"/>
-      <c r="D17" t="s" s="36">
-        <v>27</v>
-      </c>
-      <c r="E17" s="37"/>
-      <c r="F17" s="37"/>
-      <c r="G17" s="37"/>
+      <c r="C17" s="32"/>
+      <c r="D17" t="s" s="47">
+        <v>43</v>
+      </c>
+      <c r="E17" s="48"/>
+      <c r="F17" s="48"/>
+      <c r="G17" s="48"/>
     </row>
     <row r="18" ht="20.05" customHeight="1">
       <c r="A18" t="s" s="14">
@@ -2896,17 +3600,17 @@
       </c>
       <c r="B18" s="24">
         <f>B15*(1-(B16+B17))</f>
-        <v>6491520000</v>
-      </c>
-      <c r="C18" s="33"/>
-      <c r="D18" t="s" s="38">
-        <v>28</v>
-      </c>
-      <c r="E18" s="39">
+        <v>8467200000</v>
+      </c>
+      <c r="C18" s="32"/>
+      <c r="D18" t="s" s="49">
+        <v>44</v>
+      </c>
+      <c r="E18" s="50">
         <v>0.25</v>
       </c>
-      <c r="F18" s="33"/>
-      <c r="G18" s="39">
+      <c r="F18" s="32"/>
+      <c r="G18" s="50">
         <v>0.07000000000000001</v>
       </c>
     </row>
@@ -2917,18 +3621,18 @@
       <c r="B19" s="24">
         <v>164923363</v>
       </c>
-      <c r="C19" s="33"/>
-      <c r="D19" t="s" s="38">
-        <v>29</v>
-      </c>
-      <c r="E19" s="35">
+      <c r="C19" s="32"/>
+      <c r="D19" t="s" s="49">
+        <v>45</v>
+      </c>
+      <c r="E19" s="33">
         <f>$B18*E18</f>
-        <v>1622880000</v>
-      </c>
-      <c r="F19" s="33"/>
-      <c r="G19" s="35">
+        <v>2116800000</v>
+      </c>
+      <c r="F19" s="32"/>
+      <c r="G19" s="33">
         <f>$B18*G18</f>
-        <v>454406400</v>
+        <v>592704000</v>
       </c>
     </row>
     <row r="20" ht="20.05" customHeight="1">
@@ -2937,27 +3641,27 @@
       </c>
       <c r="B20" s="15">
         <f>B18/B19</f>
-        <v>39.360827246774</v>
-      </c>
-      <c r="C20" s="33"/>
-      <c r="D20" s="37"/>
-      <c r="E20" s="33"/>
-      <c r="F20" s="33"/>
-      <c r="G20" s="33"/>
+        <v>51.3402094523139</v>
+      </c>
+      <c r="C20" s="32"/>
+      <c r="D20" s="48"/>
+      <c r="E20" s="32"/>
+      <c r="F20" s="32"/>
+      <c r="G20" s="32"/>
     </row>
     <row r="21" ht="20.05" customHeight="1">
       <c r="A21" s="17"/>
       <c r="B21" s="18"/>
-      <c r="C21" s="33"/>
-      <c r="D21" t="s" s="38">
-        <v>30</v>
-      </c>
-      <c r="E21" s="34">
-        <v>2.28</v>
-      </c>
-      <c r="F21" s="33"/>
-      <c r="G21" s="34">
-        <v>2.28</v>
+      <c r="C21" s="32"/>
+      <c r="D21" t="s" s="49">
+        <v>46</v>
+      </c>
+      <c r="E21" s="30">
+        <v>1.25</v>
+      </c>
+      <c r="F21" s="32"/>
+      <c r="G21" s="30">
+        <v>1.25</v>
       </c>
     </row>
     <row r="22" ht="20.05" customHeight="1">
@@ -2965,18 +3669,18 @@
         <v>23</v>
       </c>
       <c r="B22" s="18"/>
-      <c r="C22" s="33"/>
-      <c r="D22" t="s" s="38">
-        <v>31</v>
-      </c>
-      <c r="E22" s="35">
+      <c r="C22" s="32"/>
+      <c r="D22" t="s" s="49">
+        <v>47</v>
+      </c>
+      <c r="E22" s="33">
         <f>E19/E21</f>
-        <v>711789473.684211</v>
-      </c>
-      <c r="F22" s="40"/>
-      <c r="G22" s="35">
+        <v>1693440000</v>
+      </c>
+      <c r="F22" s="51"/>
+      <c r="G22" s="33">
         <f>G19/G21</f>
-        <v>199301052.631579</v>
+        <v>474163200</v>
       </c>
     </row>
     <row r="23" ht="20.05" customHeight="1">
@@ -2986,11 +3690,11 @@
       <c r="B23" s="24">
         <v>2100000000</v>
       </c>
-      <c r="C23" s="33"/>
-      <c r="D23" s="37"/>
-      <c r="E23" s="33"/>
-      <c r="F23" s="33"/>
-      <c r="G23" s="33"/>
+      <c r="C23" s="32"/>
+      <c r="D23" s="48"/>
+      <c r="E23" s="32"/>
+      <c r="F23" s="32"/>
+      <c r="G23" s="32"/>
     </row>
     <row r="24" ht="20.05" customHeight="1">
       <c r="A24" t="s" s="14">
@@ -3000,16 +3704,16 @@
         <f>B23*B$11</f>
         <v>6174000000</v>
       </c>
-      <c r="C24" s="33"/>
-      <c r="D24" t="s" s="38">
-        <v>32</v>
-      </c>
-      <c r="E24" s="35">
-        <v>281259620</v>
-      </c>
-      <c r="F24" s="35"/>
-      <c r="G24" s="35">
-        <v>281259620</v>
+      <c r="C24" s="32"/>
+      <c r="D24" t="s" s="49">
+        <v>48</v>
+      </c>
+      <c r="E24" s="33">
+        <v>360788086</v>
+      </c>
+      <c r="F24" s="33"/>
+      <c r="G24" s="33">
+        <v>360788086</v>
       </c>
     </row>
     <row r="25" ht="20.05" customHeight="1">
@@ -3019,17 +3723,13 @@
       <c r="B25" s="20">
         <v>0.21</v>
       </c>
-      <c r="C25" s="33"/>
-      <c r="D25" t="s" s="38">
-        <v>33</v>
-      </c>
-      <c r="E25" s="35">
-        <v>50820911</v>
-      </c>
-      <c r="F25" s="35"/>
-      <c r="G25" s="35">
-        <v>50820911</v>
-      </c>
+      <c r="C25" s="32"/>
+      <c r="D25" t="s" s="49">
+        <v>49</v>
+      </c>
+      <c r="E25" s="33"/>
+      <c r="F25" s="33"/>
+      <c r="G25" s="33"/>
     </row>
     <row r="26" ht="20.05" customHeight="1">
       <c r="A26" t="s" s="14">
@@ -3038,17 +3738,13 @@
       <c r="B26" s="27">
         <v>0.1</v>
       </c>
-      <c r="C26" s="33"/>
-      <c r="D26" t="s" s="38">
-        <v>34</v>
-      </c>
-      <c r="E26" s="35">
-        <v>41845770</v>
-      </c>
-      <c r="F26" s="35"/>
-      <c r="G26" s="35">
-        <v>41845770</v>
-      </c>
+      <c r="C26" s="32"/>
+      <c r="D26" t="s" s="49">
+        <v>50</v>
+      </c>
+      <c r="E26" s="33"/>
+      <c r="F26" s="33"/>
+      <c r="G26" s="33"/>
     </row>
     <row r="27" ht="20.05" customHeight="1">
       <c r="A27" t="s" s="14">
@@ -3058,18 +3754,18 @@
         <f>B24*(1-(B25+B26))</f>
         <v>4260060000</v>
       </c>
-      <c r="C27" s="33"/>
-      <c r="D27" t="s" s="38">
-        <v>35</v>
-      </c>
-      <c r="E27" s="35">
+      <c r="C27" s="32"/>
+      <c r="D27" t="s" s="49">
+        <v>51</v>
+      </c>
+      <c r="E27" s="33">
         <f>E24-E25-E26</f>
-        <v>188592939</v>
-      </c>
-      <c r="F27" s="33"/>
-      <c r="G27" s="35">
+        <v>360788086</v>
+      </c>
+      <c r="F27" s="32"/>
+      <c r="G27" s="33">
         <f>G24-G25-G26</f>
-        <v>188592939</v>
+        <v>360788086</v>
       </c>
     </row>
     <row r="28" ht="20.05" customHeight="1">
@@ -3079,11 +3775,11 @@
       <c r="B28" s="24">
         <v>175000000</v>
       </c>
-      <c r="C28" s="33"/>
-      <c r="D28" s="37"/>
-      <c r="E28" s="35"/>
-      <c r="F28" s="35"/>
-      <c r="G28" s="35"/>
+      <c r="C28" s="32"/>
+      <c r="D28" s="48"/>
+      <c r="E28" s="33"/>
+      <c r="F28" s="33"/>
+      <c r="G28" s="33"/>
     </row>
     <row r="29" ht="20.05" customHeight="1">
       <c r="A29" t="s" s="14">
@@ -3093,28 +3789,28 @@
         <f>B27/B28</f>
         <v>24.3432</v>
       </c>
-      <c r="C29" s="33"/>
-      <c r="D29" t="s" s="38">
-        <v>36</v>
-      </c>
-      <c r="E29" s="35">
+      <c r="C29" s="32"/>
+      <c r="D29" t="s" s="49">
+        <v>52</v>
+      </c>
+      <c r="E29" s="33">
         <f>E27-E22</f>
-        <v>-523196534.684211</v>
-      </c>
-      <c r="F29" s="40"/>
-      <c r="G29" s="35">
+        <v>-1332651914</v>
+      </c>
+      <c r="F29" s="51"/>
+      <c r="G29" s="33">
         <f>G27-G22</f>
-        <v>-10708113.631579</v>
+        <v>-113375114</v>
       </c>
     </row>
     <row r="30" ht="20.05" customHeight="1">
       <c r="A30" s="17"/>
       <c r="B30" s="15"/>
-      <c r="C30" s="33"/>
-      <c r="D30" s="33"/>
-      <c r="E30" s="33"/>
-      <c r="F30" s="33"/>
-      <c r="G30" s="33"/>
+      <c r="C30" s="32"/>
+      <c r="D30" s="32"/>
+      <c r="E30" s="32"/>
+      <c r="F30" s="32"/>
+      <c r="G30" s="32"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3128,7 +3824,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -3141,13 +3837,13 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="6" width="16.3516" style="41" customWidth="1"/>
-    <col min="7" max="16384" width="16.3516" style="41" customWidth="1"/>
+    <col min="1" max="6" width="16.3516" style="52" customWidth="1"/>
+    <col min="7" max="16384" width="16.3516" style="52" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="27.65" customHeight="1">
       <c r="A1" t="s" s="7">
-        <v>37</v>
+        <v>53</v>
       </c>
       <c r="B1" s="7"/>
       <c r="C1" s="7"/>
@@ -3156,302 +3852,302 @@
       <c r="F1" s="7"/>
     </row>
     <row r="2" ht="20.05" customHeight="1">
-      <c r="A2" t="s" s="42">
-        <v>39</v>
-      </c>
-      <c r="B2" s="43">
+      <c r="A2" t="s" s="53">
+        <v>55</v>
+      </c>
+      <c r="B2" s="54">
         <v>1000</v>
       </c>
-      <c r="C2" s="33"/>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
-      <c r="F2" s="33"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
     </row>
     <row r="3" ht="20.05" customHeight="1">
-      <c r="A3" t="s" s="42">
-        <v>40</v>
-      </c>
-      <c r="B3" s="44">
+      <c r="A3" t="s" s="53">
+        <v>56</v>
+      </c>
+      <c r="B3" s="55">
         <v>1.6</v>
       </c>
-      <c r="C3" s="33"/>
-      <c r="D3" s="33"/>
-      <c r="E3" s="33"/>
-      <c r="F3" s="33"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
     </row>
     <row r="4" ht="20.05" customHeight="1">
-      <c r="A4" t="s" s="42">
-        <v>41</v>
-      </c>
-      <c r="B4" s="45">
+      <c r="A4" t="s" s="53">
+        <v>57</v>
+      </c>
+      <c r="B4" s="56">
         <f>B2*B3</f>
         <v>1600</v>
       </c>
-      <c r="C4" s="33"/>
-      <c r="D4" s="33"/>
-      <c r="E4" s="33"/>
-      <c r="F4" s="33"/>
+      <c r="C4" s="32"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="32"/>
+      <c r="F4" s="32"/>
     </row>
     <row r="5" ht="20.05" customHeight="1">
-      <c r="A5" s="46"/>
-      <c r="B5" s="47"/>
-      <c r="C5" s="33"/>
-      <c r="D5" s="33"/>
-      <c r="E5" s="33"/>
-      <c r="F5" s="33"/>
+      <c r="A5" s="57"/>
+      <c r="B5" s="58"/>
+      <c r="C5" s="32"/>
+      <c r="D5" s="32"/>
+      <c r="E5" s="32"/>
+      <c r="F5" s="32"/>
     </row>
     <row r="6" ht="20.05" customHeight="1">
-      <c r="A6" t="s" s="42">
-        <v>42</v>
-      </c>
-      <c r="B6" s="43">
+      <c r="A6" t="s" s="53">
+        <v>58</v>
+      </c>
+      <c r="B6" s="54">
         <v>75</v>
       </c>
-      <c r="C6" s="33"/>
-      <c r="D6" s="33"/>
-      <c r="E6" s="33"/>
-      <c r="F6" s="33"/>
+      <c r="C6" s="32"/>
+      <c r="D6" s="32"/>
+      <c r="E6" s="32"/>
+      <c r="F6" s="32"/>
     </row>
     <row r="7" ht="20.05" customHeight="1">
-      <c r="A7" t="s" s="42">
-        <v>43</v>
-      </c>
-      <c r="B7" s="45">
+      <c r="A7" t="s" s="53">
+        <v>59</v>
+      </c>
+      <c r="B7" s="56">
         <f>B6*B2</f>
         <v>75000</v>
       </c>
-      <c r="C7" s="33"/>
-      <c r="D7" s="33"/>
-      <c r="E7" s="33"/>
-      <c r="F7" s="33"/>
+      <c r="C7" s="32"/>
+      <c r="D7" s="32"/>
+      <c r="E7" s="32"/>
+      <c r="F7" s="32"/>
     </row>
     <row r="8" ht="20.05" customHeight="1">
-      <c r="A8" t="s" s="42">
-        <v>44</v>
-      </c>
-      <c r="B8" s="48">
+      <c r="A8" t="s" s="53">
+        <v>60</v>
+      </c>
+      <c r="B8" s="59">
         <v>0.371</v>
       </c>
-      <c r="C8" s="33"/>
-      <c r="D8" t="s" s="49">
-        <v>45</v>
-      </c>
-      <c r="E8" s="33"/>
-      <c r="F8" s="33"/>
+      <c r="C8" s="32"/>
+      <c r="D8" t="s" s="60">
+        <v>61</v>
+      </c>
+      <c r="E8" s="32"/>
+      <c r="F8" s="32"/>
     </row>
     <row r="9" ht="20.05" customHeight="1">
-      <c r="A9" t="s" s="42">
-        <v>46</v>
-      </c>
-      <c r="B9" s="45">
+      <c r="A9" t="s" s="53">
+        <v>62</v>
+      </c>
+      <c r="B9" s="56">
         <f>B8*B7</f>
         <v>27825</v>
       </c>
-      <c r="C9" s="33"/>
-      <c r="D9" s="50"/>
-      <c r="E9" s="33"/>
-      <c r="F9" s="33"/>
+      <c r="C9" s="32"/>
+      <c r="D9" s="61"/>
+      <c r="E9" s="32"/>
+      <c r="F9" s="32"/>
     </row>
     <row r="10" ht="20.05" customHeight="1">
-      <c r="A10" t="s" s="42">
-        <v>47</v>
-      </c>
-      <c r="B10" s="45">
+      <c r="A10" t="s" s="53">
+        <v>63</v>
+      </c>
+      <c r="B10" s="56">
         <f>B7-B9</f>
         <v>47175</v>
       </c>
-      <c r="C10" s="33"/>
-      <c r="D10" s="50"/>
-      <c r="E10" s="33"/>
-      <c r="F10" s="33"/>
+      <c r="C10" s="32"/>
+      <c r="D10" s="61"/>
+      <c r="E10" s="32"/>
+      <c r="F10" s="32"/>
     </row>
     <row r="11" ht="20.05" customHeight="1">
-      <c r="A11" s="46"/>
-      <c r="B11" s="47"/>
-      <c r="C11" s="33"/>
-      <c r="D11" s="50"/>
-      <c r="E11" s="33"/>
-      <c r="F11" s="33"/>
+      <c r="A11" s="57"/>
+      <c r="B11" s="58"/>
+      <c r="C11" s="32"/>
+      <c r="D11" s="61"/>
+      <c r="E11" s="32"/>
+      <c r="F11" s="32"/>
     </row>
     <row r="12" ht="20.05" customHeight="1">
-      <c r="A12" t="s" s="42">
-        <v>48</v>
-      </c>
-      <c r="B12" s="47"/>
-      <c r="C12" s="33"/>
-      <c r="D12" s="50"/>
-      <c r="E12" s="33"/>
-      <c r="F12" s="33"/>
+      <c r="A12" t="s" s="53">
+        <v>64</v>
+      </c>
+      <c r="B12" s="58"/>
+      <c r="C12" s="32"/>
+      <c r="D12" s="61"/>
+      <c r="E12" s="32"/>
+      <c r="F12" s="32"/>
     </row>
     <row r="13" ht="20.05" customHeight="1">
-      <c r="A13" t="s" s="42">
-        <v>49</v>
-      </c>
-      <c r="B13" s="51">
+      <c r="A13" t="s" s="53">
+        <v>65</v>
+      </c>
+      <c r="B13" s="62">
         <v>1</v>
       </c>
-      <c r="C13" s="33"/>
-      <c r="D13" s="50"/>
-      <c r="E13" s="33"/>
-      <c r="F13" s="33"/>
+      <c r="C13" s="32"/>
+      <c r="D13" s="61"/>
+      <c r="E13" s="32"/>
+      <c r="F13" s="32"/>
     </row>
     <row r="14" ht="20.05" customHeight="1">
-      <c r="A14" t="s" s="42">
-        <v>50</v>
-      </c>
-      <c r="B14" s="45">
+      <c r="A14" t="s" s="53">
+        <v>66</v>
+      </c>
+      <c r="B14" s="56">
         <f>B13*B10</f>
         <v>47175</v>
       </c>
-      <c r="C14" s="33"/>
-      <c r="D14" s="50"/>
-      <c r="E14" s="33"/>
-      <c r="F14" s="33"/>
+      <c r="C14" s="32"/>
+      <c r="D14" s="61"/>
+      <c r="E14" s="32"/>
+      <c r="F14" s="32"/>
     </row>
     <row r="15" ht="20.05" customHeight="1">
-      <c r="A15" t="s" s="42">
-        <v>51</v>
-      </c>
-      <c r="B15" s="43">
-        <v>2.25</v>
-      </c>
-      <c r="C15" s="33"/>
-      <c r="D15" s="50"/>
-      <c r="E15" s="33"/>
-      <c r="F15" s="33"/>
+      <c r="A15" t="s" s="53">
+        <v>67</v>
+      </c>
+      <c r="B15" s="54">
+        <v>1.25</v>
+      </c>
+      <c r="C15" s="32"/>
+      <c r="D15" s="61"/>
+      <c r="E15" s="32"/>
+      <c r="F15" s="32"/>
     </row>
     <row r="16" ht="20.05" customHeight="1">
-      <c r="A16" t="s" s="42">
-        <v>52</v>
-      </c>
-      <c r="B16" s="52">
+      <c r="A16" t="s" s="53">
+        <v>68</v>
+      </c>
+      <c r="B16" s="63">
         <f>B14/B15</f>
-        <v>20966.6666666667</v>
-      </c>
-      <c r="C16" s="33"/>
-      <c r="D16" s="50"/>
-      <c r="E16" s="33"/>
-      <c r="F16" s="33"/>
+        <v>37740</v>
+      </c>
+      <c r="C16" s="32"/>
+      <c r="D16" s="61"/>
+      <c r="E16" s="32"/>
+      <c r="F16" s="32"/>
     </row>
     <row r="17" ht="20.05" customHeight="1">
-      <c r="A17" s="46"/>
-      <c r="B17" s="47"/>
-      <c r="C17" s="33"/>
-      <c r="D17" s="50"/>
-      <c r="E17" s="33"/>
-      <c r="F17" s="33"/>
+      <c r="A17" s="57"/>
+      <c r="B17" s="58"/>
+      <c r="C17" s="32"/>
+      <c r="D17" s="61"/>
+      <c r="E17" s="32"/>
+      <c r="F17" s="32"/>
     </row>
     <row r="18" ht="20.05" customHeight="1">
-      <c r="A18" s="46"/>
-      <c r="B18" t="s" s="53">
-        <v>53</v>
-      </c>
-      <c r="C18" s="54"/>
-      <c r="D18" t="s" s="55">
-        <v>54</v>
-      </c>
-      <c r="E18" s="33"/>
-      <c r="F18" s="33"/>
+      <c r="A18" s="57"/>
+      <c r="B18" t="s" s="64">
+        <v>69</v>
+      </c>
+      <c r="C18" s="65"/>
+      <c r="D18" t="s" s="66">
+        <v>70</v>
+      </c>
+      <c r="E18" s="32"/>
+      <c r="F18" s="32"/>
     </row>
     <row r="19" ht="20.05" customHeight="1">
-      <c r="A19" t="s" s="42">
-        <v>55</v>
-      </c>
-      <c r="B19" s="43">
+      <c r="A19" t="s" s="53">
+        <v>71</v>
+      </c>
+      <c r="B19" s="54">
         <v>100</v>
       </c>
-      <c r="C19" s="33"/>
-      <c r="D19" s="34">
+      <c r="C19" s="32"/>
+      <c r="D19" s="30">
         <v>100</v>
       </c>
-      <c r="E19" s="33"/>
-      <c r="F19" s="33"/>
+      <c r="E19" s="32"/>
+      <c r="F19" s="32"/>
     </row>
     <row r="20" ht="20.05" customHeight="1">
-      <c r="A20" t="s" s="42">
+      <c r="A20" t="s" s="53">
         <v>10</v>
       </c>
-      <c r="B20" s="52">
+      <c r="B20" s="63">
         <f>B19*$B16</f>
-        <v>2096666.66666667</v>
-      </c>
-      <c r="C20" s="33"/>
-      <c r="D20" s="35">
+        <v>3774000</v>
+      </c>
+      <c r="C20" s="32"/>
+      <c r="D20" s="33">
         <f>D19*$B16</f>
-        <v>2096666.66666667</v>
-      </c>
-      <c r="E20" s="33"/>
-      <c r="F20" s="33"/>
+        <v>3774000</v>
+      </c>
+      <c r="E20" s="32"/>
+      <c r="F20" s="32"/>
     </row>
     <row r="21" ht="20.05" customHeight="1">
-      <c r="A21" t="s" s="42">
-        <v>56</v>
-      </c>
-      <c r="B21" s="52">
+      <c r="A21" t="s" s="53">
+        <v>72</v>
+      </c>
+      <c r="B21" s="63">
         <f>B20-$B14</f>
-        <v>2049491.66666667</v>
-      </c>
-      <c r="C21" s="33"/>
-      <c r="D21" s="35">
+        <v>3726825</v>
+      </c>
+      <c r="C21" s="32"/>
+      <c r="D21" s="33">
         <f>D20-$B14</f>
-        <v>2049491.66666667</v>
-      </c>
-      <c r="E21" s="33"/>
-      <c r="F21" s="33"/>
+        <v>3726825</v>
+      </c>
+      <c r="E21" s="32"/>
+      <c r="F21" s="32"/>
     </row>
     <row r="22" ht="20.05" customHeight="1">
-      <c r="A22" t="s" s="42">
-        <v>44</v>
-      </c>
-      <c r="B22" s="48">
+      <c r="A22" t="s" s="53">
+        <v>60</v>
+      </c>
+      <c r="B22" s="59">
         <v>0.541</v>
       </c>
-      <c r="C22" s="33"/>
-      <c r="D22" s="56">
+      <c r="C22" s="32"/>
+      <c r="D22" s="67">
         <v>0.371</v>
       </c>
-      <c r="E22" s="33"/>
-      <c r="F22" s="33"/>
+      <c r="E22" s="32"/>
+      <c r="F22" s="32"/>
     </row>
     <row r="23" ht="20.05" customHeight="1">
-      <c r="A23" t="s" s="42">
-        <v>46</v>
-      </c>
-      <c r="B23" s="52">
+      <c r="A23" t="s" s="53">
+        <v>62</v>
+      </c>
+      <c r="B23" s="63">
         <f>B22*B21</f>
-        <v>1108774.99166667</v>
-      </c>
-      <c r="C23" s="33"/>
-      <c r="D23" s="35">
+        <v>2016212.325</v>
+      </c>
+      <c r="C23" s="32"/>
+      <c r="D23" s="33">
         <f>D22*D21</f>
-        <v>760361.408333335</v>
-      </c>
-      <c r="E23" s="33"/>
-      <c r="F23" s="33"/>
+        <v>1382652.075</v>
+      </c>
+      <c r="E23" s="32"/>
+      <c r="F23" s="32"/>
     </row>
     <row r="24" ht="20.05" customHeight="1">
-      <c r="A24" t="s" s="42">
-        <v>47</v>
-      </c>
-      <c r="B24" s="52">
+      <c r="A24" t="s" s="53">
+        <v>63</v>
+      </c>
+      <c r="B24" s="63">
         <f>B21-B23</f>
-        <v>940716.675</v>
-      </c>
-      <c r="C24" s="33"/>
-      <c r="D24" s="35">
+        <v>1710612.675</v>
+      </c>
+      <c r="C24" s="32"/>
+      <c r="D24" s="33">
         <f>D21-D23</f>
-        <v>1289130.25833334</v>
-      </c>
-      <c r="E24" s="33"/>
-      <c r="F24" s="33"/>
+        <v>2344172.925</v>
+      </c>
+      <c r="E24" s="32"/>
+      <c r="F24" s="32"/>
     </row>
     <row r="25" ht="20.05" customHeight="1">
-      <c r="A25" s="46"/>
-      <c r="B25" s="47"/>
-      <c r="C25" s="33"/>
-      <c r="D25" s="50"/>
-      <c r="E25" s="33"/>
-      <c r="F25" s="33"/>
+      <c r="A25" s="57"/>
+      <c r="B25" s="58"/>
+      <c r="C25" s="32"/>
+      <c r="D25" s="61"/>
+      <c r="E25" s="32"/>
+      <c r="F25" s="32"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3465,7 +4161,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -3478,1309 +4174,1309 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="3.40625" style="57" customWidth="1"/>
-    <col min="2" max="2" width="44.6562" style="57" customWidth="1"/>
-    <col min="3" max="24" width="15.3047" style="57" customWidth="1"/>
-    <col min="25" max="16384" width="16.3516" style="57" customWidth="1"/>
+    <col min="1" max="1" width="3.40625" style="68" customWidth="1"/>
+    <col min="2" max="2" width="44.6562" style="68" customWidth="1"/>
+    <col min="3" max="24" width="15.3047" style="68" customWidth="1"/>
+    <col min="25" max="16384" width="16.3516" style="68" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="36.45" customHeight="1">
-      <c r="B1" t="s" s="58">
-        <v>58</v>
-      </c>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
-      <c r="E1" s="58"/>
-      <c r="F1" s="58"/>
-      <c r="G1" s="58"/>
-      <c r="H1" s="58"/>
-      <c r="I1" s="58"/>
-      <c r="J1" s="58"/>
-      <c r="K1" s="58"/>
-      <c r="L1" s="58"/>
-      <c r="M1" s="58"/>
-      <c r="N1" s="58"/>
-      <c r="O1" s="58"/>
-      <c r="P1" s="58"/>
-      <c r="Q1" s="58"/>
-      <c r="R1" s="58"/>
-      <c r="S1" s="58"/>
-      <c r="T1" s="58"/>
-      <c r="U1" s="58"/>
-      <c r="V1" s="58"/>
-      <c r="W1" s="58"/>
-      <c r="X1" s="58"/>
+      <c r="B1" t="s" s="69">
+        <v>74</v>
+      </c>
+      <c r="C1" s="69"/>
+      <c r="D1" s="69"/>
+      <c r="E1" s="69"/>
+      <c r="F1" s="69"/>
+      <c r="G1" s="69"/>
+      <c r="H1" s="69"/>
+      <c r="I1" s="69"/>
+      <c r="J1" s="69"/>
+      <c r="K1" s="69"/>
+      <c r="L1" s="69"/>
+      <c r="M1" s="69"/>
+      <c r="N1" s="69"/>
+      <c r="O1" s="69"/>
+      <c r="P1" s="69"/>
+      <c r="Q1" s="69"/>
+      <c r="R1" s="69"/>
+      <c r="S1" s="69"/>
+      <c r="T1" s="69"/>
+      <c r="U1" s="69"/>
+      <c r="V1" s="69"/>
+      <c r="W1" s="69"/>
+      <c r="X1" s="69"/>
     </row>
     <row r="2" ht="20.55" customHeight="1">
-      <c r="B2" t="s" s="59">
+      <c r="B2" t="s" s="70">
         <v>8</v>
       </c>
-      <c r="C2" s="60">
+      <c r="C2" s="71">
         <v>30</v>
       </c>
-      <c r="D2" s="60">
+      <c r="D2" s="71">
         <v>40</v>
       </c>
-      <c r="E2" s="60">
+      <c r="E2" s="71">
         <v>50</v>
       </c>
-      <c r="F2" s="60">
+      <c r="F2" s="71">
         <v>60</v>
       </c>
-      <c r="G2" s="60">
+      <c r="G2" s="71">
         <f>F2+5</f>
         <v>65</v>
       </c>
-      <c r="H2" s="60">
+      <c r="H2" s="71">
         <f>F2+10</f>
         <v>70</v>
       </c>
-      <c r="I2" s="60">
+      <c r="I2" s="71">
         <f>H2+5</f>
         <v>75</v>
       </c>
-      <c r="J2" s="60">
+      <c r="J2" s="71">
         <f>H2+10</f>
         <v>80</v>
       </c>
-      <c r="K2" s="60">
+      <c r="K2" s="71">
         <f>J2+5</f>
         <v>85</v>
       </c>
-      <c r="L2" s="60">
+      <c r="L2" s="71">
         <f>J2+10</f>
         <v>90</v>
       </c>
-      <c r="M2" s="60">
+      <c r="M2" s="71">
         <f>L2+5</f>
         <v>95</v>
       </c>
-      <c r="N2" s="60">
+      <c r="N2" s="71">
         <f>L2+10</f>
         <v>100</v>
       </c>
-      <c r="O2" s="60">
+      <c r="O2" s="71">
         <f>N2+5</f>
         <v>105</v>
       </c>
-      <c r="P2" s="60">
+      <c r="P2" s="71">
         <f>O2+5</f>
         <v>110</v>
       </c>
-      <c r="Q2" s="60">
+      <c r="Q2" s="71">
         <f>P2+5</f>
         <v>115</v>
       </c>
-      <c r="R2" s="60">
+      <c r="R2" s="71">
         <f>Q2+5</f>
         <v>120</v>
       </c>
-      <c r="S2" s="60">
+      <c r="S2" s="71">
         <f>R2+5</f>
         <v>125</v>
       </c>
-      <c r="T2" s="60">
+      <c r="T2" s="71">
         <f>S2+5</f>
         <v>130</v>
       </c>
-      <c r="U2" s="60">
+      <c r="U2" s="71">
         <f>T2+5</f>
         <v>135</v>
       </c>
-      <c r="V2" s="60">
+      <c r="V2" s="71">
         <f>U2+5</f>
         <v>140</v>
       </c>
-      <c r="W2" s="60">
+      <c r="W2" s="71">
         <f>V2+5</f>
         <v>145</v>
       </c>
-      <c r="X2" s="60">
+      <c r="X2" s="71">
         <f>W2+5</f>
         <v>150</v>
       </c>
     </row>
     <row r="3" ht="20.35" customHeight="1">
-      <c r="B3" t="s" s="61">
+      <c r="B3" t="s" s="72">
         <v>9</v>
       </c>
-      <c r="C3" s="62">
+      <c r="C3" s="73">
+        <v>35</v>
+      </c>
+      <c r="D3" s="74">
+        <v>35</v>
+      </c>
+      <c r="E3" s="74">
+        <v>35</v>
+      </c>
+      <c r="F3" s="74">
+        <v>35</v>
+      </c>
+      <c r="G3" s="74">
+        <v>35</v>
+      </c>
+      <c r="H3" s="74">
+        <v>35</v>
+      </c>
+      <c r="I3" s="74">
+        <v>35</v>
+      </c>
+      <c r="J3" s="74">
+        <v>35</v>
+      </c>
+      <c r="K3" s="74">
+        <v>35</v>
+      </c>
+      <c r="L3" s="74">
+        <v>35</v>
+      </c>
+      <c r="M3" s="74">
+        <v>35</v>
+      </c>
+      <c r="N3" s="74">
+        <v>35</v>
+      </c>
+      <c r="O3" s="74">
+        <v>35</v>
+      </c>
+      <c r="P3" s="74">
+        <v>35</v>
+      </c>
+      <c r="Q3" s="74">
+        <v>35</v>
+      </c>
+      <c r="R3" s="74">
+        <v>35</v>
+      </c>
+      <c r="S3" s="74">
+        <v>35</v>
+      </c>
+      <c r="T3" s="74">
+        <v>35</v>
+      </c>
+      <c r="U3" s="74">
+        <v>35</v>
+      </c>
+      <c r="V3" s="74">
+        <v>35</v>
+      </c>
+      <c r="W3" s="74">
+        <v>35</v>
+      </c>
+      <c r="X3" s="74">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" ht="20.35" customHeight="1">
+      <c r="B4" t="s" s="75">
+        <v>10</v>
+      </c>
+      <c r="C4" s="76">
+        <f>C2-C3</f>
+        <v>-5</v>
+      </c>
+      <c r="D4" s="77">
+        <f>D2-D3</f>
+        <v>5</v>
+      </c>
+      <c r="E4" s="77">
+        <f>E2-E3</f>
+        <v>15</v>
+      </c>
+      <c r="F4" s="77">
+        <f>F2-F3</f>
+        <v>25</v>
+      </c>
+      <c r="G4" s="77">
+        <f>G2-G3</f>
         <v>30</v>
       </c>
-      <c r="D3" s="63">
-        <v>30</v>
-      </c>
-      <c r="E3" s="63">
-        <v>30</v>
-      </c>
-      <c r="F3" s="63">
-        <v>30</v>
-      </c>
-      <c r="G3" s="63">
-        <v>30</v>
-      </c>
-      <c r="H3" s="63">
-        <v>30</v>
-      </c>
-      <c r="I3" s="63">
-        <v>30</v>
-      </c>
-      <c r="J3" s="63">
-        <v>30</v>
-      </c>
-      <c r="K3" s="63">
-        <v>30</v>
-      </c>
-      <c r="L3" s="63">
-        <v>30</v>
-      </c>
-      <c r="M3" s="63">
-        <v>30</v>
-      </c>
-      <c r="N3" s="63">
-        <v>30</v>
-      </c>
-      <c r="O3" s="63">
-        <v>30</v>
-      </c>
-      <c r="P3" s="63">
-        <v>30</v>
-      </c>
-      <c r="Q3" s="63">
-        <v>30</v>
-      </c>
-      <c r="R3" s="63">
-        <v>30</v>
-      </c>
-      <c r="S3" s="63">
-        <v>30</v>
-      </c>
-      <c r="T3" s="63">
-        <v>30</v>
-      </c>
-      <c r="U3" s="63">
-        <v>30</v>
-      </c>
-      <c r="V3" s="63">
-        <v>30</v>
-      </c>
-      <c r="W3" s="63">
-        <v>30</v>
-      </c>
-      <c r="X3" s="63">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" ht="20.35" customHeight="1">
-      <c r="B4" t="s" s="64">
-        <v>10</v>
-      </c>
-      <c r="C4" s="65">
-        <f>C2-C3</f>
+      <c r="H4" s="77">
+        <f>H2-H3</f>
+        <v>35</v>
+      </c>
+      <c r="I4" s="77">
+        <f>I2-I3</f>
+        <v>40</v>
+      </c>
+      <c r="J4" s="77">
+        <f>J2-J3</f>
+        <v>45</v>
+      </c>
+      <c r="K4" s="77">
+        <f>K2-K3</f>
+        <v>50</v>
+      </c>
+      <c r="L4" s="77">
+        <f>L2-L3</f>
+        <v>55</v>
+      </c>
+      <c r="M4" s="77">
+        <f>M2-M3</f>
+        <v>60</v>
+      </c>
+      <c r="N4" s="77">
+        <f>N2-N3</f>
+        <v>65</v>
+      </c>
+      <c r="O4" s="77">
+        <f>O2-O3</f>
+        <v>70</v>
+      </c>
+      <c r="P4" s="77">
+        <f>P2-P3</f>
+        <v>75</v>
+      </c>
+      <c r="Q4" s="77">
+        <f>Q2-Q3</f>
+        <v>80</v>
+      </c>
+      <c r="R4" s="77">
+        <f>R2-R3</f>
+        <v>85</v>
+      </c>
+      <c r="S4" s="77">
+        <f>S2-S3</f>
+        <v>90</v>
+      </c>
+      <c r="T4" s="77">
+        <f>T2-T3</f>
+        <v>95</v>
+      </c>
+      <c r="U4" s="77">
+        <f>U2-U3</f>
+        <v>100</v>
+      </c>
+      <c r="V4" s="77">
+        <f>V2-V3</f>
+        <v>105</v>
+      </c>
+      <c r="W4" s="77">
+        <f>W2-W3</f>
+        <v>110</v>
+      </c>
+      <c r="X4" s="77">
+        <f>X2-X3</f>
+        <v>115</v>
+      </c>
+    </row>
+    <row r="5" ht="20.35" customHeight="1">
+      <c r="B5" s="78"/>
+      <c r="C5" s="79"/>
+      <c r="D5" s="80"/>
+      <c r="E5" s="80"/>
+      <c r="F5" s="80"/>
+      <c r="G5" s="80"/>
+      <c r="H5" s="80"/>
+      <c r="I5" s="80"/>
+      <c r="J5" s="80"/>
+      <c r="K5" s="80"/>
+      <c r="L5" s="80"/>
+      <c r="M5" s="80"/>
+      <c r="N5" s="80"/>
+      <c r="O5" s="80"/>
+      <c r="P5" s="80"/>
+      <c r="Q5" s="80"/>
+      <c r="R5" s="80"/>
+      <c r="S5" s="80"/>
+      <c r="T5" s="80"/>
+      <c r="U5" s="80"/>
+      <c r="V5" s="80"/>
+      <c r="W5" s="80"/>
+      <c r="X5" s="80"/>
+    </row>
+    <row r="6" ht="20.35" customHeight="1">
+      <c r="B6" t="s" s="75">
+        <v>11</v>
+      </c>
+      <c r="C6" s="81">
+        <v>0.12</v>
+      </c>
+      <c r="D6" s="82">
+        <v>0.12</v>
+      </c>
+      <c r="E6" s="82">
+        <v>0.12</v>
+      </c>
+      <c r="F6" s="82">
+        <v>0.12</v>
+      </c>
+      <c r="G6" s="82">
+        <v>0.12</v>
+      </c>
+      <c r="H6" s="82">
+        <v>0.12</v>
+      </c>
+      <c r="I6" s="82">
+        <v>0.12</v>
+      </c>
+      <c r="J6" s="82">
+        <v>0.12</v>
+      </c>
+      <c r="K6" s="82">
+        <v>0.12</v>
+      </c>
+      <c r="L6" s="82">
+        <v>0.12</v>
+      </c>
+      <c r="M6" s="82">
+        <v>0.12</v>
+      </c>
+      <c r="N6" s="82">
+        <v>0.12</v>
+      </c>
+      <c r="O6" s="82">
+        <v>0.12</v>
+      </c>
+      <c r="P6" s="82">
+        <v>0.12</v>
+      </c>
+      <c r="Q6" s="82">
+        <v>0.12</v>
+      </c>
+      <c r="R6" s="82">
+        <v>0.12</v>
+      </c>
+      <c r="S6" s="82">
+        <v>0.12</v>
+      </c>
+      <c r="T6" s="82">
+        <v>0.12</v>
+      </c>
+      <c r="U6" s="82">
+        <v>0.12</v>
+      </c>
+      <c r="V6" s="82">
+        <v>0.12</v>
+      </c>
+      <c r="W6" s="82">
+        <v>0.12</v>
+      </c>
+      <c r="X6" s="82">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="7" ht="20.35" customHeight="1">
+      <c r="B7" t="s" s="75">
+        <v>12</v>
+      </c>
+      <c r="C7" s="76">
+        <f>C6*C4</f>
+        <v>-0.6</v>
+      </c>
+      <c r="D7" s="77">
+        <f>D6*D4</f>
+        <v>0.6</v>
+      </c>
+      <c r="E7" s="77">
+        <f>E6*E4</f>
+        <v>1.8</v>
+      </c>
+      <c r="F7" s="77">
+        <f>F6*F4</f>
+        <v>3</v>
+      </c>
+      <c r="G7" s="77">
+        <f>G6*G4</f>
+        <v>3.6</v>
+      </c>
+      <c r="H7" s="77">
+        <f>H6*H4</f>
+        <v>4.2</v>
+      </c>
+      <c r="I7" s="77">
+        <f>I6*I4</f>
+        <v>4.8</v>
+      </c>
+      <c r="J7" s="77">
+        <f>J6*J4</f>
+        <v>5.4</v>
+      </c>
+      <c r="K7" s="77">
+        <f>K6*K4</f>
+        <v>6</v>
+      </c>
+      <c r="L7" s="77">
+        <f>L6*L4</f>
+        <v>6.6</v>
+      </c>
+      <c r="M7" s="77">
+        <f>M6*M4</f>
+        <v>7.2</v>
+      </c>
+      <c r="N7" s="77">
+        <f>N6*N4</f>
+        <v>7.8</v>
+      </c>
+      <c r="O7" s="77">
+        <f>O6*O4</f>
+        <v>8.4</v>
+      </c>
+      <c r="P7" s="77">
+        <f>P6*P4</f>
+        <v>9</v>
+      </c>
+      <c r="Q7" s="77">
+        <f>Q6*Q4</f>
+        <v>9.6</v>
+      </c>
+      <c r="R7" s="77">
+        <f>R6*R4</f>
+        <v>10.2</v>
+      </c>
+      <c r="S7" s="77">
+        <f>S6*S4</f>
+        <v>10.8</v>
+      </c>
+      <c r="T7" s="77">
+        <f>T6*T4</f>
+        <v>11.4</v>
+      </c>
+      <c r="U7" s="77">
+        <f>U6*U4</f>
+        <v>12</v>
+      </c>
+      <c r="V7" s="77">
+        <f>V6*V4</f>
+        <v>12.6</v>
+      </c>
+      <c r="W7" s="77">
+        <f>W6*W4</f>
+        <v>13.2</v>
+      </c>
+      <c r="X7" s="77">
+        <f>X6*X4</f>
+        <v>13.8</v>
+      </c>
+    </row>
+    <row r="8" ht="20.35" customHeight="1">
+      <c r="B8" s="78"/>
+      <c r="C8" s="79"/>
+      <c r="D8" s="80"/>
+      <c r="E8" s="80"/>
+      <c r="F8" s="80"/>
+      <c r="G8" s="80"/>
+      <c r="H8" s="80"/>
+      <c r="I8" s="80"/>
+      <c r="J8" s="80"/>
+      <c r="K8" s="80"/>
+      <c r="L8" s="80"/>
+      <c r="M8" s="80"/>
+      <c r="N8" s="80"/>
+      <c r="O8" s="80"/>
+      <c r="P8" s="80"/>
+      <c r="Q8" s="80"/>
+      <c r="R8" s="80"/>
+      <c r="S8" s="80"/>
+      <c r="T8" s="80"/>
+      <c r="U8" s="80"/>
+      <c r="V8" s="80"/>
+      <c r="W8" s="80"/>
+      <c r="X8" s="80"/>
+    </row>
+    <row r="9" ht="20.35" customHeight="1">
+      <c r="B9" t="s" s="75">
+        <v>13</v>
+      </c>
+      <c r="C9" s="81">
+        <v>0.49</v>
+      </c>
+      <c r="D9" s="82">
+        <v>0.49</v>
+      </c>
+      <c r="E9" s="82">
+        <v>0.49</v>
+      </c>
+      <c r="F9" s="82">
+        <v>0.49</v>
+      </c>
+      <c r="G9" s="82">
+        <v>0.49</v>
+      </c>
+      <c r="H9" s="82">
+        <v>0.49</v>
+      </c>
+      <c r="I9" s="82">
+        <v>0.49</v>
+      </c>
+      <c r="J9" s="82">
+        <v>0.49</v>
+      </c>
+      <c r="K9" s="82">
+        <v>0.49</v>
+      </c>
+      <c r="L9" s="82">
+        <v>0.49</v>
+      </c>
+      <c r="M9" s="82">
+        <v>0.49</v>
+      </c>
+      <c r="N9" s="82">
+        <v>0.49</v>
+      </c>
+      <c r="O9" s="82">
+        <v>0.49</v>
+      </c>
+      <c r="P9" s="82">
+        <v>0.49</v>
+      </c>
+      <c r="Q9" s="82">
+        <v>0.49</v>
+      </c>
+      <c r="R9" s="82">
+        <v>0.49</v>
+      </c>
+      <c r="S9" s="82">
+        <v>0.49</v>
+      </c>
+      <c r="T9" s="82">
+        <v>0.49</v>
+      </c>
+      <c r="U9" s="82">
+        <v>0.49</v>
+      </c>
+      <c r="V9" s="82">
+        <v>0.49</v>
+      </c>
+      <c r="W9" s="82">
+        <v>0.49</v>
+      </c>
+      <c r="X9" s="82">
+        <v>0.49</v>
+      </c>
+    </row>
+    <row r="10" ht="20.35" customHeight="1">
+      <c r="B10" t="s" s="75">
+        <v>14</v>
+      </c>
+      <c r="C10" s="83">
+        <f>C7*C9</f>
+        <v>-0.294</v>
+      </c>
+      <c r="D10" s="84">
+        <f>D7*D9</f>
+        <v>0.294</v>
+      </c>
+      <c r="E10" s="84">
+        <f>E7*E9</f>
+        <v>0.882</v>
+      </c>
+      <c r="F10" s="84">
+        <f>F7*F9</f>
+        <v>1.47</v>
+      </c>
+      <c r="G10" s="84">
+        <f>G7*G9</f>
+        <v>1.764</v>
+      </c>
+      <c r="H10" s="84">
+        <f>H7*H9</f>
+        <v>2.058</v>
+      </c>
+      <c r="I10" s="84">
+        <f>I7*I9</f>
+        <v>2.352</v>
+      </c>
+      <c r="J10" s="84">
+        <f>J7*J9</f>
+        <v>2.646</v>
+      </c>
+      <c r="K10" s="84">
+        <f>K7*K9</f>
+        <v>2.94</v>
+      </c>
+      <c r="L10" s="84">
+        <f>L7*L9</f>
+        <v>3.234</v>
+      </c>
+      <c r="M10" s="84">
+        <f>M7*M9</f>
+        <v>3.528</v>
+      </c>
+      <c r="N10" s="84">
+        <f>N7*N9</f>
+        <v>3.822</v>
+      </c>
+      <c r="O10" s="84">
+        <f>O7*O9</f>
+        <v>4.116</v>
+      </c>
+      <c r="P10" s="84">
+        <f>P7*P9</f>
+        <v>4.41</v>
+      </c>
+      <c r="Q10" s="84">
+        <f>Q7*Q9</f>
+        <v>4.704</v>
+      </c>
+      <c r="R10" s="84">
+        <f>R7*R9</f>
+        <v>4.998</v>
+      </c>
+      <c r="S10" s="84">
+        <f>S7*S9</f>
+        <v>5.292</v>
+      </c>
+      <c r="T10" s="84">
+        <f>T7*T9</f>
+        <v>5.586</v>
+      </c>
+      <c r="U10" s="84">
+        <f>U7*U9</f>
+        <v>5.88</v>
+      </c>
+      <c r="V10" s="84">
+        <f>V7*V9</f>
+        <v>6.174</v>
+      </c>
+      <c r="W10" s="84">
+        <f>W7*W9</f>
+        <v>6.468</v>
+      </c>
+      <c r="X10" s="84">
+        <f>X7*X9</f>
+        <v>6.762</v>
+      </c>
+    </row>
+    <row r="11" ht="20.35" customHeight="1">
+      <c r="B11" s="78"/>
+      <c r="C11" s="79"/>
+      <c r="D11" s="80"/>
+      <c r="E11" s="80"/>
+      <c r="F11" s="80"/>
+      <c r="G11" s="80"/>
+      <c r="H11" s="80"/>
+      <c r="I11" s="80"/>
+      <c r="J11" s="80"/>
+      <c r="K11" s="80"/>
+      <c r="L11" s="80"/>
+      <c r="M11" s="80"/>
+      <c r="N11" s="80"/>
+      <c r="O11" s="80"/>
+      <c r="P11" s="80"/>
+      <c r="Q11" s="80"/>
+      <c r="R11" s="80"/>
+      <c r="S11" s="80"/>
+      <c r="T11" s="80"/>
+      <c r="U11" s="80"/>
+      <c r="V11" s="80"/>
+      <c r="W11" s="80"/>
+      <c r="X11" s="80"/>
+    </row>
+    <row r="12" ht="20.35" customHeight="1">
+      <c r="B12" t="s" s="75">
+        <v>15</v>
+      </c>
+      <c r="C12" s="79"/>
+      <c r="D12" s="80"/>
+      <c r="E12" s="80"/>
+      <c r="F12" s="80"/>
+      <c r="G12" s="80"/>
+      <c r="H12" s="80"/>
+      <c r="I12" s="80"/>
+      <c r="J12" s="80"/>
+      <c r="K12" s="80"/>
+      <c r="L12" s="80"/>
+      <c r="M12" s="80"/>
+      <c r="N12" s="80"/>
+      <c r="O12" s="80"/>
+      <c r="P12" s="80"/>
+      <c r="Q12" s="80"/>
+      <c r="R12" s="80"/>
+      <c r="S12" s="80"/>
+      <c r="T12" s="80"/>
+      <c r="U12" s="80"/>
+      <c r="V12" s="80"/>
+      <c r="W12" s="80"/>
+      <c r="X12" s="80"/>
+    </row>
+    <row r="13" ht="20.35" customHeight="1">
+      <c r="B13" t="s" s="75">
+        <v>16</v>
+      </c>
+      <c r="C13" s="85">
+        <v>3200000000</v>
+      </c>
+      <c r="D13" s="86">
+        <v>3200000000</v>
+      </c>
+      <c r="E13" s="86">
+        <v>3200000000</v>
+      </c>
+      <c r="F13" s="86">
+        <v>3200000000</v>
+      </c>
+      <c r="G13" s="86">
+        <v>3200000000</v>
+      </c>
+      <c r="H13" s="86">
+        <v>3200000000</v>
+      </c>
+      <c r="I13" s="86">
+        <v>3200000000</v>
+      </c>
+      <c r="J13" s="86">
+        <v>3200000000</v>
+      </c>
+      <c r="K13" s="86">
+        <v>3200000000</v>
+      </c>
+      <c r="L13" s="86">
+        <v>3200000000</v>
+      </c>
+      <c r="M13" s="86">
+        <v>3200000000</v>
+      </c>
+      <c r="N13" s="86">
+        <v>3200000000</v>
+      </c>
+      <c r="O13" s="86">
+        <v>3200000000</v>
+      </c>
+      <c r="P13" s="86">
+        <v>3200000000</v>
+      </c>
+      <c r="Q13" s="86">
+        <v>3200000000</v>
+      </c>
+      <c r="R13" s="86">
+        <v>3200000000</v>
+      </c>
+      <c r="S13" s="86">
+        <v>3200000000</v>
+      </c>
+      <c r="T13" s="86">
+        <v>3200000000</v>
+      </c>
+      <c r="U13" s="86">
+        <v>3200000000</v>
+      </c>
+      <c r="V13" s="86">
+        <v>3200000000</v>
+      </c>
+      <c r="W13" s="86">
+        <v>3200000000</v>
+      </c>
+      <c r="X13" s="86">
+        <v>3200000000</v>
+      </c>
+    </row>
+    <row r="14" ht="20.35" customHeight="1">
+      <c r="B14" t="s" s="75">
+        <v>17</v>
+      </c>
+      <c r="C14" s="85">
+        <f>C13*C$10</f>
+        <v>-940800000</v>
+      </c>
+      <c r="D14" s="86">
+        <f>D13*D$10</f>
+        <v>940800000</v>
+      </c>
+      <c r="E14" s="86">
+        <f>E13*E$10</f>
+        <v>2822400000</v>
+      </c>
+      <c r="F14" s="86">
+        <f>F13*F$10</f>
+        <v>4704000000</v>
+      </c>
+      <c r="G14" s="86">
+        <f>G13*G$10</f>
+        <v>5644800000</v>
+      </c>
+      <c r="H14" s="86">
+        <f>H13*H$10</f>
+        <v>6585600000</v>
+      </c>
+      <c r="I14" s="86">
+        <f>I13*I$10</f>
+        <v>7526400000</v>
+      </c>
+      <c r="J14" s="86">
+        <f>J13*J$10</f>
+        <v>8467200000</v>
+      </c>
+      <c r="K14" s="86">
+        <f>K13*K$10</f>
+        <v>9408000000</v>
+      </c>
+      <c r="L14" s="86">
+        <f>L13*L$10</f>
+        <v>10348800000</v>
+      </c>
+      <c r="M14" s="86">
+        <f>M13*M$10</f>
+        <v>11289600000</v>
+      </c>
+      <c r="N14" s="86">
+        <f>N13*N$10</f>
+        <v>12230400000</v>
+      </c>
+      <c r="O14" s="86">
+        <f>O13*O$10</f>
+        <v>13171200000</v>
+      </c>
+      <c r="P14" s="86">
+        <f>P13*P$10</f>
+        <v>14112000000</v>
+      </c>
+      <c r="Q14" s="86">
+        <f>Q13*Q$10</f>
+        <v>15052800000</v>
+      </c>
+      <c r="R14" s="86">
+        <f>R13*R$10</f>
+        <v>15993600000</v>
+      </c>
+      <c r="S14" s="86">
+        <f>S13*S$10</f>
+        <v>16934400000</v>
+      </c>
+      <c r="T14" s="86">
+        <f>T13*T$10</f>
+        <v>17875200000</v>
+      </c>
+      <c r="U14" s="86">
+        <f>U13*U$10</f>
+        <v>18816000000</v>
+      </c>
+      <c r="V14" s="86">
+        <f>V13*V$10</f>
+        <v>19756800000</v>
+      </c>
+      <c r="W14" s="86">
+        <f>W13*W$10</f>
+        <v>20697600000</v>
+      </c>
+      <c r="X14" s="86">
+        <f>X13*X$10</f>
+        <v>21638400000</v>
+      </c>
+    </row>
+    <row r="15" ht="20.35" customHeight="1">
+      <c r="B15" t="s" s="75">
+        <v>18</v>
+      </c>
+      <c r="C15" s="81">
         <v>0</v>
       </c>
-      <c r="D4" s="66">
-        <f>D2-D3</f>
-        <v>10</v>
-      </c>
-      <c r="E4" s="66">
-        <f>E2-E3</f>
+      <c r="D15" s="82">
+        <v>0</v>
+      </c>
+      <c r="E15" s="82">
+        <v>0</v>
+      </c>
+      <c r="F15" s="82">
+        <v>0</v>
+      </c>
+      <c r="G15" s="82">
+        <v>0</v>
+      </c>
+      <c r="H15" s="82">
+        <v>0</v>
+      </c>
+      <c r="I15" s="82">
+        <v>0</v>
+      </c>
+      <c r="J15" s="82">
+        <v>0</v>
+      </c>
+      <c r="K15" s="82">
+        <v>0</v>
+      </c>
+      <c r="L15" s="82">
+        <v>0</v>
+      </c>
+      <c r="M15" s="82">
+        <v>0</v>
+      </c>
+      <c r="N15" s="82">
+        <v>0</v>
+      </c>
+      <c r="O15" s="82">
+        <v>0</v>
+      </c>
+      <c r="P15" s="82">
+        <v>0</v>
+      </c>
+      <c r="Q15" s="82">
+        <v>0</v>
+      </c>
+      <c r="R15" s="82">
+        <v>0</v>
+      </c>
+      <c r="S15" s="82">
+        <v>0</v>
+      </c>
+      <c r="T15" s="82">
+        <v>0</v>
+      </c>
+      <c r="U15" s="82">
+        <v>0</v>
+      </c>
+      <c r="V15" s="82">
+        <v>0</v>
+      </c>
+      <c r="W15" s="82">
+        <v>0</v>
+      </c>
+      <c r="X15" s="82">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" ht="20.35" customHeight="1">
+      <c r="B16" t="s" s="75">
+        <v>19</v>
+      </c>
+      <c r="C16" s="87">
+        <v>0.1</v>
+      </c>
+      <c r="D16" s="88">
+        <v>0.1</v>
+      </c>
+      <c r="E16" s="88">
+        <v>0.1</v>
+      </c>
+      <c r="F16" s="88">
+        <v>0.1</v>
+      </c>
+      <c r="G16" s="88">
+        <v>0.1</v>
+      </c>
+      <c r="H16" s="88">
+        <v>0.1</v>
+      </c>
+      <c r="I16" s="88">
+        <v>0.1</v>
+      </c>
+      <c r="J16" s="88">
+        <v>0.1</v>
+      </c>
+      <c r="K16" s="88">
+        <v>0.1</v>
+      </c>
+      <c r="L16" s="88">
+        <v>0.1</v>
+      </c>
+      <c r="M16" s="88">
+        <v>0.1</v>
+      </c>
+      <c r="N16" s="88">
+        <v>0.1</v>
+      </c>
+      <c r="O16" s="88">
+        <v>0.1</v>
+      </c>
+      <c r="P16" s="88">
+        <v>0.1</v>
+      </c>
+      <c r="Q16" s="88">
+        <v>0.1</v>
+      </c>
+      <c r="R16" s="88">
+        <v>0.1</v>
+      </c>
+      <c r="S16" s="88">
+        <v>0.1</v>
+      </c>
+      <c r="T16" s="88">
+        <v>0.1</v>
+      </c>
+      <c r="U16" s="88">
+        <v>0.1</v>
+      </c>
+      <c r="V16" s="88">
+        <v>0.1</v>
+      </c>
+      <c r="W16" s="88">
+        <v>0.1</v>
+      </c>
+      <c r="X16" s="88">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="17" ht="20.35" customHeight="1">
+      <c r="B17" t="s" s="75">
         <v>20</v>
       </c>
-      <c r="F4" s="66">
-        <f>F2-F3</f>
-        <v>30</v>
-      </c>
-      <c r="G4" s="66">
-        <f>G2-G3</f>
-        <v>35</v>
-      </c>
-      <c r="H4" s="66">
-        <f>H2-H3</f>
-        <v>40</v>
-      </c>
-      <c r="I4" s="66">
-        <f>I2-I3</f>
-        <v>45</v>
-      </c>
-      <c r="J4" s="66">
-        <f>J2-J3</f>
-        <v>50</v>
-      </c>
-      <c r="K4" s="66">
-        <f>K2-K3</f>
-        <v>55</v>
-      </c>
-      <c r="L4" s="66">
-        <f>L2-L3</f>
-        <v>60</v>
-      </c>
-      <c r="M4" s="66">
-        <f>M2-M3</f>
-        <v>65</v>
-      </c>
-      <c r="N4" s="66">
-        <f>N2-N3</f>
-        <v>70</v>
-      </c>
-      <c r="O4" s="66">
-        <f>O2-O3</f>
-        <v>75</v>
-      </c>
-      <c r="P4" s="66">
-        <f>P2-P3</f>
-        <v>80</v>
-      </c>
-      <c r="Q4" s="66">
-        <f>Q2-Q3</f>
-        <v>85</v>
-      </c>
-      <c r="R4" s="66">
-        <f>R2-R3</f>
-        <v>90</v>
-      </c>
-      <c r="S4" s="66">
-        <f>S2-S3</f>
-        <v>95</v>
-      </c>
-      <c r="T4" s="66">
-        <f>T2-T3</f>
-        <v>100</v>
-      </c>
-      <c r="U4" s="66">
-        <f>U2-U3</f>
-        <v>105</v>
-      </c>
-      <c r="V4" s="66">
-        <f>V2-V3</f>
-        <v>110</v>
-      </c>
-      <c r="W4" s="66">
-        <f>W2-W3</f>
-        <v>115</v>
-      </c>
-      <c r="X4" s="66">
-        <f>X2-X3</f>
-        <v>120</v>
-      </c>
-    </row>
-    <row r="5" ht="20.35" customHeight="1">
-      <c r="B5" s="67"/>
-      <c r="C5" s="68"/>
-      <c r="D5" s="69"/>
-      <c r="E5" s="69"/>
-      <c r="F5" s="69"/>
-      <c r="G5" s="69"/>
-      <c r="H5" s="69"/>
-      <c r="I5" s="69"/>
-      <c r="J5" s="69"/>
-      <c r="K5" s="69"/>
-      <c r="L5" s="69"/>
-      <c r="M5" s="69"/>
-      <c r="N5" s="69"/>
-      <c r="O5" s="69"/>
-      <c r="P5" s="69"/>
-      <c r="Q5" s="69"/>
-      <c r="R5" s="69"/>
-      <c r="S5" s="69"/>
-      <c r="T5" s="69"/>
-      <c r="U5" s="69"/>
-      <c r="V5" s="69"/>
-      <c r="W5" s="69"/>
-      <c r="X5" s="69"/>
-    </row>
-    <row r="6" ht="20.35" customHeight="1">
-      <c r="B6" t="s" s="64">
-        <v>11</v>
-      </c>
-      <c r="C6" s="70">
-        <v>0.12</v>
-      </c>
-      <c r="D6" s="71">
-        <v>0.12</v>
-      </c>
-      <c r="E6" s="71">
-        <v>0.12</v>
-      </c>
-      <c r="F6" s="71">
-        <v>0.12</v>
-      </c>
-      <c r="G6" s="71">
-        <v>0.12</v>
-      </c>
-      <c r="H6" s="71">
-        <v>0.12</v>
-      </c>
-      <c r="I6" s="71">
-        <v>0.12</v>
-      </c>
-      <c r="J6" s="71">
-        <v>0.12</v>
-      </c>
-      <c r="K6" s="71">
-        <v>0.12</v>
-      </c>
-      <c r="L6" s="71">
-        <v>0.12</v>
-      </c>
-      <c r="M6" s="71">
-        <v>0.12</v>
-      </c>
-      <c r="N6" s="71">
-        <v>0.12</v>
-      </c>
-      <c r="O6" s="71">
-        <v>0.12</v>
-      </c>
-      <c r="P6" s="71">
-        <v>0.12</v>
-      </c>
-      <c r="Q6" s="71">
-        <v>0.12</v>
-      </c>
-      <c r="R6" s="71">
-        <v>0.12</v>
-      </c>
-      <c r="S6" s="71">
-        <v>0.12</v>
-      </c>
-      <c r="T6" s="71">
-        <v>0.12</v>
-      </c>
-      <c r="U6" s="71">
-        <v>0.12</v>
-      </c>
-      <c r="V6" s="71">
-        <v>0.12</v>
-      </c>
-      <c r="W6" s="71">
-        <v>0.12</v>
-      </c>
-      <c r="X6" s="71">
-        <v>0.12</v>
-      </c>
-    </row>
-    <row r="7" ht="20.35" customHeight="1">
-      <c r="B7" t="s" s="64">
-        <v>12</v>
-      </c>
-      <c r="C7" s="65">
-        <f>C6*C4</f>
-        <v>0</v>
-      </c>
-      <c r="D7" s="66">
-        <f>D6*D4</f>
-        <v>1.2</v>
-      </c>
-      <c r="E7" s="66">
-        <f>E6*E4</f>
-        <v>2.4</v>
-      </c>
-      <c r="F7" s="66">
-        <f>F6*F4</f>
-        <v>3.6</v>
-      </c>
-      <c r="G7" s="66">
-        <f>G6*G4</f>
-        <v>4.2</v>
-      </c>
-      <c r="H7" s="66">
-        <f>H6*H4</f>
-        <v>4.8</v>
-      </c>
-      <c r="I7" s="66">
-        <f>I6*I4</f>
-        <v>5.4</v>
-      </c>
-      <c r="J7" s="66">
-        <f>J6*J4</f>
-        <v>6</v>
-      </c>
-      <c r="K7" s="66">
-        <f>K6*K4</f>
-        <v>6.6</v>
-      </c>
-      <c r="L7" s="66">
-        <f>L6*L4</f>
-        <v>7.2</v>
-      </c>
-      <c r="M7" s="66">
-        <f>M6*M4</f>
-        <v>7.8</v>
-      </c>
-      <c r="N7" s="66">
-        <f>N6*N4</f>
-        <v>8.4</v>
-      </c>
-      <c r="O7" s="66">
-        <f>O6*O4</f>
-        <v>9</v>
-      </c>
-      <c r="P7" s="66">
-        <f>P6*P4</f>
-        <v>9.6</v>
-      </c>
-      <c r="Q7" s="66">
-        <f>Q6*Q4</f>
-        <v>10.2</v>
-      </c>
-      <c r="R7" s="66">
-        <f>R6*R4</f>
-        <v>10.8</v>
-      </c>
-      <c r="S7" s="66">
-        <f>S6*S4</f>
-        <v>11.4</v>
-      </c>
-      <c r="T7" s="66">
-        <f>T6*T4</f>
-        <v>12</v>
-      </c>
-      <c r="U7" s="66">
-        <f>U6*U4</f>
-        <v>12.6</v>
-      </c>
-      <c r="V7" s="66">
-        <f>V6*V4</f>
-        <v>13.2</v>
-      </c>
-      <c r="W7" s="66">
-        <f>W6*W4</f>
-        <v>13.8</v>
-      </c>
-      <c r="X7" s="66">
-        <f>X6*X4</f>
-        <v>14.4</v>
-      </c>
-    </row>
-    <row r="8" ht="20.35" customHeight="1">
-      <c r="B8" s="67"/>
-      <c r="C8" s="68"/>
-      <c r="D8" s="69"/>
-      <c r="E8" s="69"/>
-      <c r="F8" s="69"/>
-      <c r="G8" s="69"/>
-      <c r="H8" s="69"/>
-      <c r="I8" s="69"/>
-      <c r="J8" s="69"/>
-      <c r="K8" s="69"/>
-      <c r="L8" s="69"/>
-      <c r="M8" s="69"/>
-      <c r="N8" s="69"/>
-      <c r="O8" s="69"/>
-      <c r="P8" s="69"/>
-      <c r="Q8" s="69"/>
-      <c r="R8" s="69"/>
-      <c r="S8" s="69"/>
-      <c r="T8" s="69"/>
-      <c r="U8" s="69"/>
-      <c r="V8" s="69"/>
-      <c r="W8" s="69"/>
-      <c r="X8" s="69"/>
-    </row>
-    <row r="9" ht="20.35" customHeight="1">
-      <c r="B9" t="s" s="64">
-        <v>13</v>
-      </c>
-      <c r="C9" s="70">
-        <v>0.49</v>
-      </c>
-      <c r="D9" s="71">
-        <v>0.49</v>
-      </c>
-      <c r="E9" s="71">
-        <v>0.49</v>
-      </c>
-      <c r="F9" s="71">
-        <v>0.49</v>
-      </c>
-      <c r="G9" s="71">
-        <v>0.49</v>
-      </c>
-      <c r="H9" s="71">
-        <v>0.49</v>
-      </c>
-      <c r="I9" s="71">
-        <v>0.49</v>
-      </c>
-      <c r="J9" s="71">
-        <v>0.49</v>
-      </c>
-      <c r="K9" s="71">
-        <v>0.49</v>
-      </c>
-      <c r="L9" s="71">
-        <v>0.49</v>
-      </c>
-      <c r="M9" s="71">
-        <v>0.49</v>
-      </c>
-      <c r="N9" s="71">
-        <v>0.49</v>
-      </c>
-      <c r="O9" s="71">
-        <v>0.49</v>
-      </c>
-      <c r="P9" s="71">
-        <v>0.49</v>
-      </c>
-      <c r="Q9" s="71">
-        <v>0.49</v>
-      </c>
-      <c r="R9" s="71">
-        <v>0.49</v>
-      </c>
-      <c r="S9" s="71">
-        <v>0.49</v>
-      </c>
-      <c r="T9" s="71">
-        <v>0.49</v>
-      </c>
-      <c r="U9" s="71">
-        <v>0.49</v>
-      </c>
-      <c r="V9" s="71">
-        <v>0.49</v>
-      </c>
-      <c r="W9" s="71">
-        <v>0.49</v>
-      </c>
-      <c r="X9" s="71">
-        <v>0.49</v>
-      </c>
-    </row>
-    <row r="10" ht="20.35" customHeight="1">
-      <c r="B10" t="s" s="64">
-        <v>14</v>
-      </c>
-      <c r="C10" s="72">
-        <f>C7*C9</f>
-        <v>0</v>
-      </c>
-      <c r="D10" s="73">
-        <f>D7*D9</f>
-        <v>0.588</v>
-      </c>
-      <c r="E10" s="73">
-        <f>E7*E9</f>
-        <v>1.176</v>
-      </c>
-      <c r="F10" s="73">
-        <f>F7*F9</f>
-        <v>1.764</v>
-      </c>
-      <c r="G10" s="73">
-        <f>G7*G9</f>
-        <v>2.058</v>
-      </c>
-      <c r="H10" s="73">
-        <f>H7*H9</f>
-        <v>2.352</v>
-      </c>
-      <c r="I10" s="73">
-        <f>I7*I9</f>
-        <v>2.646</v>
-      </c>
-      <c r="J10" s="73">
-        <f>J7*J9</f>
-        <v>2.94</v>
-      </c>
-      <c r="K10" s="73">
-        <f>K7*K9</f>
-        <v>3.234</v>
-      </c>
-      <c r="L10" s="73">
-        <f>L7*L9</f>
-        <v>3.528</v>
-      </c>
-      <c r="M10" s="73">
-        <f>M7*M9</f>
-        <v>3.822</v>
-      </c>
-      <c r="N10" s="73">
-        <f>N7*N9</f>
-        <v>4.116</v>
-      </c>
-      <c r="O10" s="73">
-        <f>O7*O9</f>
-        <v>4.41</v>
-      </c>
-      <c r="P10" s="73">
-        <f>P7*P9</f>
-        <v>4.704</v>
-      </c>
-      <c r="Q10" s="73">
-        <f>Q7*Q9</f>
-        <v>4.998</v>
-      </c>
-      <c r="R10" s="73">
-        <f>R7*R9</f>
-        <v>5.292</v>
-      </c>
-      <c r="S10" s="73">
-        <f>S7*S9</f>
-        <v>5.586</v>
-      </c>
-      <c r="T10" s="73">
-        <f>T7*T9</f>
-        <v>5.88</v>
-      </c>
-      <c r="U10" s="73">
-        <f>U7*U9</f>
-        <v>6.174</v>
-      </c>
-      <c r="V10" s="73">
-        <f>V7*V9</f>
-        <v>6.468</v>
-      </c>
-      <c r="W10" s="73">
-        <f>W7*W9</f>
-        <v>6.762</v>
-      </c>
-      <c r="X10" s="73">
-        <f>X7*X9</f>
-        <v>7.056</v>
-      </c>
-    </row>
-    <row r="11" ht="20.35" customHeight="1">
-      <c r="B11" s="67"/>
-      <c r="C11" s="68"/>
-      <c r="D11" s="69"/>
-      <c r="E11" s="69"/>
-      <c r="F11" s="69"/>
-      <c r="G11" s="69"/>
-      <c r="H11" s="69"/>
-      <c r="I11" s="69"/>
-      <c r="J11" s="69"/>
-      <c r="K11" s="69"/>
-      <c r="L11" s="69"/>
-      <c r="M11" s="69"/>
-      <c r="N11" s="69"/>
-      <c r="O11" s="69"/>
-      <c r="P11" s="69"/>
-      <c r="Q11" s="69"/>
-      <c r="R11" s="69"/>
-      <c r="S11" s="69"/>
-      <c r="T11" s="69"/>
-      <c r="U11" s="69"/>
-      <c r="V11" s="69"/>
-      <c r="W11" s="69"/>
-      <c r="X11" s="69"/>
-    </row>
-    <row r="12" ht="20.35" customHeight="1">
-      <c r="B12" t="s" s="64">
-        <v>15</v>
-      </c>
-      <c r="C12" s="68"/>
-      <c r="D12" s="69"/>
-      <c r="E12" s="69"/>
-      <c r="F12" s="69"/>
-      <c r="G12" s="69"/>
-      <c r="H12" s="69"/>
-      <c r="I12" s="69"/>
-      <c r="J12" s="69"/>
-      <c r="K12" s="69"/>
-      <c r="L12" s="69"/>
-      <c r="M12" s="69"/>
-      <c r="N12" s="69"/>
-      <c r="O12" s="69"/>
-      <c r="P12" s="69"/>
-      <c r="Q12" s="69"/>
-      <c r="R12" s="69"/>
-      <c r="S12" s="69"/>
-      <c r="T12" s="69"/>
-      <c r="U12" s="69"/>
-      <c r="V12" s="69"/>
-      <c r="W12" s="69"/>
-      <c r="X12" s="69"/>
-    </row>
-    <row r="13" ht="20.35" customHeight="1">
-      <c r="B13" t="s" s="64">
-        <v>16</v>
-      </c>
-      <c r="C13" s="74">
-        <v>3200000000</v>
-      </c>
-      <c r="D13" s="75">
-        <v>3200000000</v>
-      </c>
-      <c r="E13" s="75">
-        <v>3200000000</v>
-      </c>
-      <c r="F13" s="75">
-        <v>3200000000</v>
-      </c>
-      <c r="G13" s="75">
-        <v>3200000000</v>
-      </c>
-      <c r="H13" s="75">
-        <v>3200000000</v>
-      </c>
-      <c r="I13" s="75">
-        <v>3200000000</v>
-      </c>
-      <c r="J13" s="75">
-        <v>3200000000</v>
-      </c>
-      <c r="K13" s="75">
-        <v>3200000000</v>
-      </c>
-      <c r="L13" s="75">
-        <v>3200000000</v>
-      </c>
-      <c r="M13" s="75">
-        <v>3200000000</v>
-      </c>
-      <c r="N13" s="75">
-        <v>3200000000</v>
-      </c>
-      <c r="O13" s="75">
-        <v>3200000000</v>
-      </c>
-      <c r="P13" s="75">
-        <v>3200000000</v>
-      </c>
-      <c r="Q13" s="75">
-        <v>3200000000</v>
-      </c>
-      <c r="R13" s="75">
-        <v>3200000000</v>
-      </c>
-      <c r="S13" s="75">
-        <v>3200000000</v>
-      </c>
-      <c r="T13" s="75">
-        <v>3200000000</v>
-      </c>
-      <c r="U13" s="75">
-        <v>3200000000</v>
-      </c>
-      <c r="V13" s="75">
-        <v>3200000000</v>
-      </c>
-      <c r="W13" s="75">
-        <v>3200000000</v>
-      </c>
-      <c r="X13" s="75">
-        <v>3200000000</v>
-      </c>
-    </row>
-    <row r="14" ht="20.35" customHeight="1">
-      <c r="B14" t="s" s="64">
-        <v>17</v>
-      </c>
-      <c r="C14" s="74">
-        <f>C13*C$10</f>
-        <v>0</v>
-      </c>
-      <c r="D14" s="75">
-        <f>D13*D$10</f>
-        <v>1881600000</v>
-      </c>
-      <c r="E14" s="75">
-        <f>E13*E$10</f>
-        <v>3763200000</v>
-      </c>
-      <c r="F14" s="75">
-        <f>F13*F$10</f>
-        <v>5644800000</v>
-      </c>
-      <c r="G14" s="75">
-        <f>G13*G$10</f>
-        <v>6585600000</v>
-      </c>
-      <c r="H14" s="75">
-        <f>H13*H$10</f>
-        <v>7526400000</v>
-      </c>
-      <c r="I14" s="75">
-        <f>I13*I$10</f>
+      <c r="C17" s="85">
+        <f>C14*(1-(C15+C16))</f>
+        <v>-846720000</v>
+      </c>
+      <c r="D17" s="86">
+        <f>D14*(1-(D15+D16))</f>
+        <v>846720000</v>
+      </c>
+      <c r="E17" s="86">
+        <f>E14*(1-(E15+E16))</f>
+        <v>2540160000</v>
+      </c>
+      <c r="F17" s="86">
+        <f>F14*(1-(F15+F16))</f>
+        <v>4233600000</v>
+      </c>
+      <c r="G17" s="86">
+        <f>G14*(1-(G15+G16))</f>
+        <v>5080320000</v>
+      </c>
+      <c r="H17" s="86">
+        <f>H14*(1-(H15+H16))</f>
+        <v>5927040000</v>
+      </c>
+      <c r="I17" s="86">
+        <f>I14*(1-(I15+I16))</f>
+        <v>6773760000</v>
+      </c>
+      <c r="J17" s="86">
+        <f>J14*(1-(J15+J16))</f>
+        <v>7620480000</v>
+      </c>
+      <c r="K17" s="86">
+        <f>K14*(1-(K15+K16))</f>
         <v>8467200000</v>
       </c>
-      <c r="J14" s="75">
-        <f>J13*J$10</f>
-        <v>9408000000</v>
-      </c>
-      <c r="K14" s="75">
-        <f>K13*K$10</f>
-        <v>10348800000</v>
-      </c>
-      <c r="L14" s="75">
-        <f>L13*L$10</f>
-        <v>11289600000</v>
-      </c>
-      <c r="M14" s="75">
-        <f>M13*M$10</f>
-        <v>12230400000</v>
-      </c>
-      <c r="N14" s="75">
-        <f>N13*N$10</f>
-        <v>13171200000</v>
-      </c>
-      <c r="O14" s="75">
-        <f>O13*O$10</f>
-        <v>14112000000</v>
-      </c>
-      <c r="P14" s="75">
-        <f>P13*P$10</f>
-        <v>15052800000</v>
-      </c>
-      <c r="Q14" s="75">
-        <f>Q13*Q$10</f>
-        <v>15993600000</v>
-      </c>
-      <c r="R14" s="75">
-        <f>R13*R$10</f>
+      <c r="L17" s="86">
+        <f>L14*(1-(L15+L16))</f>
+        <v>9313920000</v>
+      </c>
+      <c r="M17" s="86">
+        <f>M14*(1-(M15+M16))</f>
+        <v>10160640000</v>
+      </c>
+      <c r="N17" s="86">
+        <f>N14*(1-(N15+N16))</f>
+        <v>11007360000</v>
+      </c>
+      <c r="O17" s="86">
+        <f>O14*(1-(O15+O16))</f>
+        <v>11854080000</v>
+      </c>
+      <c r="P17" s="86">
+        <f>P14*(1-(P15+P16))</f>
+        <v>12700800000</v>
+      </c>
+      <c r="Q17" s="86">
+        <f>Q14*(1-(Q15+Q16))</f>
+        <v>13547520000</v>
+      </c>
+      <c r="R17" s="86">
+        <f>R14*(1-(R15+R16))</f>
+        <v>14394240000</v>
+      </c>
+      <c r="S17" s="86">
+        <f>S14*(1-(S15+S16))</f>
+        <v>15240960000</v>
+      </c>
+      <c r="T17" s="86">
+        <f>T14*(1-(T15+T16))</f>
+        <v>16087680000</v>
+      </c>
+      <c r="U17" s="86">
+        <f>U14*(1-(U15+U16))</f>
         <v>16934400000</v>
       </c>
-      <c r="S14" s="75">
-        <f>S13*S$10</f>
-        <v>17875200000</v>
-      </c>
-      <c r="T14" s="75">
-        <f>T13*T$10</f>
-        <v>18816000000</v>
-      </c>
-      <c r="U14" s="75">
-        <f>U13*U$10</f>
-        <v>19756800000</v>
-      </c>
-      <c r="V14" s="75">
-        <f>V13*V$10</f>
-        <v>20697600000</v>
-      </c>
-      <c r="W14" s="75">
-        <f>W13*W$10</f>
-        <v>21638400000</v>
-      </c>
-      <c r="X14" s="75">
-        <f>X13*X$10</f>
-        <v>22579200000</v>
-      </c>
-    </row>
-    <row r="15" ht="20.35" customHeight="1">
-      <c r="B15" t="s" s="64">
-        <v>18</v>
-      </c>
-      <c r="C15" s="70">
-        <v>0</v>
-      </c>
-      <c r="D15" s="71">
-        <v>0</v>
-      </c>
-      <c r="E15" s="71">
-        <v>0</v>
-      </c>
-      <c r="F15" s="71">
-        <v>0</v>
-      </c>
-      <c r="G15" s="71">
-        <v>0</v>
-      </c>
-      <c r="H15" s="71">
-        <v>0</v>
-      </c>
-      <c r="I15" s="71">
-        <v>0</v>
-      </c>
-      <c r="J15" s="71">
-        <v>0</v>
-      </c>
-      <c r="K15" s="71">
-        <v>0</v>
-      </c>
-      <c r="L15" s="71">
-        <v>0</v>
-      </c>
-      <c r="M15" s="71">
-        <v>0</v>
-      </c>
-      <c r="N15" s="71">
-        <v>0</v>
-      </c>
-      <c r="O15" s="71">
-        <v>0</v>
-      </c>
-      <c r="P15" s="71">
-        <v>0</v>
-      </c>
-      <c r="Q15" s="71">
-        <v>0</v>
-      </c>
-      <c r="R15" s="71">
-        <v>0</v>
-      </c>
-      <c r="S15" s="71">
-        <v>0</v>
-      </c>
-      <c r="T15" s="71">
-        <v>0</v>
-      </c>
-      <c r="U15" s="71">
-        <v>0</v>
-      </c>
-      <c r="V15" s="71">
-        <v>0</v>
-      </c>
-      <c r="W15" s="71">
-        <v>0</v>
-      </c>
-      <c r="X15" s="71">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" ht="20.35" customHeight="1">
-      <c r="B16" t="s" s="64">
-        <v>19</v>
-      </c>
-      <c r="C16" s="76">
-        <v>0.1</v>
-      </c>
-      <c r="D16" s="77">
-        <v>0.1</v>
-      </c>
-      <c r="E16" s="77">
-        <v>0.1</v>
-      </c>
-      <c r="F16" s="77">
-        <v>0.1</v>
-      </c>
-      <c r="G16" s="77">
-        <v>0.1</v>
-      </c>
-      <c r="H16" s="77">
-        <v>0.1</v>
-      </c>
-      <c r="I16" s="77">
-        <v>0.1</v>
-      </c>
-      <c r="J16" s="77">
-        <v>0.1</v>
-      </c>
-      <c r="K16" s="77">
-        <v>0.1</v>
-      </c>
-      <c r="L16" s="77">
-        <v>0.1</v>
-      </c>
-      <c r="M16" s="77">
-        <v>0.1</v>
-      </c>
-      <c r="N16" s="77">
-        <v>0.1</v>
-      </c>
-      <c r="O16" s="77">
-        <v>0.1</v>
-      </c>
-      <c r="P16" s="77">
-        <v>0.1</v>
-      </c>
-      <c r="Q16" s="77">
-        <v>0.1</v>
-      </c>
-      <c r="R16" s="77">
-        <v>0.1</v>
-      </c>
-      <c r="S16" s="77">
-        <v>0.1</v>
-      </c>
-      <c r="T16" s="77">
-        <v>0.1</v>
-      </c>
-      <c r="U16" s="77">
-        <v>0.1</v>
-      </c>
-      <c r="V16" s="77">
-        <v>0.1</v>
-      </c>
-      <c r="W16" s="77">
-        <v>0.1</v>
-      </c>
-      <c r="X16" s="77">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="17" ht="20.35" customHeight="1">
-      <c r="B17" t="s" s="64">
-        <v>20</v>
-      </c>
-      <c r="C17" s="74">
-        <f>C14*(1-(C15+C16))</f>
-        <v>0</v>
-      </c>
-      <c r="D17" s="75">
-        <f>D14*(1-(D15+D16))</f>
-        <v>1693440000</v>
-      </c>
-      <c r="E17" s="75">
-        <f>E14*(1-(E15+E16))</f>
-        <v>3386880000</v>
-      </c>
-      <c r="F17" s="75">
-        <f>F14*(1-(F15+F16))</f>
-        <v>5080320000</v>
-      </c>
-      <c r="G17" s="75">
-        <f>G14*(1-(G15+G16))</f>
-        <v>5927040000</v>
-      </c>
-      <c r="H17" s="75">
-        <f>H14*(1-(H15+H16))</f>
-        <v>6773760000</v>
-      </c>
-      <c r="I17" s="75">
-        <f>I14*(1-(I15+I16))</f>
-        <v>7620480000</v>
-      </c>
-      <c r="J17" s="75">
-        <f>J14*(1-(J15+J16))</f>
-        <v>8467200000</v>
-      </c>
-      <c r="K17" s="75">
-        <f>K14*(1-(K15+K16))</f>
-        <v>9313920000</v>
-      </c>
-      <c r="L17" s="75">
-        <f>L14*(1-(L15+L16))</f>
-        <v>10160640000</v>
-      </c>
-      <c r="M17" s="75">
-        <f>M14*(1-(M15+M16))</f>
-        <v>11007360000</v>
-      </c>
-      <c r="N17" s="75">
-        <f>N14*(1-(N15+N16))</f>
-        <v>11854080000</v>
-      </c>
-      <c r="O17" s="75">
-        <f>O14*(1-(O15+O16))</f>
-        <v>12700800000</v>
-      </c>
-      <c r="P17" s="75">
-        <f>P14*(1-(P15+P16))</f>
-        <v>13547520000</v>
-      </c>
-      <c r="Q17" s="75">
-        <f>Q14*(1-(Q15+Q16))</f>
-        <v>14394240000</v>
-      </c>
-      <c r="R17" s="75">
-        <f>R14*(1-(R15+R16))</f>
-        <v>15240960000</v>
-      </c>
-      <c r="S17" s="75">
-        <f>S14*(1-(S15+S16))</f>
-        <v>16087680000</v>
-      </c>
-      <c r="T17" s="75">
-        <f>T14*(1-(T15+T16))</f>
-        <v>16934400000</v>
-      </c>
-      <c r="U17" s="75">
-        <f>U14*(1-(U15+U16))</f>
+      <c r="V17" s="86">
+        <f>V14*(1-(V15+V16))</f>
         <v>17781120000</v>
       </c>
-      <c r="V17" s="75">
-        <f>V14*(1-(V15+V16))</f>
+      <c r="W17" s="86">
+        <f>W14*(1-(W15+W16))</f>
         <v>18627840000</v>
       </c>
-      <c r="W17" s="75">
-        <f>W14*(1-(W15+W16))</f>
+      <c r="X17" s="86">
+        <f>X14*(1-(X15+X16))</f>
         <v>19474560000</v>
       </c>
-      <c r="X17" s="75">
-        <f>X14*(1-(X15+X16))</f>
-        <v>20321280000</v>
-      </c>
     </row>
     <row r="18" ht="20.35" customHeight="1">
-      <c r="B18" t="s" s="64">
+      <c r="B18" t="s" s="75">
         <v>21</v>
       </c>
-      <c r="C18" s="74">
+      <c r="C18" s="85">
         <v>164923363</v>
       </c>
-      <c r="D18" s="75">
+      <c r="D18" s="86">
         <v>164923363</v>
       </c>
-      <c r="E18" s="75">
+      <c r="E18" s="86">
         <v>164923363</v>
       </c>
-      <c r="F18" s="75">
+      <c r="F18" s="86">
         <v>164923363</v>
       </c>
-      <c r="G18" s="75">
+      <c r="G18" s="86">
         <v>164923363</v>
       </c>
-      <c r="H18" s="75">
+      <c r="H18" s="86">
         <v>164923363</v>
       </c>
-      <c r="I18" s="75">
+      <c r="I18" s="86">
         <v>164923363</v>
       </c>
-      <c r="J18" s="75">
+      <c r="J18" s="86">
         <v>164923363</v>
       </c>
-      <c r="K18" s="75">
+      <c r="K18" s="86">
         <v>164923363</v>
       </c>
-      <c r="L18" s="75">
+      <c r="L18" s="86">
         <v>164923363</v>
       </c>
-      <c r="M18" s="75">
+      <c r="M18" s="86">
         <v>164923363</v>
       </c>
-      <c r="N18" s="75">
+      <c r="N18" s="86">
         <v>164923363</v>
       </c>
-      <c r="O18" s="75">
+      <c r="O18" s="86">
         <v>164923363</v>
       </c>
-      <c r="P18" s="75">
+      <c r="P18" s="86">
         <v>164923363</v>
       </c>
-      <c r="Q18" s="75">
+      <c r="Q18" s="86">
         <v>164923363</v>
       </c>
-      <c r="R18" s="75">
+      <c r="R18" s="86">
         <v>164923363</v>
       </c>
-      <c r="S18" s="75">
+      <c r="S18" s="86">
         <v>164923363</v>
       </c>
-      <c r="T18" s="75">
+      <c r="T18" s="86">
         <v>164923363</v>
       </c>
-      <c r="U18" s="75">
+      <c r="U18" s="86">
         <v>164923363</v>
       </c>
-      <c r="V18" s="75">
+      <c r="V18" s="86">
         <v>164923363</v>
       </c>
-      <c r="W18" s="75">
+      <c r="W18" s="86">
         <v>164923363</v>
       </c>
-      <c r="X18" s="75">
+      <c r="X18" s="86">
         <v>164923363</v>
       </c>
     </row>
     <row r="19" ht="20.35" customHeight="1">
-      <c r="B19" t="s" s="64">
+      <c r="B19" t="s" s="75">
         <v>22</v>
       </c>
-      <c r="C19" s="65">
+      <c r="C19" s="76">
         <f>C17/C18</f>
-        <v>0</v>
-      </c>
-      <c r="D19" s="66">
+        <v>-5.13402094523139</v>
+      </c>
+      <c r="D19" s="77">
         <f>D17/D18</f>
-        <v>10.2680418904628</v>
-      </c>
-      <c r="E19" s="66">
+        <v>5.13402094523139</v>
+      </c>
+      <c r="E19" s="77">
         <f>E17/E18</f>
-        <v>20.5360837809256</v>
-      </c>
-      <c r="F19" s="66">
+        <v>15.4020628356942</v>
+      </c>
+      <c r="F19" s="77">
         <f>F17/F18</f>
+        <v>25.670104726157</v>
+      </c>
+      <c r="G19" s="77">
+        <f>G17/G18</f>
         <v>30.8041256713884</v>
       </c>
-      <c r="G19" s="66">
-        <f>G17/G18</f>
+      <c r="H19" s="77">
+        <f>H17/H18</f>
         <v>35.9381466166197</v>
       </c>
-      <c r="H19" s="66">
-        <f>H17/H18</f>
+      <c r="I19" s="77">
+        <f>I17/I18</f>
         <v>41.0721675618511</v>
       </c>
-      <c r="I19" s="66">
-        <f>I17/I18</f>
+      <c r="J19" s="77">
+        <f>J17/J18</f>
         <v>46.2061885070825</v>
       </c>
-      <c r="J19" s="66">
-        <f>J17/J18</f>
+      <c r="K19" s="77">
+        <f>K17/K18</f>
         <v>51.3402094523139</v>
       </c>
-      <c r="K19" s="66">
-        <f>K17/K18</f>
+      <c r="L19" s="77">
+        <f>L17/L18</f>
         <v>56.4742303975453</v>
       </c>
-      <c r="L19" s="66">
-        <f>L17/L18</f>
+      <c r="M19" s="77">
+        <f>M17/M18</f>
         <v>61.6082513427767</v>
       </c>
-      <c r="M19" s="66">
-        <f>M17/M18</f>
+      <c r="N19" s="77">
+        <f>N17/N18</f>
         <v>66.7422722880081</v>
       </c>
-      <c r="N19" s="66">
-        <f>N17/N18</f>
+      <c r="O19" s="77">
+        <f>O17/O18</f>
         <v>71.87629323323949</v>
       </c>
-      <c r="O19" s="66">
-        <f>O17/O18</f>
+      <c r="P19" s="77">
+        <f>P17/P18</f>
         <v>77.01031417847091</v>
       </c>
-      <c r="P19" s="66">
-        <f>P17/P18</f>
+      <c r="Q19" s="77">
+        <f>Q17/Q18</f>
         <v>82.14433512370231</v>
       </c>
-      <c r="Q19" s="66">
-        <f>Q17/Q18</f>
+      <c r="R19" s="77">
+        <f>R17/R18</f>
         <v>87.2783560689337</v>
       </c>
-      <c r="R19" s="66">
-        <f>R17/R18</f>
+      <c r="S19" s="77">
+        <f>S17/S18</f>
         <v>92.4123770141651</v>
       </c>
-      <c r="S19" s="66">
-        <f>S17/S18</f>
+      <c r="T19" s="77">
+        <f>T17/T18</f>
         <v>97.5463979593965</v>
       </c>
-      <c r="T19" s="66">
-        <f>T17/T18</f>
+      <c r="U19" s="77">
+        <f>U17/U18</f>
         <v>102.680418904628</v>
       </c>
-      <c r="U19" s="66">
-        <f>U17/U18</f>
+      <c r="V19" s="77">
+        <f>V17/V18</f>
         <v>107.814439849859</v>
       </c>
-      <c r="V19" s="66">
-        <f>V17/V18</f>
+      <c r="W19" s="77">
+        <f>W17/W18</f>
         <v>112.948460795091</v>
       </c>
-      <c r="W19" s="66">
-        <f>W17/W18</f>
+      <c r="X19" s="77">
+        <f>X17/X18</f>
         <v>118.082481740322</v>
       </c>
-      <c r="X19" s="66">
-        <f>X17/X18</f>
-        <v>123.216502685553</v>
-      </c>
     </row>
     <row r="20" ht="20.35" customHeight="1">
-      <c r="B20" s="67"/>
-      <c r="C20" s="68"/>
-      <c r="D20" s="69"/>
-      <c r="E20" s="69"/>
-      <c r="F20" s="69"/>
-      <c r="G20" s="69"/>
-      <c r="H20" s="69"/>
-      <c r="I20" s="69"/>
-      <c r="J20" s="69"/>
-      <c r="K20" s="69"/>
-      <c r="L20" s="69"/>
-      <c r="M20" s="69"/>
-      <c r="N20" s="69"/>
-      <c r="O20" s="69"/>
-      <c r="P20" s="69"/>
-      <c r="Q20" s="69"/>
-      <c r="R20" s="69"/>
-      <c r="S20" s="69"/>
-      <c r="T20" s="69"/>
-      <c r="U20" s="69"/>
-      <c r="V20" s="69"/>
-      <c r="W20" s="69"/>
-      <c r="X20" s="69"/>
+      <c r="B20" s="78"/>
+      <c r="C20" s="79"/>
+      <c r="D20" s="80"/>
+      <c r="E20" s="80"/>
+      <c r="F20" s="80"/>
+      <c r="G20" s="80"/>
+      <c r="H20" s="80"/>
+      <c r="I20" s="80"/>
+      <c r="J20" s="80"/>
+      <c r="K20" s="80"/>
+      <c r="L20" s="80"/>
+      <c r="M20" s="80"/>
+      <c r="N20" s="80"/>
+      <c r="O20" s="80"/>
+      <c r="P20" s="80"/>
+      <c r="Q20" s="80"/>
+      <c r="R20" s="80"/>
+      <c r="S20" s="80"/>
+      <c r="T20" s="80"/>
+      <c r="U20" s="80"/>
+      <c r="V20" s="80"/>
+      <c r="W20" s="80"/>
+      <c r="X20" s="80"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>